<commit_message>
Finalize reporting table, with logos.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="41">
   <si>
     <t>Forest</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Summary of change in soil organic carbon</t>
+  </si>
+  <si>
+    <t>For more information on trends.earth, see http://trends.earth, or contact the team at trends.earth@conservation.org.</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -659,6 +662,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
@@ -668,19 +684,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1186,7 +1190,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1223,18 +1227,18 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
@@ -1329,18 +1333,18 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
@@ -1385,7 +1389,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1404,7 +1408,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="49"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="4" t="s">
         <v>1</v>
       </c>
@@ -1421,7 +1425,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="49"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1438,7 +1442,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="49"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1455,7 +1459,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="49"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1472,7 +1476,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="49"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1493,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="49"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1544,18 +1548,18 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
@@ -1600,7 +1604,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1619,7 +1623,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="49"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="4" t="s">
         <v>1</v>
       </c>
@@ -1636,7 +1640,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="49"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="4" t="s">
         <v>2</v>
       </c>
@@ -1653,7 +1657,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="49"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="4" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1674,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="49"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="4" t="s">
         <v>4</v>
       </c>
@@ -1687,7 +1691,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="49"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1708,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="49"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
@@ -1759,18 +1763,18 @@
       </c>
     </row>
     <row r="35" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
     </row>
     <row r="36" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
@@ -1815,7 +1819,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1834,7 +1838,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="49"/>
+      <c r="A39" s="54"/>
       <c r="B39" s="4" t="s">
         <v>1</v>
       </c>
@@ -1851,7 +1855,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="49"/>
+      <c r="A40" s="54"/>
       <c r="B40" s="4" t="s">
         <v>2</v>
       </c>
@@ -1868,7 +1872,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="49"/>
+      <c r="A41" s="54"/>
       <c r="B41" s="4" t="s">
         <v>3</v>
       </c>
@@ -1885,7 +1889,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="49"/>
+      <c r="A42" s="54"/>
       <c r="B42" s="4" t="s">
         <v>4</v>
       </c>
@@ -1902,7 +1906,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="49"/>
+      <c r="A43" s="54"/>
       <c r="B43" s="4" t="s">
         <v>5</v>
       </c>
@@ -1919,7 +1923,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="49"/>
+      <c r="A44" s="54"/>
       <c r="B44" s="4" t="s">
         <v>6</v>
       </c>
@@ -1984,18 +1988,18 @@
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="51" t="s">
+      <c r="A47" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="51"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
     </row>
     <row r="48" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="3"/>
@@ -2040,7 +2044,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -2059,7 +2063,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="49"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="4" t="s">
         <v>1</v>
       </c>
@@ -2076,7 +2080,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="49"/>
+      <c r="A52" s="54"/>
       <c r="B52" s="4" t="s">
         <v>2</v>
       </c>
@@ -2093,7 +2097,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="49"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="4" t="s">
         <v>3</v>
       </c>
@@ -2110,7 +2114,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="49"/>
+      <c r="A54" s="54"/>
       <c r="B54" s="4" t="s">
         <v>4</v>
       </c>
@@ -2127,7 +2131,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="49"/>
+      <c r="A55" s="54"/>
       <c r="B55" s="4" t="s">
         <v>5</v>
       </c>
@@ -2144,7 +2148,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="49"/>
+      <c r="A56" s="54"/>
       <c r="B56" s="4" t="s">
         <v>6</v>
       </c>
@@ -2209,27 +2213,26 @@
       <c r="J58" s="13"/>
     </row>
     <row r="59" spans="1:10" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="50" t="s">
+      <c r="A59" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="50"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="55"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="55"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="55"/>
+      <c r="I59" s="55"/>
+      <c r="J59" s="55"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A61" s="49" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A14:A20"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A59:J59"/>
@@ -2238,6 +2241,12 @@
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="C36:I36"/>
     <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="A14:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2247,11 +2256,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2269,17 +2276,17 @@
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
@@ -2320,7 +2327,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="59"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2344,7 +2351,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
@@ -2368,7 +2375,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="59"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
@@ -2392,7 +2399,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -2416,7 +2423,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="59"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2440,7 +2447,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="59"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
@@ -2464,7 +2471,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="59"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
@@ -2509,30 +2516,30 @@
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
@@ -2560,7 +2567,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2575,7 +2582,7 @@
       <c r="I20" s="40"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="49"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="4" t="s">
         <v>1</v>
       </c>
@@ -2588,7 +2595,7 @@
       <c r="I21" s="40"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="49"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="4" t="s">
         <v>2</v>
       </c>
@@ -2601,7 +2608,7 @@
       <c r="I22" s="40"/>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="49"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="4" t="s">
         <v>3</v>
       </c>
@@ -2614,7 +2621,7 @@
       <c r="I23" s="40"/>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="49"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="4" t="s">
         <v>4</v>
       </c>
@@ -2627,7 +2634,7 @@
       <c r="I24" s="40"/>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="49"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="4" t="s">
         <v>5</v>
       </c>
@@ -2640,7 +2647,7 @@
       <c r="I25" s="40"/>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="49"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="4" t="s">
         <v>6</v>
       </c>
@@ -2664,30 +2671,35 @@
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" s="15" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
     </row>
     <row r="30" spans="1:9" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="49" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2707,11 +2719,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2731,18 +2741,18 @@
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
@@ -2765,7 +2775,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="59"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
@@ -2787,7 +2797,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="59"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -2809,7 +2819,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="59"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
@@ -2831,7 +2841,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
@@ -2853,7 +2863,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="59"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
@@ -2875,7 +2885,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
@@ -2897,7 +2907,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="59"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
@@ -2945,18 +2955,18 @@
       <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
@@ -3001,7 +3011,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -3020,7 +3030,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="49"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="4" t="s">
         <v>1</v>
       </c>
@@ -3037,7 +3047,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="49"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="4" t="s">
         <v>2</v>
       </c>
@@ -3054,7 +3064,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="49"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="4" t="s">
         <v>3</v>
       </c>
@@ -3071,7 +3081,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="49"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
@@ -3088,7 +3098,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="49"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
@@ -3105,7 +3115,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="49"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
@@ -3163,18 +3173,23 @@
       <c r="J26" s="13"/>
     </row>
     <row r="27" spans="1:10" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="55"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="49" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Add more decimals to percent output.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -576,18 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -596,9 +584,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -629,9 +614,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,18 +645,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
@@ -684,7 +654,19 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -700,6 +682,24 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1202,18 +1202,18 @@
     <col min="10" max="10" width="15.6328125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
@@ -1227,18 +1227,18 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
@@ -1253,10 +1253,10 @@
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="40">
         <f>SUM(J21,J33,J45,J57)</f>
         <v>0</v>
       </c>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="19" t="e">
+      <c r="F6" s="57" t="e">
         <f>J21/F5</f>
         <v>#DIV/0!</v>
       </c>
@@ -1281,10 +1281,10 @@
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="20" t="e">
+      <c r="F7" s="58" t="e">
         <f>J33/F5</f>
         <v>#DIV/0!</v>
       </c>
@@ -1295,10 +1295,10 @@
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="21" t="e">
+      <c r="F8" s="59" t="e">
         <f>J45/F5</f>
         <v>#DIV/0!</v>
       </c>
@@ -1309,10 +1309,10 @@
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="22" t="e">
+      <c r="F9" s="60" t="e">
         <f>J57/F5</f>
         <v>#DIV/0!</v>
       </c>
@@ -1333,55 +1333,55 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="29" t="s">
+      <c r="C13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="30" t="s">
+      <c r="I13" s="25" t="s">
         <v>6</v>
       </c>
       <c r="J13" s="11" t="s">
@@ -1389,122 +1389,122 @@
       </c>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="42">
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="36">
         <f t="shared" ref="J14:J20" si="0">SUM(C14:I14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="54"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="42">
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="54"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="42">
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="54"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="42">
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42">
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="54"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="42">
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="54"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="42">
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1514,65 +1514,65 @@
       <c r="B21" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="36">
         <f t="shared" ref="C21:J21" si="1">SUM(C14:C20)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F21" s="42">
+      <c r="F21" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G21" s="42">
+      <c r="G21" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H21" s="42">
+      <c r="H21" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I21" s="42">
+      <c r="I21" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J21" s="43">
+      <c r="J21" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
       <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -1604,122 +1604,122 @@
       </c>
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="42">
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="36">
         <f t="shared" ref="J26:J32" si="2">SUM(C26:I26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="54"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="42">
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="54"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="42">
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="54"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="42">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="54"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="42">
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="54"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="42">
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="54"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="42">
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1729,65 +1729,65 @@
       <c r="B33" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="36">
         <f t="shared" ref="C33:J33" si="3">SUM(C26:C32)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="42">
+      <c r="D33" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F33" s="42">
+      <c r="F33" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G33" s="42">
+      <c r="G33" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H33" s="42">
+      <c r="H33" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I33" s="42">
+      <c r="I33" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J33" s="43">
+      <c r="J33" s="37">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="57"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
     </row>
     <row r="36" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="52"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
-      <c r="I36" s="52"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
       <c r="J36" s="12"/>
     </row>
     <row r="37" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -1819,122 +1819,122 @@
       </c>
     </row>
     <row r="38" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="42">
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="36">
         <f t="shared" ref="J38:J44" si="4">SUM(C38:I38)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="54"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="42">
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="54"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="42">
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="54"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="41"/>
-      <c r="J41" s="42">
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="54"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="42">
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="54"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="42">
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="54"/>
+      <c r="A44" s="44"/>
       <c r="B44" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="42">
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1944,35 +1944,35 @@
       <c r="B45" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="42">
+      <c r="C45" s="36">
         <f t="shared" ref="C45:J45" si="5">SUM(C38:C44)</f>
         <v>0</v>
       </c>
-      <c r="D45" s="42">
+      <c r="D45" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E45" s="42">
+      <c r="E45" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F45" s="42">
+      <c r="F45" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G45" s="42">
+      <c r="G45" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H45" s="42">
+      <c r="H45" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I45" s="42">
+      <c r="I45" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J45" s="43">
+      <c r="J45" s="37">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1988,31 +1988,31 @@
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
     </row>
     <row r="48" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="3"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="52" t="s">
+      <c r="C48" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
       <c r="J48" s="12"/>
     </row>
     <row r="49" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -2044,122 +2044,122 @@
       </c>
     </row>
     <row r="50" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="42">
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="36">
         <f t="shared" ref="J50:J56" si="6">SUM(C50:I50)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="54"/>
+      <c r="A51" s="44"/>
       <c r="B51" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="42">
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="54"/>
+      <c r="A52" s="44"/>
       <c r="B52" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="41"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="41"/>
-      <c r="J52" s="42">
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="54"/>
+      <c r="A53" s="44"/>
       <c r="B53" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="42">
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="54"/>
+      <c r="A54" s="44"/>
       <c r="B54" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="41"/>
-      <c r="J54" s="42">
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="54"/>
+      <c r="A55" s="44"/>
       <c r="B55" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="41"/>
-      <c r="I55" s="41"/>
-      <c r="J55" s="42">
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="54"/>
+      <c r="A56" s="44"/>
       <c r="B56" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="42">
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2169,35 +2169,35 @@
       <c r="B57" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="42">
+      <c r="C57" s="36">
         <f t="shared" ref="C57:J57" si="7">SUM(C50:C56)</f>
         <v>0</v>
       </c>
-      <c r="D57" s="42">
+      <c r="D57" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="E57" s="42">
+      <c r="E57" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F57" s="42">
+      <c r="F57" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G57" s="42">
+      <c r="G57" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H57" s="42">
+      <c r="H57" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I57" s="42">
+      <c r="I57" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J57" s="43">
+      <c r="J57" s="37">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2213,26 +2213,32 @@
       <c r="J58" s="13"/>
     </row>
     <row r="59" spans="1:10" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="55" t="s">
+      <c r="A59" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="55"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="45"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="43" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="A14:A20"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A59:J59"/>
@@ -2241,12 +2247,6 @@
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="C36:I36"/>
     <mergeCell ref="A38:A44"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A14:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2268,7 +2268,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2276,27 +2276,27 @@
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="27" t="e">
+      <c r="F5" s="62" t="e">
         <f>G15/E15</f>
         <v>#DIV/0!</v>
       </c>
@@ -2307,357 +2307,357 @@
     <row r="7" spans="1:9" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="28" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="60"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45">
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39">
         <f>C8*'Land cover'!C6*100</f>
         <v>0</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="39">
         <f>D8*'Land cover'!D6*100</f>
         <v>0</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="35">
         <f>F8-E8</f>
         <v>0</v>
       </c>
-      <c r="H8" s="38" t="e">
+      <c r="H8" s="61" t="e">
         <f>(D8-C8)/C8</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="60"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45">
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39">
         <f>C9*'Land cover'!C7*100</f>
         <v>0</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="39">
         <f>D9*'Land cover'!D7*100</f>
         <v>0</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="35">
         <f t="shared" ref="G9:G14" si="0">F9-E9</f>
         <v>0</v>
       </c>
-      <c r="H9" s="38" t="e">
+      <c r="H9" s="61" t="e">
         <f t="shared" ref="H9:H14" si="1">(D9-C9)/C9</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="60"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45">
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39">
         <f>C10*'Land cover'!C8*100</f>
         <v>0</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="39">
         <f>D10*'Land cover'!D8*100</f>
         <v>0</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="38" t="e">
+      <c r="H10" s="61" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45">
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39">
         <f>C11*'Land cover'!C9*100</f>
         <v>0</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="39">
         <f>D11*'Land cover'!D9*100</f>
         <v>0</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G11" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="38" t="e">
+      <c r="H11" s="61" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="60"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39">
         <f>C12*'Land cover'!C10*100</f>
         <v>0</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="39">
         <f>D12*'Land cover'!D10*100</f>
         <v>0</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="38" t="e">
+      <c r="H12" s="61" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="60"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45">
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39">
         <f>C13*'Land cover'!C11*100</f>
         <v>0</v>
       </c>
-      <c r="F13" s="45">
+      <c r="F13" s="39">
         <f>D13*'Land cover'!D11*100</f>
         <v>0</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="38" t="e">
+      <c r="H13" s="61" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="60"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45">
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39">
         <f>C14*'Land cover'!C12*100</f>
         <v>0</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="39">
         <f>D14*'Land cover'!D12*100</f>
         <v>0</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="38" t="e">
+      <c r="H14" s="61" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17"/>
-      <c r="C15" s="44"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="38">
         <f>SUM(E8:E14)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="38">
         <f>SUM(F8:F14)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="44">
+      <c r="G15" s="38">
         <f>SUM(G8:G14)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="39"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="31" t="s">
+      <c r="C19" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="54"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="54"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="54"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="54"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="54"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="54"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
     </row>
     <row r="27" spans="1:9" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
@@ -2671,33 +2671,33 @@
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" s="15" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="61"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
     </row>
     <row r="30" spans="1:9" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="43" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2721,7 +2721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2731,28 +2733,28 @@
     <col min="10" max="10" width="15.6328125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="26"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
@@ -2761,169 +2763,169 @@
     <row r="5" spans="1:10" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="28" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="60"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="35">
         <f t="shared" ref="C6:C12" si="0">J18</f>
         <v>0</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="35">
         <f>C25</f>
         <v>0</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="35">
         <f>D6-C6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="38" t="e">
+      <c r="F6" s="61" t="e">
         <f>(D6-C6)/C6</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="60"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="35">
         <f>D25</f>
         <v>0</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="35">
         <f t="shared" ref="E7:E12" si="1">D7-C7</f>
         <v>0</v>
       </c>
-      <c r="F7" s="38" t="e">
+      <c r="F7" s="61" t="e">
         <f t="shared" ref="F7:F12" si="2">(D7-C7)/C7</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="60"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="35">
         <f>E25</f>
         <v>0</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="38" t="e">
+      <c r="F8" s="61" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="60"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="35">
         <f>F25</f>
         <v>0</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="38" t="e">
+      <c r="F9" s="61" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="60"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="35">
         <f>G25</f>
         <v>0</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F10" s="38" t="e">
+      <c r="F10" s="61" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="35">
         <f>H25</f>
         <v>0</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="38" t="e">
+      <c r="F11" s="61" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="60"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="35">
         <f>I25</f>
         <v>0</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12" s="38" t="e">
+      <c r="F12" s="61" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -2933,77 +2935,77 @@
       <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="38">
         <f>SUM(C6:C12)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="38">
         <f>SUM(D6:D12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="38">
         <f>SUM(E6:E12)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="39"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="36" t="s">
+      <c r="C17" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="36" t="s">
+      <c r="H17" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="37" t="s">
+      <c r="I17" s="32" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="11" t="s">
@@ -3011,122 +3013,122 @@
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42">
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="36">
         <f t="shared" ref="J18:J25" si="3">SUM(C18:I18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="54"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="42">
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="54"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="42">
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="54"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="42">
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="54"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="42">
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="54"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="42">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="54"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="42">
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3136,35 +3138,35 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="36">
         <f t="shared" ref="C25:I25" si="4">SUM(C18:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="42">
+      <c r="D25" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E25" s="42">
+      <c r="E25" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F25" s="42">
+      <c r="F25" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G25" s="42">
+      <c r="G25" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H25" s="42">
+      <c r="H25" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I25" s="42">
+      <c r="I25" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J25" s="43">
+      <c r="J25" s="37">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3173,21 +3175,21 @@
       <c r="J26" s="13"/>
     </row>
     <row r="27" spans="1:10" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="43" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean units for reporting table.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="41">
   <si>
     <t>trends.earth productivity summary table</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Change in soil organic carbon (percent)</t>
   </si>
   <si>
-    <t>Soil organic carbon change by type of land cover transition (percent)*</t>
-  </si>
-  <si>
-    <t>* trends.earth calculates soil organic carbon change based on annual land cover transitions. This table shows percent change in soil organic carbon based on the baseline and target years only. The target year soil organic carbon value used to produce this table accounts for all land cover transitions that ocurred between the baseline and target years. The value in cell C21, for example, shows the percent change in soil organic carbon for all pixels that were in the "Grasslands" class in the baseline year, and in the "Forest" class in the target year.</t>
-  </si>
-  <si>
     <t>trends.earth land cover summary table</t>
   </si>
   <si>
@@ -144,6 +138,12 @@
   </si>
   <si>
     <t>Land area by type of land cover transition (sq. km)</t>
+  </si>
+  <si>
+    <t>Soil organic carbon change by type of land cover transition (tons)*</t>
+  </si>
+  <si>
+    <t>* trends.earth calculates soil organic carbon change based on annual land cover transitions. This table shows percent change in soil organic carbon based on the baseline and target years only. The target year soil organic carbon value used to produce this table accounts for all land cover transitions that ocurred between the baseline and target years. The value in cell C20, for example, shows the percent change in soil organic carbon for all pixels that were in the "Grasslands" class in the baseline year, and in the "Forest" class in the target year.</t>
   </si>
 </sst>
 </file>
@@ -271,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,12 +320,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -611,9 +605,6 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,22 +645,8 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="9" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -685,19 +662,30 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1067,68 +1055,68 @@
       <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="58"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
     </row>
     <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="35">
         <f>SUM(J21,J33,J45,J57)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="6"/>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="40" t="e">
+      <c r="F6" s="39" t="e">
         <f>J21/F5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="6"/>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="41" t="e">
+      <c r="F7" s="40" t="e">
         <f>J33/F5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="6"/>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="42" t="e">
+      <c r="F8" s="41" t="e">
         <f>J45/F5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="6"/>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="43" t="e">
+      <c r="F9" s="42" t="e">
         <f>J57/F5</f>
         <v>#DIV/0!</v>
       </c>
@@ -1140,27 +1128,27 @@
       <c r="A11" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="20" t="s">
@@ -1189,122 +1177,122 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="47" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="34">
-        <f t="shared" ref="J14:J20" si="0">SUM(C14:I14)</f>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="33">
+        <f>SUM(C14:I14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="53"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="34">
-        <f t="shared" si="0"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="33">
+        <f t="shared" ref="J15:J20" si="0">SUM(C15:I15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="53"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="34">
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="53"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="34">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="53"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="34">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="53"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="34">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="53"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="34">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1314,35 +1302,35 @@
       <c r="B21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="34">
-        <f t="shared" ref="C21:J21" si="1">SUM(C14:C20)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="34">
+      <c r="C21" s="33">
+        <f>SUM(C14:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <f t="shared" ref="D21:J21" si="1">SUM(D14:D20)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E21" s="34">
+      <c r="F21" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F21" s="34">
+      <c r="G21" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G21" s="34">
+      <c r="H21" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H21" s="34">
+      <c r="I21" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I21" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="33">
+      <c r="J21" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1351,27 +1339,27 @@
       <c r="A23" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="58"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="54"/>
     </row>
     <row r="24" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
     </row>
     <row r="25" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="4" t="s">
@@ -1400,122 +1388,122 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="47" t="s">
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="34">
-        <f t="shared" ref="J26:J32" si="2">SUM(C26:I26)</f>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="33">
+        <f>SUM(C26:I26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="53"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="34">
-        <f t="shared" si="2"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="33">
+        <f t="shared" ref="J27:J32" si="2">SUM(C27:I27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="53"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="34">
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="53"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="34">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="53"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="34">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="53"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="34">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="53"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="34">
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1525,64 +1513,64 @@
       <c r="B33" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="34">
-        <f t="shared" ref="C33:J33" si="3">SUM(C26:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="34">
+      <c r="C33" s="33">
+        <f>SUM(C26:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <f t="shared" ref="D33:J33" si="3">SUM(D26:D32)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E33" s="34">
+      <c r="F33" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F33" s="34">
+      <c r="G33" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G33" s="34">
+      <c r="H33" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H33" s="34">
+      <c r="I33" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I33" s="34">
+      <c r="J33" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J33" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="35" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="60" t="s">
+      <c r="A35" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="58"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="54"/>
     </row>
     <row r="36" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="1"/>
-      <c r="C36" s="59" t="s">
+      <c r="C36" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
     </row>
     <row r="37" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="4" t="s">
@@ -1611,122 +1599,122 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="47" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="34">
-        <f t="shared" ref="J38:J44" si="4">SUM(C38:I38)</f>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="33">
+        <f>SUM(C38:I38)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="53"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="34">
-        <f t="shared" si="4"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="33">
+        <f t="shared" ref="J39:J44" si="4">SUM(C39:I39)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="53"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="34">
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="53"/>
+      <c r="A41" s="48"/>
       <c r="B41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="34">
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="53"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="34">
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="53"/>
+      <c r="A43" s="48"/>
       <c r="B43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="34">
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="53"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="34">
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1736,64 +1724,64 @@
       <c r="B45" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="34">
-        <f t="shared" ref="C45:J45" si="5">SUM(C38:C44)</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="34">
+      <c r="C45" s="33">
+        <f>SUM(C38:C44)</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <f t="shared" ref="D45:J45" si="5">SUM(D38:D44)</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E45" s="34">
+      <c r="F45" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F45" s="34">
+      <c r="G45" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G45" s="34">
+      <c r="H45" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H45" s="34">
+      <c r="I45" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I45" s="34">
+      <c r="J45" s="32">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J45" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="47" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="53"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="57"/>
-      <c r="J47" s="58"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="54"/>
     </row>
     <row r="48" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="1"/>
-      <c r="C48" s="59" t="s">
+      <c r="C48" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="57"/>
-      <c r="H48" s="57"/>
-      <c r="I48" s="57"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
     </row>
     <row r="49" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C49" s="4" t="s">
@@ -1822,122 +1810,122 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="52" t="s">
+      <c r="A50" s="47" t="s">
         <v>17</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="34">
-        <f t="shared" ref="J50:J56" si="6">SUM(C50:I50)</f>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="33">
+        <f>SUM(C50:I50)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="53"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="34">
-        <f t="shared" si="6"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="33">
+        <f t="shared" ref="J51:J56" si="6">SUM(C51:I51)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="53"/>
+      <c r="A52" s="48"/>
       <c r="B52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="34">
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="53"/>
+      <c r="A53" s="48"/>
       <c r="B53" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
-      <c r="J53" s="34">
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="53"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="34">
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="53"/>
+      <c r="A55" s="48"/>
       <c r="B55" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="34">
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="53"/>
+      <c r="A56" s="48"/>
       <c r="B56" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="34">
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -1947,55 +1935,55 @@
       <c r="B57" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="34">
-        <f t="shared" ref="C57:J57" si="7">SUM(C50:C56)</f>
-        <v>0</v>
-      </c>
-      <c r="D57" s="34">
+      <c r="C57" s="33">
+        <f>SUM(C50:C56)</f>
+        <v>0</v>
+      </c>
+      <c r="D57" s="33">
+        <f t="shared" ref="D57:J57" si="7">SUM(D50:D56)</f>
+        <v>0</v>
+      </c>
+      <c r="E57" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="E57" s="34">
+      <c r="F57" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F57" s="34">
+      <c r="G57" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G57" s="34">
+      <c r="H57" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H57" s="34">
+      <c r="I57" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I57" s="34">
+      <c r="J57" s="32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J57" s="33">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="59" spans="1:10" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="54" t="s">
+      <c r="A59" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B59" s="55"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="50"/>
+      <c r="I59" s="50"/>
+      <c r="J59" s="50"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="38" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2017,60 +2005,63 @@
     <mergeCell ref="A38:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.54296875" style="2" customWidth="1"/>
-    <col min="3" max="9" width="15.6328125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="15.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" style="45" customWidth="1"/>
+    <col min="6" max="10" width="15.6328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="61" t="s">
+    <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
-      <c r="E5" s="37" t="s">
+      <c r="F5" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="45" t="e">
-        <f>G15/E15</f>
+      <c r="G5" s="44" t="e">
+        <f>I14/G14</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="6"/>
     </row>
-    <row r="7" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="24" t="s">
         <v>26</v>
       </c>
@@ -2078,260 +2069,274 @@
         <v>27</v>
       </c>
       <c r="E7" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="H7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="I7" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="J7" s="25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="66"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35">
-        <f>C8*'Land cover'!C6*100</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="35">
-        <f>D8*'Land cover'!D6*100</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="32">
-        <f t="shared" ref="G8:G14" si="0">F8-E8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="44" t="e">
-        <f t="shared" ref="H8:H14" si="1">(D8-C8)/C8</f>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34">
+        <f>C8*E8*100</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="34">
+        <f>D8*F8*100</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="31">
+        <f t="shared" ref="I8:I13" si="0">H8-G8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="43" t="e">
+        <f>I8/G8</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
+    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="48"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35">
-        <f>C9*'Land cover'!C7*100</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="35">
-        <f>D9*'Land cover'!D7*100</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="32">
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34">
+        <f t="shared" ref="G9:G13" si="1">C9*E9*100</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="34">
+        <f t="shared" ref="H9:H13" si="2">D9*F9*100</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="44" t="e">
-        <f t="shared" si="1"/>
+      <c r="J9" s="43" t="e">
+        <f t="shared" ref="J9:J13" si="3">I9/G9</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="53"/>
+    <row r="10" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="48"/>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35">
-        <f>C10*'Land cover'!C8*100</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="35">
-        <f>D10*'Land cover'!D8*100</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="32">
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="44" t="e">
-        <f t="shared" si="1"/>
+      <c r="J10" s="43" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
+    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="48"/>
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35">
-        <f>C11*'Land cover'!C9*100</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="35">
-        <f>D11*'Land cover'!D9*100</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="32">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="44" t="e">
-        <f t="shared" si="1"/>
+      <c r="J11" s="43" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="53"/>
+    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="48"/>
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35">
-        <f>C12*'Land cover'!C10*100</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="35">
-        <f>D12*'Land cover'!D10*100</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="32">
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="44" t="e">
-        <f t="shared" si="1"/>
+      <c r="J12" s="43" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="53"/>
+    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="48"/>
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35">
-        <f>C13*'Land cover'!C11*100</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="35">
-        <f>D13*'Land cover'!D11*100</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="32">
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="44" t="e">
-        <f t="shared" si="1"/>
+      <c r="J13" s="43" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="53"/>
-      <c r="B14" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47">
-        <f>C14*'Land cover'!C12*100</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="47">
-        <f>D14*'Land cover'!D12*100</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="49" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="8" t="s">
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="34">
-        <f>SUM(E8:E14)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="34">
-        <f>SUM(F8:F14)</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="34">
-        <f>SUM(G8:G14)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="17" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="65" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-    </row>
-    <row r="18" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="1"/>
-      <c r="C18" s="64" t="s">
+      <c r="E14" s="33">
+        <f>SUM(E8:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <f>SUM(F8:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <f>SUM(G8:G13)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="33">
+        <f>SUM(H8:H13)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <f>SUM(I8:I13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+    </row>
+    <row r="17" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="1"/>
+      <c r="C17" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-    </row>
-    <row r="19" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="23" t="s">
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+    </row>
+    <row r="18" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D18" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E18" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F18" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H18" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="52" t="s">
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="47" t="s">
         <v>17</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="48"/>
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
@@ -2339,12 +2344,12 @@
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
       <c r="H20" s="31"/>
-      <c r="I20" s="50"/>
-    </row>
-    <row r="21" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="53"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="48"/>
       <c r="B21" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
@@ -2352,12 +2357,12 @@
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
-      <c r="I21" s="50"/>
-    </row>
-    <row r="22" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="53"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="48"/>
       <c r="B22" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
@@ -2365,12 +2370,12 @@
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
-      <c r="I22" s="50"/>
-    </row>
-    <row r="23" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="48"/>
       <c r="B23" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
@@ -2378,12 +2383,12 @@
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
-      <c r="I23" s="50"/>
-    </row>
-    <row r="24" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="53"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="48"/>
       <c r="B24" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
@@ -2391,88 +2396,65 @@
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
-      <c r="I24" s="50"/>
-    </row>
-    <row r="25" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="53"/>
-      <c r="B25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="50"/>
-    </row>
-    <row r="26" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="53"/>
-      <c r="B26" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-    </row>
-    <row r="27" spans="1:9" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-    </row>
-    <row r="28" spans="1:9" s="12" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-    </row>
-    <row r="30" spans="1:9" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="54" t="s">
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="11"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="1:10" s="12" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+    </row>
+    <row r="28" spans="1:10" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="39" t="s">
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="38" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2492,7 +2474,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J1" s="19"/>
     </row>
@@ -2500,34 +2482,34 @@
       <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="58"/>
+      <c r="A3" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="F5" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2535,151 +2517,151 @@
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <f t="shared" ref="C6:C12" si="0">J18</f>
         <v>0</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <f>C25</f>
         <v>0</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <f t="shared" ref="E6:E12" si="1">D6-C6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="44" t="e">
+      <c r="F6" s="43" t="e">
         <f t="shared" ref="F6:F12" si="2">(D6-C6)/C6</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="53"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <f>D25</f>
         <v>0</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="44" t="e">
+      <c r="F7" s="43" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <f>E25</f>
         <v>0</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="44" t="e">
+      <c r="F8" s="43" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <f>F25</f>
         <v>0</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="44" t="e">
+      <c r="F9" s="43" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="53"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <f>G25</f>
         <v>0</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F10" s="44" t="e">
+      <c r="F10" s="43" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <f>H25</f>
         <v>0</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="44" t="e">
+      <c r="F11" s="43" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="53"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <f>I25</f>
         <v>0</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12" s="44" t="e">
+      <c r="F12" s="43" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -2689,15 +2671,15 @@
       <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="33">
         <f>SUM(C6:C12)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="33">
         <f>SUM(D6:D12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="33">
         <f>SUM(E6:E12)</f>
         <v>0</v>
       </c>
@@ -2711,29 +2693,29 @@
     </row>
     <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="58"/>
+        <v>38</v>
+      </c>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="54"/>
     </row>
     <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
     </row>
     <row r="17" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="27" t="s">
@@ -2762,122 +2744,122 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="47" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="34">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="33">
         <f t="shared" ref="J18:J25" si="3">SUM(C18:I18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="53"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="34">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="53"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="34">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="53"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="34">
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="53"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="34">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="34">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="53"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="34">
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2887,55 +2869,55 @@
       <c r="B25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="33">
         <f t="shared" ref="C25:I25" si="4">SUM(C18:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H25" s="34">
+      <c r="H25" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I25" s="34">
+      <c r="I25" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J25" s="33">
+      <c r="J25" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="38" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new basemap function, and start fixing new reporting.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,19 +12,17 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10400"/>
   </bookViews>
   <sheets>
-    <sheet name="Productivity" sheetId="1" r:id="rId1"/>
-    <sheet name="Soil organic carbon" sheetId="2" r:id="rId2"/>
-    <sheet name="Land cover" sheetId="3" r:id="rId3"/>
+    <sheet name="SDG 15.3.1" sheetId="4" r:id="rId1"/>
+    <sheet name="Productivity" sheetId="1" r:id="rId2"/>
+    <sheet name="Soil organic carbon" sheetId="2" r:id="rId3"/>
+    <sheet name="Land cover" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="41">
-  <si>
-    <t>trends.earth productivity summary table</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="58">
   <si>
     <t>Summary of change in productivity</t>
   </si>
@@ -89,18 +87,9 @@
     <t>The boundaries, names, and designations used in this report do not imply official endorsement or acceptance by Conservation International Foundation, or its partner organizations and contributors.  This report is available under the terms of Creative Commons Attribution 4.0 International License (CC BY 4.0).</t>
   </si>
   <si>
-    <t>For more information on trends.earth, see http://trends.earth, or contact the team at trends.earth@conservation.org.</t>
-  </si>
-  <si>
-    <t>trends.earth soil organic carbon summary table</t>
-  </si>
-  <si>
     <t>Summary of change in soil organic carbon</t>
   </si>
   <si>
-    <t>Percent change in soil organic carbon from baseline to target:</t>
-  </si>
-  <si>
     <t>Baseline soil organic carbon (tons / ha)</t>
   </si>
   <si>
@@ -119,9 +108,6 @@
     <t>Change in soil organic carbon (percent)</t>
   </si>
   <si>
-    <t>trends.earth land cover summary table</t>
-  </si>
-  <si>
     <t>Summary of change in land cover</t>
   </si>
   <si>
@@ -144,6 +130,72 @@
   </si>
   <si>
     <t>* trends.earth calculates soil organic carbon change based on annual land cover transitions. This table shows change in soil organic carbon based on the baseline and target years only. The target year soil organic carbon value used to produce this table accounts for all land cover transitions that ocurred between the baseline and target years.</t>
+  </si>
+  <si>
+    <t>Land area improved:</t>
+  </si>
+  <si>
+    <t>Land area stable:</t>
+  </si>
+  <si>
+    <t>Land area degraded:</t>
+  </si>
+  <si>
+    <t>Land area with no data:</t>
+  </si>
+  <si>
+    <t>Trends.Earth productivity summary table</t>
+  </si>
+  <si>
+    <t>Trends.Earth soil organic carbon summary table</t>
+  </si>
+  <si>
+    <t>Trends.Earth land cover summary table</t>
+  </si>
+  <si>
+    <t>Trends.Earth SDG 15.3.1 summary table</t>
+  </si>
+  <si>
+    <t>Summary of SDG 15.3.1 Indicator</t>
+  </si>
+  <si>
+    <t>Land area with improved soil organic carbon:</t>
+  </si>
+  <si>
+    <t>Land area with stable soil organic carbon:</t>
+  </si>
+  <si>
+    <t>Land area with degraded soil organic carbon:</t>
+  </si>
+  <si>
+    <t>Land area with no data for soil organic carbon:</t>
+  </si>
+  <si>
+    <t>Land area with no data for land cover:</t>
+  </si>
+  <si>
+    <t>Land area with degraded land cover:</t>
+  </si>
+  <si>
+    <t>Land area with stable land cover:</t>
+  </si>
+  <si>
+    <t>Land area with improved land cover:</t>
+  </si>
+  <si>
+    <t>Percent change in soil organic carbon storage from baseline to target:</t>
+  </si>
+  <si>
+    <t>Soil organic carbon change from baseline to target</t>
+  </si>
+  <si>
+    <t>Land cover change by cover class</t>
+  </si>
+  <si>
+    <t>For more information on Trends.Earth, see http://trends.earth, or contact the team at trends.earth@conservation.org.</t>
+  </si>
+  <si>
+    <t>Total land area (sq. km, baseline year):</t>
   </si>
 </sst>
 </file>
@@ -153,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,8 +322,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +380,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -523,7 +595,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -626,7 +698,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -649,6 +720,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -659,39 +755,33 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -707,7 +797,18 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -718,6 +819,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF39797"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1026,9 +1132,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="52"/>
+    <col min="2" max="2" width="14.54296875" style="52" customWidth="1"/>
+    <col min="3" max="5" width="15.6328125" style="53" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" style="53" customWidth="1"/>
+    <col min="7" max="9" width="15.6328125" style="53" customWidth="1"/>
+    <col min="10" max="10" width="15.6328125" style="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="6"/>
+      <c r="E5" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="35">
+        <f>SUM(F6:F9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="6"/>
+      <c r="E6" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="38"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="6"/>
+      <c r="E7" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="6"/>
+      <c r="E8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="6"/>
+      <c r="E9" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="41"/>
+    </row>
+    <row r="10" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" s="50" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+    </row>
+    <row r="13" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1040,7 +1277,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -1055,18 +1292,18 @@
       <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="50"/>
+      <c r="A3" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="60"/>
     </row>
     <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6"/>
@@ -1074,7 +1311,7 @@
     <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
       <c r="E5" s="37" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="F5" s="35">
         <f>SUM(J21,J33,J45,J57)</f>
@@ -1084,40 +1321,40 @@
     <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="6"/>
       <c r="E6" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="39" t="e">
-        <f>J21/F5</f>
+        <v>2</v>
+      </c>
+      <c r="F6" s="38" t="e">
+        <f>SUM(J14:J19)/F5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="6"/>
       <c r="E7" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="40" t="e">
-        <f>J33/F5</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="39" t="e">
+        <f>SUM(J26:J31)/F5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="6"/>
       <c r="E8" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="41" t="e">
-        <f>J45/F5</f>
+        <v>4</v>
+      </c>
+      <c r="F8" s="40" t="e">
+        <f>SUM(J38:J43)/F5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="6"/>
       <c r="E9" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="42" t="e">
-        <f>J57/F5</f>
+        <v>5</v>
+      </c>
+      <c r="F9" s="41" t="e">
+        <f>SUM(J50:J55)/F5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1125,63 +1362,63 @@
       <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="54"/>
+      <c r="A11" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
-      <c r="C12" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
+      <c r="C12" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="G13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="H13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="I13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="J13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="10" t="s">
+    </row>
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="61" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="59" t="s">
-        <v>17</v>
-      </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
@@ -1196,9 +1433,9 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="52"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -1213,9 +1450,9 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -1230,9 +1467,9 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="52"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -1247,9 +1484,9 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="52"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
@@ -1264,9 +1501,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="52"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
@@ -1281,9 +1518,9 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="52"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
@@ -1300,7 +1537,7 @@
     <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
       <c r="B21" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="33">
         <f>SUM(C14:C20)</f>
@@ -1336,63 +1573,63 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="54"/>
+      <c r="A23" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="62"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="66"/>
     </row>
     <row r="24" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
+      <c r="C24" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
     </row>
     <row r="25" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="J25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="10" t="s">
+    </row>
+    <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="61" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="59" t="s">
-        <v>17</v>
-      </c>
       <c r="B26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
@@ -1407,9 +1644,9 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="52"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="31"/>
       <c r="D27" s="31"/>
@@ -1424,9 +1661,9 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="52"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="31"/>
@@ -1441,9 +1678,9 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="52"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31"/>
@@ -1458,9 +1695,9 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="52"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
@@ -1475,9 +1712,9 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="52"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
@@ -1492,9 +1729,9 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="52"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31"/>
@@ -1511,7 +1748,7 @@
     <row r="33" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="33">
         <f>SUM(C26:C32)</f>
@@ -1547,63 +1784,63 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="54"/>
+      <c r="A35" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="64"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="66"/>
     </row>
     <row r="36" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="1"/>
-      <c r="C36" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
+      <c r="C36" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
     </row>
     <row r="37" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="I37" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="J37" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J37" s="10" t="s">
+    </row>
+    <row r="38" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="61" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="59" t="s">
-        <v>17</v>
-      </c>
       <c r="B38" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="31"/>
       <c r="D38" s="31"/>
@@ -1618,9 +1855,9 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="52"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" s="31"/>
       <c r="D39" s="31"/>
@@ -1635,9 +1872,9 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="52"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="31"/>
@@ -1652,9 +1889,9 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="52"/>
+      <c r="A41" s="62"/>
       <c r="B41" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C41" s="31"/>
       <c r="D41" s="31"/>
@@ -1669,9 +1906,9 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="52"/>
+      <c r="A42" s="62"/>
       <c r="B42" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="31"/>
@@ -1686,9 +1923,9 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="52"/>
+      <c r="A43" s="62"/>
       <c r="B43" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C43" s="31"/>
       <c r="D43" s="31"/>
@@ -1703,9 +1940,9 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="52"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44" s="31"/>
       <c r="D44" s="31"/>
@@ -1722,7 +1959,7 @@
     <row r="45" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7"/>
       <c r="B45" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C45" s="33">
         <f>SUM(C38:C44)</f>
@@ -1758,63 +1995,63 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="57"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="54"/>
+      <c r="A47" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="64"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="65"/>
+      <c r="I47" s="65"/>
+      <c r="J47" s="66"/>
     </row>
     <row r="48" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="1"/>
-      <c r="C48" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="53"/>
+      <c r="C48" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="68"/>
+      <c r="E48" s="68"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="68"/>
     </row>
     <row r="49" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="F49" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="G49" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="H49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="I49" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I49" s="9" t="s">
+      <c r="J49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J49" s="10" t="s">
+    </row>
+    <row r="50" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="61" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="59" t="s">
-        <v>17</v>
-      </c>
       <c r="B50" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
@@ -1829,9 +2066,9 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="52"/>
+      <c r="A51" s="62"/>
       <c r="B51" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="31"/>
@@ -1846,9 +2083,9 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="52"/>
+      <c r="A52" s="62"/>
       <c r="B52" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="31"/>
@@ -1863,9 +2100,9 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="52"/>
+      <c r="A53" s="62"/>
       <c r="B53" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" s="31"/>
       <c r="D53" s="31"/>
@@ -1880,9 +2117,9 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="52"/>
+      <c r="A54" s="62"/>
       <c r="B54" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="31"/>
@@ -1897,9 +2134,9 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="52"/>
+      <c r="A55" s="62"/>
       <c r="B55" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C55" s="31"/>
       <c r="D55" s="31"/>
@@ -1914,9 +2151,9 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="52"/>
+      <c r="A56" s="62"/>
       <c r="B56" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
@@ -1933,7 +2170,7 @@
     <row r="57" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="7"/>
       <c r="B57" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C57" s="33">
         <f>SUM(C50:C56)</f>
@@ -1969,26 +2206,40 @@
       </c>
     </row>
     <row r="59" spans="1:10" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="B59" s="61"/>
-      <c r="C59" s="61"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
-      <c r="H59" s="61"/>
-      <c r="I59" s="61"/>
-      <c r="J59" s="61"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A61" s="38" t="s">
-        <v>22</v>
-      </c>
+      <c r="A59" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="56"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
+      <c r="F59" s="56"/>
+      <c r="G59" s="56"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="56"/>
+      <c r="J59" s="56"/>
+    </row>
+    <row r="61" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="A14:A20"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A59:J59"/>
@@ -1997,461 +2248,6 @@
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="C36:I36"/>
     <mergeCell ref="A38:A44"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A14:A20"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="14.54296875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="15.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="45" customWidth="1"/>
-    <col min="6" max="10" width="15.6328125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="6"/>
-      <c r="F5" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="44" t="e">
-        <f>I14/G14</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="66"/>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34">
-        <f>C8*E8*100</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="34">
-        <f>D8*F8*100</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="31">
-        <f t="shared" ref="I8:I13" si="0">H8-G8</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="43" t="e">
-        <f>I8/G8</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="52"/>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34">
-        <f t="shared" ref="G9:G13" si="1">C9*E9*100</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="34">
-        <f t="shared" ref="H9:H13" si="2">D9*F9*100</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="43" t="e">
-        <f t="shared" ref="J9:J13" si="3">I9/G9</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="52"/>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="43" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="43" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="52"/>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="43" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="52"/>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="43" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="33">
-        <f>SUM(E8:E13)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="33">
-        <f>SUM(F8:F13)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="33">
-        <f>SUM(G8:G13)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="33">
-        <f>SUM(H8:H13)</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="33">
-        <f>SUM(I8:I13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-    </row>
-    <row r="17" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="1"/>
-      <c r="C17" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-    </row>
-    <row r="18" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="J19"/>
-    </row>
-    <row r="20" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="52"/>
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="52"/>
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="J21"/>
-    </row>
-    <row r="22" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="52"/>
-      <c r="B22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="J22"/>
-    </row>
-    <row r="23" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="52"/>
-      <c r="B23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="J23"/>
-    </row>
-    <row r="24" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="52"/>
-      <c r="B24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="J24"/>
-    </row>
-    <row r="25" spans="1:10" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-    </row>
-    <row r="26" spans="1:10" s="12" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-    </row>
-    <row r="28" spans="1:10" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2460,9 +2256,559 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.54296875" style="2" customWidth="1"/>
+    <col min="3" max="4" width="15.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" style="44" customWidth="1"/>
+    <col min="6" max="10" width="15.6328125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="6"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="35">
+        <f>SUM(E16:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="48"/>
+    </row>
+    <row r="6" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="6"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="48"/>
+    </row>
+    <row r="7" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="6"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="39"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="48"/>
+    </row>
+    <row r="8" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="6"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="48"/>
+    </row>
+    <row r="9" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="6"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="48"/>
+    </row>
+    <row r="10" spans="1:10" s="46" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="6"/>
+      <c r="F11" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="43" t="e">
+        <f>I22/G22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" s="49" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+    </row>
+    <row r="14" spans="1:10" s="49" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="74"/>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34">
+        <f>C16*E16*100</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="34">
+        <f>D16*F16*100</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="31">
+        <f t="shared" ref="I16:I21" si="0">H16-G16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="42" t="e">
+        <f>I16/G16</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="62"/>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34">
+        <f t="shared" ref="G17:G21" si="1">C17*E17*100</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="34">
+        <f t="shared" ref="H17:H21" si="2">D17*F17*100</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="42" t="e">
+        <f t="shared" ref="J17:J21" si="3">I17/G17</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="62"/>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="42" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="62"/>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="42" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="62"/>
+      <c r="B20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="42" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="62"/>
+      <c r="B21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="42" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="33">
+        <f>SUM(E16:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <f>SUM(F16:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <f>SUM(G16:G21)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="33">
+        <f>SUM(H16:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <f>SUM(I16:I21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+    </row>
+    <row r="25" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="1"/>
+      <c r="C25" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+    </row>
+    <row r="26" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="62"/>
+      <c r="B28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="62"/>
+      <c r="B29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="62"/>
+      <c r="B30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="62"/>
+      <c r="B31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="62"/>
+      <c r="B32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="1:10" s="12" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+    </row>
+    <row r="36" spans="1:10" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+    </row>
+    <row r="38" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A13:J13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2474,7 +2820,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="J1" s="19"/>
     </row>
@@ -2482,453 +2828,550 @@
       <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="54"/>
+      <c r="A3" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="66"/>
-      <c r="B6" s="3" t="s">
+    <row r="5" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="6"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="35">
+        <f>SUM(C14:C19)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="48"/>
+    </row>
+    <row r="6" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="6"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="48"/>
+    </row>
+    <row r="7" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="6"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="39"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="48"/>
+    </row>
+    <row r="8" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="6"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="48"/>
+    </row>
+    <row r="9" spans="1:10" s="46" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="6"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="48"/>
+    </row>
+    <row r="10" spans="1:10" s="46" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" s="49" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="82"/>
+    </row>
+    <row r="12" spans="1:10" s="49" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="74"/>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="31">
+        <f t="shared" ref="C14:C20" si="0">J26</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="31">
+        <f>C33</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="31">
+        <f t="shared" ref="E14:E20" si="1">D14-C14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="42" t="e">
+        <f t="shared" ref="F14:F20" si="2">(D14-C14)/C14</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="62"/>
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="31">
-        <f t="shared" ref="C6:C12" si="0">J18</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="31">
-        <f>C25</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="31">
-        <f t="shared" ref="E6:E12" si="1">D6-C6</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="43" t="e">
-        <f t="shared" ref="F6:F12" si="2">(D6-C6)/C6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="52"/>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="31">
+      <c r="C15" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D7" s="31">
-        <f>D25</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="31">
+      <c r="D15" s="31">
+        <f>D33</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="43" t="e">
+      <c r="F15" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="52"/>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="31">
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="62"/>
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="31">
-        <f>E25</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="31">
+      <c r="D16" s="31">
+        <f>E33</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="43" t="e">
+      <c r="F16" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="52"/>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="31">
+    <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="62"/>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D9" s="31">
-        <f>F25</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="31">
+      <c r="D17" s="31">
+        <f>F33</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="43" t="e">
+      <c r="F17" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="52"/>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="31">
+    <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="62"/>
+      <c r="B18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="31">
-        <f>G25</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="31">
+      <c r="D18" s="31">
+        <f>G33</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F10" s="43" t="e">
+      <c r="F18" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="31">
+    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="62"/>
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D11" s="31">
-        <f>H25</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="31">
+      <c r="D19" s="31">
+        <f>H33</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="43" t="e">
+      <c r="F19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="52"/>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="31">
+    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="62"/>
+      <c r="B20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D12" s="31">
-        <f>I25</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="31">
+      <c r="D20" s="31">
+        <f>I33</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12" s="43" t="e">
+      <c r="F20" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="8" t="s">
+    <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14"/>
+      <c r="B21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="33">
+        <f>SUM(C14:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <f>SUM(D14:D20)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <f>SUM(E14:E20)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+    </row>
+    <row r="23" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="66"/>
+    </row>
+    <row r="24" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+    </row>
+    <row r="25" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="33">
-        <f>SUM(C6:C12)</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="33">
-        <f>SUM(D6:D12)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="33">
-        <f>SUM(E6:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="6"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-    </row>
-    <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="69" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="54"/>
-    </row>
-    <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="1"/>
-      <c r="C16" s="55" t="s">
+      <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-    </row>
-    <row r="17" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="27" t="s">
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="33">
+        <f t="shared" ref="J26:J33" si="3">SUM(C26:I26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="62"/>
+      <c r="B27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="62"/>
+      <c r="B28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="62"/>
+      <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="62"/>
+      <c r="B30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="62"/>
+      <c r="B31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="62"/>
+      <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="33">
-        <f t="shared" ref="J18:J25" si="3">SUM(C18:I18)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="52"/>
-      <c r="B19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="33">
+      <c r="C33" s="33">
+        <f t="shared" ref="C33:I33" si="4">SUM(C26:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="52"/>
-      <c r="B20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="52"/>
-      <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="52"/>
-      <c r="B22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="52"/>
-      <c r="B23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="52"/>
-      <c r="B24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="33">
-        <f t="shared" ref="C25:I25" si="4">SUM(C18:C24)</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="33">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="33">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="33">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="33">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="33">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="33">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="38" t="s">
-        <v>22</v>
-      </c>
+    <row r="35" spans="1:10" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+    </row>
+    <row r="37" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="A18:A24"/>
+  <mergeCells count="7">
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A26:A32"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Finish formatting of summary table.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -23,14 +23,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="88">
   <si>
     <t>Summary of change in productivity</t>
   </si>
   <si>
-    <t>Total land area (sq. km):</t>
-  </si>
-  <si>
     <t>Land area with improved productivity:</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Land area</t>
-  </si>
-  <si>
     <t>Total land sq. km</t>
   </si>
   <si>
@@ -244,9 +238,6 @@
     <t>Trends.Earth productivity summary table</t>
   </si>
   <si>
-    <t>Total land area (sq. km, baseline year):</t>
-  </si>
-  <si>
     <t>Trends.Earth soil organic carbon summary table</t>
   </si>
   <si>
@@ -287,14 +278,24 @@
   </si>
   <si>
     <t>Land cover in target year</t>
+  </si>
+  <si>
+    <t>Total land area:</t>
+  </si>
+  <si>
+    <t>Area (sq km)</t>
+  </si>
+  <si>
+    <t>Percent of total land area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -753,7 +754,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -834,9 +835,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -915,49 +913,86 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -987,23 +1022,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1020,9 +1040,28 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1346,24 +1385,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="57"/>
-    <col min="2" max="2" width="14.5703125" style="57" customWidth="1"/>
-    <col min="3" max="5" width="15.5703125" style="58" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="58" customWidth="1"/>
-    <col min="7" max="9" width="15.5703125" style="58" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="59" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="57"/>
+    <col min="1" max="1" width="9.140625" style="56"/>
+    <col min="2" max="2" width="14.5703125" style="56" customWidth="1"/>
+    <col min="3" max="5" width="15.5703125" style="57" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="57" customWidth="1"/>
+    <col min="7" max="9" width="15.5703125" style="57" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="58" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -1379,80 +1416,115 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A3" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+    </row>
+    <row r="4" spans="1:10" s="62" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="E5" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="30">
+      <c r="E5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
         <v>0</v>
+      </c>
+      <c r="G5" s="57">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="E6" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="33"/>
+      <c r="E6" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="68"/>
+      <c r="G6" s="32" t="e">
+        <f>F6/$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="E7" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="34"/>
+      <c r="E7" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="69"/>
+      <c r="G7" s="33" t="e">
+        <f t="shared" ref="G7:G9" si="0">F7/$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="63"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="E8" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="35"/>
+      <c r="E8" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="70"/>
+      <c r="G8" s="34" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="63"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="E9" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="36"/>
+      <c r="E9" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="35" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:10" s="60" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
+    <row r="11" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
-        <v>71</v>
+      <c r="A13" s="55" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1461,6 +1533,7 @@
     <mergeCell ref="A11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1468,22 +1541,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="57" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="57" customWidth="1"/>
-    <col min="3" max="9" width="15.5703125" style="58" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="59" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="57"/>
+    <col min="1" max="1" width="8.7109375" style="56" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="56" customWidth="1"/>
+    <col min="3" max="9" width="15.5703125" style="57" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="58" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1498,69 +1569,82 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="77"/>
-    </row>
-    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
+    </row>
+    <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
+      <c r="F4" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="E5" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="30">
-        <f>SUM(J21,J33,J45,J57)</f>
-        <v>0</v>
+      <c r="E5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="67">
+        <f>SUM(F6:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="73">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="E6" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="33" t="e">
-        <f>SUM(J14:J19)/F5</f>
+      <c r="E6" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="68"/>
+      <c r="G6" s="32" t="e">
+        <f>F6/$F$5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="E7" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="34" t="e">
-        <f>SUM(J26:J31)/F5</f>
+      <c r="E7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="69"/>
+      <c r="G7" s="33" t="e">
+        <f t="shared" ref="G7:G9" si="0">F7/$F$5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="E8" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="35" t="e">
-        <f>SUM(J38:J43)/F5</f>
+      <c r="E8" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="70"/>
+      <c r="G8" s="34" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="E9" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="36" t="e">
-        <f>SUM(J50:J55)/F5</f>
+      <c r="E9" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="35" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1568,63 +1652,63 @@
       <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="71"/>
+      <c r="A11" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="83"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="85"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
+      <c r="C12" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="G13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="H13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="I13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="J13" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="59" t="s">
+    </row>
+    <row r="14" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="86" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="65" t="s">
-        <v>16</v>
-      </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
@@ -1639,9 +1723,9 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
+      <c r="A15" s="87"/>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
@@ -1651,14 +1735,14 @@
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
       <c r="J15" s="28">
-        <f t="shared" ref="J15:J20" si="0">SUM(C15:I15)</f>
+        <f t="shared" ref="J15:J20" si="1">SUM(C15:I15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
+      <c r="A16" s="87"/>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
@@ -1668,14 +1752,14 @@
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
       <c r="J16" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
+      <c r="A17" s="87"/>
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
@@ -1685,14 +1769,14 @@
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
       <c r="J17" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
+      <c r="A18" s="87"/>
       <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
@@ -1702,14 +1786,14 @@
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
+      <c r="A19" s="87"/>
       <c r="B19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
@@ -1719,14 +1803,14 @@
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
       <c r="J19" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
+      <c r="A20" s="87"/>
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -1736,106 +1820,106 @@
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
       <c r="J20" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="28">
         <f>SUM(C14:C20)</f>
         <v>0</v>
       </c>
       <c r="D21" s="28">
-        <f t="shared" ref="D21:J21" si="1">SUM(D14:D20)</f>
+        <f t="shared" ref="D21:J21" si="2">SUM(D14:D20)</f>
         <v>0</v>
       </c>
       <c r="E21" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F21" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G21" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H21" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I21" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J21" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="71"/>
+      <c r="A23" s="88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="87"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="85"/>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
+      <c r="C24" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="I25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="59" t="s">
+    </row>
+    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="86" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
-        <v>16</v>
-      </c>
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -1850,9 +1934,9 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
+      <c r="A27" s="87"/>
       <c r="B27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -1862,14 +1946,14 @@
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
       <c r="J27" s="28">
-        <f t="shared" ref="J27:J32" si="2">SUM(C27:I27)</f>
+        <f t="shared" ref="J27:J32" si="3">SUM(C27:I27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
+      <c r="A28" s="87"/>
       <c r="B28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -1879,14 +1963,14 @@
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
+      <c r="A29" s="87"/>
       <c r="B29" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
@@ -1896,14 +1980,14 @@
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
       <c r="J29" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
@@ -1913,14 +1997,14 @@
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
       <c r="J30" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -1930,14 +2014,14 @@
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
       <c r="J31" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
@@ -1947,106 +2031,106 @@
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
       <c r="J32" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="28">
         <f>SUM(C26:C32)</f>
         <v>0</v>
       </c>
       <c r="D33" s="28">
-        <f t="shared" ref="D33:J33" si="3">SUM(D26:D32)</f>
+        <f t="shared" ref="D33:J33" si="4">SUM(D26:D32)</f>
         <v>0</v>
       </c>
       <c r="E33" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F33" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G33" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H33" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I33" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J33" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="69"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="71"/>
+      <c r="A35" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="84"/>
+      <c r="H35" s="84"/>
+      <c r="I35" s="84"/>
+      <c r="J35" s="85"/>
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
-      <c r="C36" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="73"/>
+      <c r="C36" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="78"/>
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="H37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="I37" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="J37" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J37" s="59" t="s">
+    </row>
+    <row r="38" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="86" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="65" t="s">
-        <v>16</v>
-      </c>
       <c r="B38" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -2061,9 +2145,9 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="66"/>
+      <c r="A39" s="87"/>
       <c r="B39" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
@@ -2073,14 +2157,14 @@
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
       <c r="J39" s="28">
-        <f t="shared" ref="J39:J44" si="4">SUM(C39:I39)</f>
+        <f t="shared" ref="J39:J44" si="5">SUM(C39:I39)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="66"/>
+      <c r="A40" s="87"/>
       <c r="B40" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
@@ -2090,14 +2174,14 @@
       <c r="H40" s="26"/>
       <c r="I40" s="26"/>
       <c r="J40" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="66"/>
+      <c r="A41" s="87"/>
       <c r="B41" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
@@ -2107,14 +2191,14 @@
       <c r="H41" s="26"/>
       <c r="I41" s="26"/>
       <c r="J41" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="66"/>
+      <c r="A42" s="87"/>
       <c r="B42" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
@@ -2124,14 +2208,14 @@
       <c r="H42" s="26"/>
       <c r="I42" s="26"/>
       <c r="J42" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="66"/>
+      <c r="A43" s="87"/>
       <c r="B43" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -2141,14 +2225,14 @@
       <c r="H43" s="26"/>
       <c r="I43" s="26"/>
       <c r="J43" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="66"/>
+      <c r="A44" s="87"/>
       <c r="B44" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -2158,106 +2242,106 @@
       <c r="H44" s="26"/>
       <c r="I44" s="26"/>
       <c r="J44" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C45" s="28">
         <f>SUM(C38:C44)</f>
         <v>0</v>
       </c>
       <c r="D45" s="28">
-        <f t="shared" ref="D45:J45" si="5">SUM(D38:D44)</f>
+        <f t="shared" ref="D45:J45" si="6">SUM(D38:D44)</f>
         <v>0</v>
       </c>
       <c r="E45" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F45" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G45" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H45" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I45" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J45" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="74" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="69"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="71"/>
+      <c r="A47" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="83"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="84"/>
+      <c r="F47" s="84"/>
+      <c r="G47" s="84"/>
+      <c r="H47" s="84"/>
+      <c r="I47" s="84"/>
+      <c r="J47" s="85"/>
     </row>
     <row r="48" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
-      <c r="C48" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="73"/>
+      <c r="C48" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
     </row>
     <row r="49" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="I49" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="J49" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J49" s="59" t="s">
+    </row>
+    <row r="50" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="86" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="65" t="s">
-        <v>16</v>
-      </c>
       <c r="B50" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="26"/>
@@ -2272,9 +2356,9 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="66"/>
+      <c r="A51" s="87"/>
       <c r="B51" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="26"/>
@@ -2284,14 +2368,14 @@
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
       <c r="J51" s="28">
-        <f t="shared" ref="J51:J56" si="6">SUM(C51:I51)</f>
+        <f t="shared" ref="J51:J56" si="7">SUM(C51:I51)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="66"/>
+      <c r="A52" s="87"/>
       <c r="B52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C52" s="26"/>
       <c r="D52" s="26"/>
@@ -2301,14 +2385,14 @@
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
       <c r="J52" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="66"/>
+      <c r="A53" s="87"/>
       <c r="B53" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C53" s="26"/>
       <c r="D53" s="26"/>
@@ -2318,14 +2402,14 @@
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
       <c r="J53" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="66"/>
+      <c r="A54" s="87"/>
       <c r="B54" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54" s="26"/>
       <c r="D54" s="26"/>
@@ -2335,14 +2419,14 @@
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
       <c r="J54" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="66"/>
+      <c r="A55" s="87"/>
       <c r="B55" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C55" s="26"/>
       <c r="D55" s="26"/>
@@ -2352,14 +2436,14 @@
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
       <c r="J55" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="66"/>
+      <c r="A56" s="87"/>
       <c r="B56" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C56" s="26"/>
       <c r="D56" s="26"/>
@@ -2369,75 +2453,69 @@
       <c r="H56" s="26"/>
       <c r="I56" s="26"/>
       <c r="J56" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="28">
         <f>SUM(C50:C56)</f>
         <v>0</v>
       </c>
       <c r="D57" s="28">
-        <f t="shared" ref="D57:J57" si="7">SUM(D50:D56)</f>
+        <f t="shared" ref="D57:J57" si="8">SUM(D50:D56)</f>
         <v>0</v>
       </c>
       <c r="E57" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F57" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G57" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H57" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I57" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J57" s="27">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" s="60" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" s="67"/>
-      <c r="C59" s="67"/>
-      <c r="D59" s="67"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="67"/>
-      <c r="G59" s="67"/>
-      <c r="H59" s="67"/>
-      <c r="I59" s="67"/>
-      <c r="J59" s="67"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="89"/>
+      <c r="C59" s="89"/>
+      <c r="D59" s="89"/>
+      <c r="E59" s="89"/>
+      <c r="F59" s="89"/>
+      <c r="G59" s="89"/>
+      <c r="H59" s="89"/>
+      <c r="I59" s="89"/>
+      <c r="J59" s="89"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="56" t="s">
-        <v>71</v>
+      <c r="A61" s="55" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A23:J23"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A26:A32"/>
@@ -2446,6 +2524,12 @@
     <mergeCell ref="A38:A44"/>
     <mergeCell ref="A47:J47"/>
     <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2456,120 +2540,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="57"/>
-    <col min="2" max="2" width="14.5703125" style="57" customWidth="1"/>
-    <col min="3" max="10" width="15.5703125" style="57" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="57"/>
+    <col min="1" max="1" width="9.140625" style="56"/>
+    <col min="2" max="2" width="14.5703125" style="56" customWidth="1"/>
+    <col min="3" max="10" width="15.5703125" style="56" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+    </row>
+    <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
+      <c r="F4" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="30">
-        <f>SUM(E16:E21)</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="67">
+        <f>SUM(F6:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="73">
+        <v>100</v>
+      </c>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="68"/>
+      <c r="G6" s="32" t="e">
+        <f>F6/$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="59"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="69"/>
+      <c r="G7" s="33" t="e">
+        <f t="shared" ref="G7:G9" si="0">F7/$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="59"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="70"/>
+      <c r="G8" s="34" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="59"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="35" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
-      <c r="F11" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="38" t="e">
+      <c r="F11" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="37" t="e">
         <f>I22/G22</f>
         <v>#DIV/0!</v>
       </c>
@@ -2578,52 +2680,52 @@
       <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="82" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
+      <c r="A13" s="94" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="95"/>
     </row>
     <row r="14" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="E15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="19" t="s">
+      <c r="H15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="I15" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="J15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="20" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="84"/>
+      <c r="A16" s="96"/>
       <c r="B16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
@@ -2638,141 +2740,141 @@
         <v>0</v>
       </c>
       <c r="I16" s="26">
-        <f t="shared" ref="I16:I21" si="0">H16-G16</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="37" t="e">
+        <f t="shared" ref="I16:I21" si="1">H16-G16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="36" t="e">
         <f>I16/G16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
+      <c r="A17" s="87"/>
       <c r="B17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29">
-        <f t="shared" ref="G17:H21" si="1">C17*E17*100</f>
+        <f t="shared" ref="G17:H21" si="2">C17*E17*100</f>
         <v>0</v>
       </c>
       <c r="H17" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="37" t="e">
-        <f t="shared" ref="J17:J21" si="2">I17/G17</f>
+      <c r="J17" s="36" t="e">
+        <f t="shared" ref="J17:J21" si="3">I17/G17</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
+      <c r="A18" s="87"/>
       <c r="B18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H18" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="37" t="e">
-        <f t="shared" si="2"/>
+      <c r="J18" s="36" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
+      <c r="A19" s="87"/>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="37" t="e">
-        <f t="shared" si="2"/>
+      <c r="J19" s="36" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
+      <c r="A20" s="87"/>
       <c r="B20" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H20" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="37" t="e">
-        <f t="shared" si="2"/>
+      <c r="J20" s="36" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
+      <c r="A21" s="87"/>
       <c r="B21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
       <c r="G21" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H21" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="37" t="e">
-        <f t="shared" si="2"/>
+      <c r="J21" s="36" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2780,7 +2882,7 @@
       <c r="A22" s="10"/>
       <c r="C22" s="28"/>
       <c r="D22" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="28">
         <f>SUM(E16:E21)</f>
@@ -2804,58 +2906,58 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
+      <c r="A24" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
+      <c r="J24" s="87"/>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
+      <c r="C25" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="87"/>
+      <c r="J25" s="87"/>
     </row>
     <row r="26" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="E26" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="F26" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="G26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="H26" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="27" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
-        <v>16</v>
+      <c r="A27" s="86" t="s">
+        <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -2865,9 +2967,9 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
+      <c r="A28" s="87"/>
       <c r="B28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -2877,9 +2979,9 @@
       <c r="H28" s="26"/>
     </row>
     <row r="29" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
+      <c r="A29" s="87"/>
       <c r="B29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
@@ -2889,9 +2991,9 @@
       <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
@@ -2901,9 +3003,9 @@
       <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -2913,9 +3015,9 @@
       <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
@@ -2924,58 +3026,58 @@
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
     </row>
-    <row r="33" spans="1:10" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="60" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="59"/>
-    </row>
-    <row r="34" spans="1:10" s="61" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="81"/>
-    </row>
-    <row r="36" spans="1:10" s="60" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="67"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+    </row>
+    <row r="34" spans="1:10" s="60" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="93"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
+    </row>
+    <row r="36" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="59"/>
+      <c r="A38" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2997,22 +3099,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="57" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="57" customWidth="1"/>
-    <col min="3" max="9" width="15.5703125" style="57" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="59" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="57"/>
+    <col min="1" max="1" width="8.7109375" style="56" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="56" customWidth="1"/>
+    <col min="3" max="9" width="15.5703125" style="56" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="58" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J1" s="14"/>
     </row>
@@ -3020,128 +3120,148 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="71"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="85"/>
+    </row>
+    <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
+      <c r="F4" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="30">
-        <f>SUM(C14:C19)</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="67">
+        <f>SUM(F6:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="73">
+        <v>100</v>
+      </c>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="68"/>
+      <c r="G6" s="32" t="e">
+        <f>F6/$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="69"/>
+      <c r="G7" s="33" t="e">
+        <f t="shared" ref="G7:G9" si="0">F7/$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="70"/>
+      <c r="G8" s="34" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="35" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
     </row>
     <row r="10" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="J10" s="57"/>
+      <c r="J10" s="56"/>
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="89"/>
+      <c r="A11" s="99" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="100"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="100"/>
+      <c r="J11" s="101"/>
     </row>
     <row r="12" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
-      <c r="J12" s="57"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="E13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="F13" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="14" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="84"/>
+      <c r="A14" s="96"/>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="26">
-        <f t="shared" ref="C14:C20" si="0">J26</f>
+        <f t="shared" ref="C14:C20" si="1">J26</f>
         <v>0</v>
       </c>
       <c r="D14" s="26">
@@ -3149,21 +3269,21 @@
         <v>0</v>
       </c>
       <c r="E14" s="26">
-        <f t="shared" ref="E14:E20" si="1">D14-C14</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="37" t="e">
-        <f t="shared" ref="F14:F20" si="2">(D14-C14)/C14</f>
+        <f t="shared" ref="E14:E20" si="2">D14-C14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="36" t="e">
+        <f t="shared" ref="F14:F20" si="3">(D14-C14)/C14</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
+      <c r="A15" s="87"/>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D15" s="26">
@@ -3171,21 +3291,21 @@
         <v>0</v>
       </c>
       <c r="E15" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="36" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="87"/>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="37" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="26">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D16" s="26">
@@ -3193,21 +3313,21 @@
         <v>0</v>
       </c>
       <c r="E16" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="36" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="87"/>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="37" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
-      <c r="B17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="26">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D17" s="26">
@@ -3215,21 +3335,21 @@
         <v>0</v>
       </c>
       <c r="E17" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="36" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="87"/>
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="37" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
-      <c r="B18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="26">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D18" s="26">
@@ -3237,21 +3357,21 @@
         <v>0</v>
       </c>
       <c r="E18" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="36" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="87"/>
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="37" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
-      <c r="B19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="26">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D19" s="26">
@@ -3259,21 +3379,21 @@
         <v>0</v>
       </c>
       <c r="E19" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="36" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="87"/>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="37" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="26">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D20" s="26">
@@ -3281,18 +3401,18 @@
         <v>0</v>
       </c>
       <c r="E20" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="37" t="e">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="36" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="28">
         <f>SUM(C14:C20)</f>
@@ -3315,63 +3435,63 @@
       <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="90" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="71"/>
+      <c r="A23" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="85"/>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
+      <c r="C24" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="E25" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="F25" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="G25" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="H25" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="I25" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="24" t="s">
+      <c r="J25" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="59" t="s">
+    </row>
+    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="86" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
-        <v>16</v>
-      </c>
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -3381,14 +3501,14 @@
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
       <c r="J26" s="28">
-        <f t="shared" ref="J26:J33" si="3">SUM(C26:I26)</f>
+        <f t="shared" ref="J26:J33" si="4">SUM(C26:I26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
+      <c r="A27" s="87"/>
       <c r="B27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -3398,14 +3518,14 @@
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
       <c r="J27" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
+      <c r="A28" s="87"/>
       <c r="B28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -3415,14 +3535,14 @@
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
+      <c r="A29" s="87"/>
       <c r="B29" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
@@ -3432,14 +3552,14 @@
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
       <c r="J29" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
@@ -3449,14 +3569,14 @@
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
       <c r="J30" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -3466,14 +3586,14 @@
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
       <c r="J31" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
@@ -3483,73 +3603,73 @@
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
       <c r="J32" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="60" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="28">
-        <f t="shared" ref="C33:I33" si="4">SUM(C26:C32)</f>
+        <f t="shared" ref="C33:I33" si="5">SUM(C26:C32)</f>
         <v>0</v>
       </c>
       <c r="D33" s="28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E33" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="27">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="60" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
+    </row>
+    <row r="35" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
+      <c r="A37" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3570,9 +3690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3583,7 +3701,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -3595,131 +3713,129 @@
       <c r="I1" s="13"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="2" spans="1:10" s="40" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
+    <row r="2" spans="1:10" s="39" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="92" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="103" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="C4" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="D4" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="51" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="113"/>
+      <c r="B5" s="43">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44">
+        <f>SUM(C5,D5,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="113"/>
+      <c r="B6" s="43">
+        <v>2005</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44">
+        <f>SUM(C6,D6,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="113"/>
+      <c r="B7" s="43">
+        <v>2010</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44">
+        <f>SUM(C7,D7,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="113"/>
+      <c r="B8" s="43">
+        <v>2015</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44">
+        <f>SUM(C8,D8,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="103"/>
+    </row>
+    <row r="11" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="45" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="96" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="44">
-        <v>2000</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45">
-        <f>SUM(C5,D5,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="96"/>
-      <c r="B6" s="44">
-        <v>2005</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45">
-        <f>SUM(C6,D6,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="44">
-        <v>2010</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45">
-        <f>SUM(C7,D7,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="96"/>
-      <c r="B8" s="44">
-        <v>2015</v>
-      </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45">
-        <f>SUM(C8,D8,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="92" t="s">
+      <c r="D11" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-    </row>
-    <row r="11" spans="1:10" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="46" t="s">
+      <c r="E11" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="F11" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="G11" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="H11" s="46" t="s">
         <v>46</v>
-      </c>
-      <c r="G11" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="47" t="s">
-        <v>48</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
-      <c r="B12" s="48">
+      <c r="B12" s="47">
         <v>2000</v>
       </c>
       <c r="C12" s="26">
@@ -3743,9 +3859,9 @@
       <c r="I12"/>
       <c r="J12"/>
     </row>
-    <row r="13" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
-      <c r="B13" s="48">
+      <c r="B13" s="47">
         <v>2001</v>
       </c>
       <c r="C13" s="26">
@@ -3769,8 +3885,8 @@
       <c r="I13"/>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="48">
+    <row r="14" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="47">
         <v>2002</v>
       </c>
       <c r="C14" s="26">
@@ -3792,8 +3908,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="48">
+    <row r="15" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="47">
         <v>2003</v>
       </c>
       <c r="C15" s="26">
@@ -3815,8 +3931,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="48">
+    <row r="16" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="74"/>
+      <c r="B16" s="47">
         <v>2004</v>
       </c>
       <c r="C16" s="26">
@@ -3838,8 +3955,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="48">
+    <row r="17" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="74"/>
+      <c r="B17" s="47">
         <v>2005</v>
       </c>
       <c r="C17" s="26">
@@ -3861,8 +3979,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="48">
+    <row r="18" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="74"/>
+      <c r="B18" s="47">
         <v>2006</v>
       </c>
       <c r="C18" s="26">
@@ -3884,8 +4003,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="48">
+    <row r="19" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="74"/>
+      <c r="B19" s="47">
         <v>2007</v>
       </c>
       <c r="C19" s="26">
@@ -3907,8 +4027,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="48">
+    <row r="20" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="74"/>
+      <c r="B20" s="47">
         <v>2008</v>
       </c>
       <c r="C20" s="26">
@@ -3930,8 +4051,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="48">
+    <row r="21" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="74"/>
+      <c r="B21" s="47">
         <v>2009</v>
       </c>
       <c r="C21" s="26">
@@ -3953,8 +4075,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="48">
+    <row r="22" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="74"/>
+      <c r="B22" s="47">
         <v>2010</v>
       </c>
       <c r="C22" s="26">
@@ -3977,8 +4100,8 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="48">
+      <c r="A23" s="74"/>
+      <c r="B23" s="47">
         <v>2011</v>
       </c>
       <c r="C23" s="26">
@@ -3999,12 +4122,12 @@
       <c r="H23" s="26">
         <v>0</v>
       </c>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="B24" s="48">
+      <c r="A24" s="74"/>
+      <c r="B24" s="47">
         <v>2012</v>
       </c>
       <c r="C24" s="26">
@@ -4025,12 +4148,12 @@
       <c r="H24" s="26">
         <v>0</v>
       </c>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="48">
+      <c r="A25" s="74"/>
+      <c r="B25" s="47">
         <v>2013</v>
       </c>
       <c r="C25" s="26">
@@ -4051,11 +4174,12 @@
       <c r="H25" s="26">
         <v>0</v>
       </c>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="48">
+      <c r="A26" s="74"/>
+      <c r="B26" s="47">
         <v>2014</v>
       </c>
       <c r="C26" s="26">
@@ -4078,7 +4202,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="48">
+      <c r="A27" s="74"/>
+      <c r="B27" s="47">
         <v>2015</v>
       </c>
       <c r="C27" s="26">
@@ -4101,8 +4226,8 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="49" t="s">
-        <v>49</v>
+      <c r="B28" s="48" t="s">
+        <v>47</v>
       </c>
       <c r="C28" s="28">
         <f t="shared" ref="C28:H28" si="0">SUM(C12:C27)</f>
@@ -4131,55 +4256,55 @@
     </row>
     <row r="29" spans="1:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="101" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="101"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="101"/>
-      <c r="H30" s="101"/>
-    </row>
-    <row r="31" spans="1:10" s="57" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="62"/>
-      <c r="C31" s="93" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="94"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="94"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="95"/>
+      <c r="B30" s="108" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="108"/>
+      <c r="H30" s="108"/>
+    </row>
+    <row r="31" spans="1:10" s="56" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="61"/>
+      <c r="C31" s="109" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="110"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="110"/>
+      <c r="G31" s="110"/>
+      <c r="H31" s="111"/>
     </row>
     <row r="32" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="51" t="s">
-        <v>43</v>
+      <c r="A32" s="38"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="50" t="s">
+        <v>41</v>
       </c>
       <c r="D32" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="F32" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="18" t="s">
+      <c r="G32" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="18" t="s">
-        <v>12</v>
-      </c>
       <c r="H32" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="102" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="53" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="112" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>41</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
@@ -4188,10 +4313,10 @@
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
     </row>
-    <row r="34" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
+    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="83"/>
       <c r="B34" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
@@ -4200,10 +4325,10 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
     </row>
-    <row r="35" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
+    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="83"/>
       <c r="B35" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
@@ -4212,10 +4337,10 @@
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="69"/>
+    <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="83"/>
       <c r="B36" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
@@ -4224,10 +4349,10 @@
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="69"/>
+    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="83"/>
       <c r="B37" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
@@ -4236,10 +4361,10 @@
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="69"/>
+    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="83"/>
       <c r="B38" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -4248,7 +4373,7 @@
       <c r="G38" s="26"/>
       <c r="H38" s="26"/>
     </row>
-    <row r="39" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -4260,55 +4385,57 @@
       <c r="I39"/>
     </row>
     <row r="40" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="101" t="s">
+      <c r="A40" s="116"/>
+      <c r="B40" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="108"/>
+      <c r="D40" s="108"/>
+      <c r="E40" s="108"/>
+      <c r="F40" s="108"/>
+      <c r="G40" s="108"/>
+      <c r="H40" s="108"/>
+    </row>
+    <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="116"/>
+      <c r="C41" s="109" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="110"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="110"/>
+      <c r="G41" s="110"/>
+      <c r="H41" s="111"/>
+    </row>
+    <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="38"/>
+      <c r="B42" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
-      <c r="E40" s="101"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
-      <c r="H40" s="101"/>
-    </row>
-    <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="39"/>
-      <c r="C41" s="93" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="94"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="94"/>
-      <c r="G41" s="94"/>
-      <c r="H41" s="95"/>
-    </row>
-    <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39"/>
-      <c r="B42" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="18" t="s">
+      <c r="E42" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="51" t="s">
+      <c r="F42" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="G42" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="H42" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G42" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="I42" s="39"/>
-    </row>
-    <row r="43" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="53" t="s">
-        <v>43</v>
+      <c r="I42" s="38"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="115"/>
+      <c r="B43" s="52" t="s">
+        <v>41</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -4317,9 +4444,10 @@
       <c r="G43" s="26"/>
       <c r="H43" s="26"/>
     </row>
-    <row r="44" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="115"/>
       <c r="B44" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -4328,9 +4456,10 @@
       <c r="G44" s="26"/>
       <c r="H44" s="26"/>
     </row>
-    <row r="45" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="115"/>
       <c r="B45" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
@@ -4339,9 +4468,10 @@
       <c r="G45" s="26"/>
       <c r="H45" s="26"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="115"/>
       <c r="B46" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C46" s="26"/>
       <c r="D46" s="26"/>
@@ -4350,9 +4480,10 @@
       <c r="G46" s="26"/>
       <c r="H46" s="26"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="115"/>
       <c r="B47" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C47" s="26"/>
       <c r="D47" s="26"/>
@@ -4361,10 +4492,10 @@
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
     </row>
-    <row r="48" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48"/>
+    <row r="48" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="115"/>
       <c r="B48" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
@@ -4375,7 +4506,7 @@
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" s="28"/>
       <c r="D49" s="28"/>
@@ -4385,55 +4516,55 @@
       <c r="H49" s="28"/>
     </row>
     <row r="50" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B50" s="92" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="92"/>
-      <c r="D50" s="92"/>
-      <c r="E50" s="92"/>
-      <c r="F50" s="92"/>
-      <c r="G50" s="92"/>
-      <c r="H50" s="92"/>
+      <c r="B50" s="103" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="103"/>
+      <c r="D50" s="103"/>
+      <c r="E50" s="103"/>
+      <c r="F50" s="103"/>
+      <c r="G50" s="103"/>
+      <c r="H50" s="103"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="39"/>
-      <c r="B51" s="98" t="s">
-        <v>60</v>
-      </c>
-      <c r="C51" s="99"/>
-      <c r="D51" s="99"/>
-      <c r="E51" s="99"/>
-      <c r="F51" s="99"/>
-      <c r="G51" s="99"/>
-      <c r="H51" s="100"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39"/>
+      <c r="A51" s="38"/>
+      <c r="B51" s="105" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="106"/>
+      <c r="D51" s="106"/>
+      <c r="E51" s="106"/>
+      <c r="F51" s="106"/>
+      <c r="G51" s="106"/>
+      <c r="H51" s="107"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="46" t="s">
+      <c r="B52" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="D52" s="46" t="s">
+      <c r="F52" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="46" t="s">
+      <c r="G52" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F52" s="46" t="s">
+      <c r="H52" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="G52" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="H52" s="47" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="48">
+      <c r="B53" s="47">
         <v>2000</v>
       </c>
       <c r="C53" s="26">
@@ -4456,7 +4587,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="48">
+      <c r="B54" s="47">
         <v>2001</v>
       </c>
       <c r="C54" s="26">
@@ -4479,7 +4610,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="48">
+      <c r="B55" s="47">
         <v>2002</v>
       </c>
       <c r="C55" s="26">
@@ -4502,7 +4633,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="48">
+      <c r="B56" s="47">
         <v>2003</v>
       </c>
       <c r="C56" s="26">
@@ -4525,7 +4656,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="48">
+      <c r="B57" s="47">
         <v>2004</v>
       </c>
       <c r="C57" s="26">
@@ -4548,7 +4679,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="48">
+      <c r="B58" s="47">
         <v>2005</v>
       </c>
       <c r="C58" s="26">
@@ -4571,7 +4702,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="48">
+      <c r="B59" s="47">
         <v>2006</v>
       </c>
       <c r="C59" s="26">
@@ -4594,7 +4725,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="48">
+      <c r="B60" s="47">
         <v>2007</v>
       </c>
       <c r="C60" s="26">
@@ -4617,7 +4748,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="48">
+      <c r="B61" s="47">
         <v>2008</v>
       </c>
       <c r="C61" s="26">
@@ -4640,7 +4771,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="48">
+      <c r="B62" s="47">
         <v>2009</v>
       </c>
       <c r="C62" s="26">
@@ -4663,7 +4794,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="48">
+      <c r="B63" s="47">
         <v>2010</v>
       </c>
       <c r="C63" s="26">
@@ -4686,7 +4817,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="48">
+      <c r="B64" s="47">
         <v>2011</v>
       </c>
       <c r="C64" s="26">
@@ -4709,7 +4840,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="48">
+      <c r="B65" s="47">
         <v>2012</v>
       </c>
       <c r="C65" s="26">
@@ -4732,7 +4863,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="48">
+      <c r="B66" s="47">
         <v>2013</v>
       </c>
       <c r="C66" s="26">
@@ -4754,9 +4885,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67"/>
-      <c r="B67" s="48">
+      <c r="B67" s="47">
         <v>2014</v>
       </c>
       <c r="C67" s="26">
@@ -4778,9 +4909,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68"/>
-      <c r="B68" s="48">
+      <c r="B68" s="47">
         <v>2015</v>
       </c>
       <c r="C68" s="26">
@@ -4802,7 +4933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -4812,57 +4943,56 @@
       <c r="G69"/>
       <c r="H69"/>
     </row>
-    <row r="70" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:10" s="39" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="55"/>
-      <c r="B71" s="97" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="97"/>
-      <c r="D71" s="97"/>
-      <c r="E71" s="97"/>
-      <c r="F71" s="97"/>
-      <c r="G71" s="97"/>
-      <c r="H71" s="97"/>
-    </row>
-    <row r="72" spans="1:10" s="39" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:10" s="38" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="54"/>
+      <c r="B71" s="104" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" s="104"/>
+      <c r="D71" s="104"/>
+      <c r="E71" s="104"/>
+      <c r="F71" s="104"/>
+      <c r="G71" s="104"/>
+      <c r="H71" s="104"/>
+    </row>
+    <row r="72" spans="1:10" s="38" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="1"/>
-      <c r="C72" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="86"/>
-      <c r="E72" s="86"/>
-      <c r="F72" s="86"/>
-      <c r="G72" s="86"/>
-      <c r="H72" s="86"/>
-    </row>
-    <row r="73" spans="1:10" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="91" t="s">
-        <v>16</v>
-      </c>
-      <c r="C73" s="54" t="s">
-        <v>43</v>
+      <c r="C72" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="98"/>
+      <c r="E72" s="98"/>
+      <c r="F72" s="98"/>
+      <c r="G72" s="98"/>
+      <c r="H72" s="98"/>
+    </row>
+    <row r="73" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="53" t="s">
+        <v>41</v>
       </c>
       <c r="D73" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E73" s="18" t="s">
+      <c r="F73" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F73" s="18" t="s">
+      <c r="G73" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G73" s="18" t="s">
-        <v>12</v>
-      </c>
       <c r="H73" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="91"/>
-      <c r="B74" s="54" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="114" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74" s="53" t="s">
+        <v>41</v>
       </c>
       <c r="C74" s="26"/>
       <c r="D74" s="26"/>
@@ -4871,10 +5001,10 @@
       <c r="G74" s="26"/>
       <c r="H74" s="26"/>
     </row>
-    <row r="75" spans="1:10" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="91"/>
+    <row r="75" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="114"/>
       <c r="B75" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C75" s="26"/>
       <c r="D75" s="26"/>
@@ -4883,10 +5013,10 @@
       <c r="G75" s="26"/>
       <c r="H75" s="26"/>
     </row>
-    <row r="76" spans="1:10" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="91"/>
+    <row r="76" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="114"/>
       <c r="B76" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C76" s="26"/>
       <c r="D76" s="26"/>
@@ -4895,10 +5025,10 @@
       <c r="G76" s="26"/>
       <c r="H76" s="26"/>
     </row>
-    <row r="77" spans="1:10" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="91"/>
+    <row r="77" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="114"/>
       <c r="B77" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C77" s="26"/>
       <c r="D77" s="26"/>
@@ -4907,10 +5037,10 @@
       <c r="G77" s="26"/>
       <c r="H77" s="26"/>
     </row>
-    <row r="78" spans="1:10" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="91"/>
+    <row r="78" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="114"/>
       <c r="B78" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C78" s="26"/>
       <c r="D78" s="26"/>
@@ -4920,9 +5050,9 @@
       <c r="H78" s="26"/>
     </row>
     <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="91"/>
+      <c r="A79" s="114"/>
       <c r="B79" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C79" s="26"/>
       <c r="D79" s="26"/>
@@ -4930,71 +5060,69 @@
       <c r="F79" s="26"/>
       <c r="G79" s="26"/>
       <c r="H79" s="26"/>
-      <c r="I79" s="39"/>
-      <c r="J79" s="39"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="38"/>
     </row>
     <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="39"/>
-      <c r="B80" s="39"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
-      <c r="F80" s="39"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="39"/>
-      <c r="I80" s="39"/>
-      <c r="J80" s="39"/>
+      <c r="A80" s="38"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+      <c r="J80" s="38"/>
     </row>
     <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="39"/>
-      <c r="B81" s="92" t="s">
-        <v>62</v>
-      </c>
-      <c r="C81" s="92"/>
-      <c r="D81" s="92"/>
-      <c r="E81" s="92"/>
-      <c r="F81" s="92"/>
-      <c r="G81" s="92"/>
-      <c r="H81" s="92"/>
-      <c r="I81" s="92"/>
-      <c r="J81" s="92"/>
+      <c r="A81" s="38"/>
+      <c r="B81" s="103" t="s">
+        <v>60</v>
+      </c>
+      <c r="C81" s="103"/>
+      <c r="D81" s="103"/>
+      <c r="E81" s="103"/>
+      <c r="F81" s="103"/>
+      <c r="G81" s="103"/>
+      <c r="H81" s="103"/>
+      <c r="I81" s="103"/>
+      <c r="J81" s="103"/>
     </row>
     <row r="82" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="39"/>
-      <c r="B82" s="44" t="s">
-        <v>59</v>
+      <c r="A82" s="38"/>
+      <c r="B82" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="C82" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D82" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D82" s="19" t="s">
+      <c r="E82" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F82" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G82" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E82" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G82" s="19" t="s">
+      <c r="H82" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H82" s="19" t="s">
+      <c r="I82" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I82" s="20" t="s">
+      <c r="J82" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J82" s="20" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="83" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="B83" s="54" t="s">
-        <v>43</v>
+      <c r="A83" s="10"/>
+      <c r="B83" s="53" t="s">
+        <v>41</v>
       </c>
       <c r="C83" s="29"/>
       <c r="D83" s="29"/>
@@ -5012,15 +5140,15 @@
         <f t="shared" ref="I83:I88" si="1">H83-G83</f>
         <v>0</v>
       </c>
-      <c r="J83" s="37" t="e">
+      <c r="J83" s="36" t="e">
         <f>I83/G83</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="66"/>
+      <c r="A84" s="38"/>
       <c r="B84" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C84" s="29"/>
       <c r="D84" s="29"/>
@@ -5038,15 +5166,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J84" s="37" t="e">
+      <c r="J84" s="36" t="e">
         <f t="shared" ref="J84:J88" si="3">I84/G84</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="66"/>
       <c r="B85" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C85" s="29"/>
       <c r="D85" s="29"/>
@@ -5064,15 +5191,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J85" s="37" t="e">
+      <c r="J85" s="36" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="66"/>
       <c r="B86" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C86" s="29"/>
       <c r="D86" s="29"/>
@@ -5090,15 +5216,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J86" s="37" t="e">
+      <c r="J86" s="36" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="66"/>
       <c r="B87" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C87" s="29"/>
       <c r="D87" s="29"/>
@@ -5116,15 +5241,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J87" s="37" t="e">
+      <c r="J87" s="36" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="66"/>
       <c r="B88" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="29"/>
@@ -5142,17 +5266,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J88" s="37" t="e">
+      <c r="J88" s="36" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="10"/>
-      <c r="B89" s="39"/>
+      <c r="B89" s="38"/>
       <c r="C89" s="28"/>
       <c r="D89" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E89" s="28">
         <f>SUM(E83:E88)</f>
@@ -5174,22 +5297,25 @@
         <f>SUM(I83:I88)</f>
         <v>0</v>
       </c>
-      <c r="J89" s="39"/>
+      <c r="J89" s="38"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="39"/>
-      <c r="B90" s="39"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="39"/>
-      <c r="I90" s="39"/>
-      <c r="J90" s="39"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="38"/>
+      <c r="J90" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="13">
+    <mergeCell ref="B81:J81"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A74:A79"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="C72:H72"/>
@@ -5199,12 +5325,6 @@
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="C41:H41"/>
-    <mergeCell ref="A73:A79"/>
-    <mergeCell ref="A83:A88"/>
-    <mergeCell ref="B81:J81"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A33:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Final tweaks to table formatting.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Productivity" sheetId="6" r:id="rId2"/>
     <sheet name="Soil organic carbon" sheetId="7" r:id="rId3"/>
     <sheet name="Land cover" sheetId="8" r:id="rId4"/>
-    <sheet name="UNCDD Reporting" sheetId="4" r:id="rId5"/>
+    <sheet name="UNCCD Reporting" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="88">
   <si>
     <t>Summary of change in productivity</t>
   </si>
@@ -124,12 +124,6 @@
     <t>Land area by type of land cover transition (sq. km)</t>
   </si>
   <si>
-    <t>Soil organic carbon change from baseline to target by type of land cover transition (tons)*</t>
-  </si>
-  <si>
-    <t>* trends.earth calculates soil organic carbon change based on annual land cover transitions. This table shows change in soil organic carbon based on the baseline and target years only. The target year soil organic carbon value used to produce this table accounts for all land cover transitions that ocurred between the baseline and target years.</t>
-  </si>
-  <si>
     <t>Page 3 of 34 - Country Profile</t>
   </si>
   <si>
@@ -287,6 +281,12 @@
   </si>
   <si>
     <t>Percent of total land area</t>
+  </si>
+  <si>
+    <t>* Trends.Earth calculates soil organic carbon change based on annual land cover transitions. This table shows change in soil organic carbon based on the baseline and target years only. The target year soil organic carbon value used to produce this table accounts for all land cover transitions that ocurred between the baseline and target years. An empty cell indicates that transition was not observed over the time period.</t>
+  </si>
+  <si>
+    <t>Soil organic carbon change from baseline to target by type of land cover transition (as percentage of initial stock)*</t>
   </si>
 </sst>
 </file>
@@ -754,7 +754,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -954,19 +954,37 @@
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,9 +1075,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1400,7 +1415,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -1416,18 +1431,18 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
+      <c r="A3" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="4" spans="1:10" s="62" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="64"/>
@@ -1435,10 +1450,10 @@
       <c r="D4" s="65"/>
       <c r="E4" s="65"/>
       <c r="F4" s="72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H4" s="65"/>
       <c r="I4" s="65"/>
@@ -1447,13 +1462,13 @@
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="116" t="e">
+      <c r="G5" s="77" t="e">
         <f>SUM(G6:G9)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1461,7 +1476,7 @@
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="E6" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -1473,7 +1488,7 @@
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="E7" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -1485,7 +1500,7 @@
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="E8" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -1497,7 +1512,7 @@
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="E9" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -1510,22 +1525,22 @@
       <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1555,7 +1570,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1570,38 +1585,38 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
+      <c r="A3" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="116" t="e">
+      <c r="G5" s="77" t="e">
         <f>SUM(G6:G9)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1654,30 +1669,30 @@
       <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="92" t="s">
+      <c r="A11" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="83"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="85"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="93"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="15" t="s">
@@ -1706,7 +1721,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1725,7 +1740,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="80"/>
+      <c r="A15" s="88"/>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1742,7 +1757,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
+      <c r="A16" s="88"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1759,7 +1774,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
+      <c r="A17" s="88"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1776,7 +1791,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1793,7 +1808,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
+      <c r="A19" s="88"/>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1825,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
+      <c r="A20" s="88"/>
       <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1865,30 +1880,30 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="93" t="s">
+      <c r="A23" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="85"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="93"/>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="95"/>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
@@ -1917,7 +1932,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="79" t="s">
+      <c r="A26" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1936,7 +1951,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="80"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1953,7 +1968,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
@@ -1970,7 +1985,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
+      <c r="A29" s="88"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
@@ -1987,7 +2002,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
+      <c r="A30" s="88"/>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
@@ -2004,7 +2019,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="80"/>
+      <c r="A31" s="88"/>
       <c r="B31" s="2" t="s">
         <v>12</v>
       </c>
@@ -2021,7 +2036,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="80"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
@@ -2076,30 +2091,30 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="82" t="s">
+      <c r="A35" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="83"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="84"/>
-      <c r="F35" s="84"/>
-      <c r="G35" s="84"/>
-      <c r="H35" s="84"/>
-      <c r="I35" s="84"/>
-      <c r="J35" s="85"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="92"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="92"/>
+      <c r="G35" s="92"/>
+      <c r="H35" s="92"/>
+      <c r="I35" s="92"/>
+      <c r="J35" s="93"/>
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
-      <c r="C36" s="86" t="s">
+      <c r="C36" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="87"/>
-      <c r="I36" s="87"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="95"/>
+      <c r="I36" s="95"/>
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
@@ -2128,7 +2143,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="79" t="s">
+      <c r="A38" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2147,7 +2162,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="80"/>
+      <c r="A39" s="88"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -2164,7 +2179,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="80"/>
+      <c r="A40" s="88"/>
       <c r="B40" s="2" t="s">
         <v>9</v>
       </c>
@@ -2181,7 +2196,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="80"/>
+      <c r="A41" s="88"/>
       <c r="B41" s="2" t="s">
         <v>10</v>
       </c>
@@ -2198,7 +2213,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="80"/>
+      <c r="A42" s="88"/>
       <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
@@ -2215,7 +2230,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="80"/>
+      <c r="A43" s="88"/>
       <c r="B43" s="2" t="s">
         <v>12</v>
       </c>
@@ -2232,7 +2247,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="80"/>
+      <c r="A44" s="88"/>
       <c r="B44" s="2" t="s">
         <v>13</v>
       </c>
@@ -2287,30 +2302,30 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="83"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
-      <c r="E47" s="84"/>
-      <c r="F47" s="84"/>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84"/>
-      <c r="I47" s="84"/>
-      <c r="J47" s="85"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
+      <c r="E47" s="92"/>
+      <c r="F47" s="92"/>
+      <c r="G47" s="92"/>
+      <c r="H47" s="92"/>
+      <c r="I47" s="92"/>
+      <c r="J47" s="93"/>
     </row>
     <row r="48" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
-      <c r="C48" s="86" t="s">
+      <c r="C48" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="87"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="87"/>
-      <c r="H48" s="87"/>
-      <c r="I48" s="87"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="95"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="95"/>
+      <c r="H48" s="95"/>
+      <c r="I48" s="95"/>
     </row>
     <row r="49" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="3" t="s">
@@ -2339,7 +2354,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="79" t="s">
+      <c r="A50" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2358,7 +2373,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="80"/>
+      <c r="A51" s="88"/>
       <c r="B51" s="2" t="s">
         <v>8</v>
       </c>
@@ -2375,7 +2390,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="80"/>
+      <c r="A52" s="88"/>
       <c r="B52" s="2" t="s">
         <v>9</v>
       </c>
@@ -2392,7 +2407,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="80"/>
+      <c r="A53" s="88"/>
       <c r="B53" s="2" t="s">
         <v>10</v>
       </c>
@@ -2409,7 +2424,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="80"/>
+      <c r="A54" s="88"/>
       <c r="B54" s="2" t="s">
         <v>11</v>
       </c>
@@ -2426,7 +2441,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="80"/>
+      <c r="A55" s="88"/>
       <c r="B55" s="2" t="s">
         <v>12</v>
       </c>
@@ -2443,7 +2458,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="80"/>
+      <c r="A56" s="88"/>
       <c r="B56" s="2" t="s">
         <v>13</v>
       </c>
@@ -2498,22 +2513,22 @@
       </c>
     </row>
     <row r="59" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="78" t="s">
+      <c r="A59" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="81"/>
-      <c r="C59" s="81"/>
-      <c r="D59" s="81"/>
-      <c r="E59" s="81"/>
-      <c r="F59" s="81"/>
-      <c r="G59" s="81"/>
-      <c r="H59" s="81"/>
-      <c r="I59" s="81"/>
-      <c r="J59" s="81"/>
+      <c r="B59" s="89"/>
+      <c r="C59" s="89"/>
+      <c r="D59" s="89"/>
+      <c r="E59" s="89"/>
+      <c r="F59" s="89"/>
+      <c r="G59" s="89"/>
+      <c r="H59" s="89"/>
+      <c r="I59" s="89"/>
+      <c r="J59" s="89"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2542,7 +2557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2554,33 +2569,33 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -2588,13 +2603,13 @@
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
       <c r="E5" s="31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="116" t="e">
+      <c r="G5" s="77" t="e">
         <f>SUM(G6:G9)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2607,7 +2622,7 @@
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
       <c r="E6" s="31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -2623,7 +2638,7 @@
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -2639,7 +2654,7 @@
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -2655,7 +2670,7 @@
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
       <c r="E9" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -2672,7 +2687,7 @@
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="F11" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G11" s="37" t="e">
         <f>I22/G22</f>
@@ -2683,18 +2698,18 @@
       <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="96" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
+      <c r="A13" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
     </row>
     <row r="14" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
@@ -2726,7 +2741,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
@@ -2752,7 +2767,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
+      <c r="A17" s="88"/>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2778,7 +2793,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2804,7 +2819,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
+      <c r="A19" s="88"/>
       <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2830,7 +2845,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
+      <c r="A20" s="88"/>
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
@@ -2856,7 +2871,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
+      <c r="A21" s="88"/>
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
@@ -2909,31 +2924,31 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="99" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
+      <c r="A24" s="107" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="100" t="s">
+      <c r="C25" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
     </row>
     <row r="26" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="18" t="s">
@@ -2956,122 +2971,122 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
     </row>
     <row r="28" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
     </row>
     <row r="29" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
+      <c r="A29" s="88"/>
       <c r="B29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
     </row>
     <row r="30" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
+      <c r="A30" s="88"/>
       <c r="B30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
     </row>
     <row r="31" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="80"/>
+      <c r="A31" s="88"/>
       <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="78"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="80"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
     </row>
     <row r="33" spans="1:10" s="60" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="79"/>
       <c r="I33" s="58"/>
       <c r="J33" s="58"/>
     </row>
-    <row r="34" spans="1:10" s="60" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="94" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="95"/>
-      <c r="C34" s="95"/>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="95"/>
+    <row r="34" spans="1:10" s="60" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="102" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="103"/>
+      <c r="C34" s="103"/>
+      <c r="D34" s="103"/>
+      <c r="E34" s="103"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
+      <c r="H34" s="103"/>
+      <c r="I34" s="103"/>
+      <c r="J34" s="103"/>
     </row>
     <row r="36" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="81"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="81"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C38" s="57"/>
       <c r="D38" s="57"/>
@@ -3102,9 +3117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3117,7 +3130,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J1" s="14"/>
     </row>
@@ -3125,26 +3138,26 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="85"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="93"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -3152,13 +3165,13 @@
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
       <c r="E5" s="31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="116" t="e">
+      <c r="G5" s="77" t="e">
         <f>SUM(G6:G9)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3170,7 +3183,7 @@
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
       <c r="E6" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -3185,7 +3198,7 @@
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -3200,7 +3213,7 @@
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -3215,7 +3228,7 @@
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
       <c r="E9" s="31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -3230,18 +3243,18 @@
       <c r="J10" s="56"/>
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="102"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="103"/>
+      <c r="A11" s="109" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="110"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="111"/>
     </row>
     <row r="12" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -3262,7 +3275,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="98"/>
+      <c r="A14" s="106"/>
       <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
@@ -3284,7 +3297,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="80"/>
+      <c r="A15" s="88"/>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -3306,7 +3319,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
+      <c r="A16" s="88"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -3328,7 +3341,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
+      <c r="A17" s="88"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
@@ -3350,7 +3363,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -3372,7 +3385,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
+      <c r="A19" s="88"/>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -3394,7 +3407,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
+      <c r="A20" s="88"/>
       <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
@@ -3441,30 +3454,30 @@
       <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="104" t="s">
+      <c r="A23" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="85"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="93"/>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="22" t="s">
@@ -3493,7 +3506,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="79" t="s">
+      <c r="A26" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -3512,7 +3525,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="80"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3529,7 +3542,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3546,7 +3559,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
+      <c r="A29" s="88"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
@@ -3563,7 +3576,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
+      <c r="A30" s="88"/>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
@@ -3580,7 +3593,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="80"/>
+      <c r="A31" s="88"/>
       <c r="B31" s="2" t="s">
         <v>12</v>
       </c>
@@ -3597,7 +3610,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="80"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
@@ -3652,22 +3665,22 @@
       </c>
     </row>
     <row r="35" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="81"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
-      <c r="I35" s="81"/>
-      <c r="J35" s="81"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C37" s="57"/>
       <c r="D37" s="57"/>
@@ -3694,7 +3707,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3707,7 +3720,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -3732,25 +3745,25 @@
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="51"/>
-      <c r="B3" s="105" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
+      <c r="B3" s="113" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="E4" s="50" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3803,38 +3816,38 @@
     </row>
     <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="51"/>
-      <c r="B10" s="105" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
+      <c r="B10" s="113" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
     </row>
     <row r="11" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" s="43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="F11" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="G11" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="H11" s="46" t="s">
         <v>44</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>46</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -4233,7 +4246,7 @@
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" s="28">
         <f t="shared" ref="C28:H28" si="0">SUM(C12:C27)</f>
@@ -4262,32 +4275,32 @@
     </row>
     <row r="29" spans="1:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="115" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="115"/>
-      <c r="D30" s="115"/>
-      <c r="E30" s="115"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="115"/>
-      <c r="H30" s="115"/>
+      <c r="B30" s="123" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="123"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="123"/>
+      <c r="H30" s="123"/>
     </row>
     <row r="31" spans="1:10" s="56" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="61"/>
-      <c r="C31" s="106" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="107"/>
-      <c r="E31" s="107"/>
-      <c r="F31" s="107"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="108"/>
+      <c r="C31" s="114" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="115"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="115"/>
+      <c r="G31" s="115"/>
+      <c r="H31" s="116"/>
     </row>
     <row r="32" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="38"/>
       <c r="B32" s="38"/>
       <c r="C32" s="50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>8</v>
@@ -4302,15 +4315,15 @@
         <v>11</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="109" t="s">
+      <c r="A33" s="117" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
@@ -4320,7 +4333,7 @@
       <c r="H33" s="26"/>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="83"/>
+      <c r="A34" s="91"/>
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
@@ -4332,7 +4345,7 @@
       <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="83"/>
+      <c r="A35" s="91"/>
       <c r="B35" s="2" t="s">
         <v>9</v>
       </c>
@@ -4344,7 +4357,7 @@
       <c r="H35" s="26"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="83"/>
+      <c r="A36" s="91"/>
       <c r="B36" s="2" t="s">
         <v>10</v>
       </c>
@@ -4356,7 +4369,7 @@
       <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="83"/>
+      <c r="A37" s="91"/>
       <c r="B37" s="2" t="s">
         <v>11</v>
       </c>
@@ -4368,9 +4381,9 @@
       <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="83"/>
+      <c r="A38" s="91"/>
       <c r="B38" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -4392,56 +4405,56 @@
     </row>
     <row r="40" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="76"/>
-      <c r="B40" s="115" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="115"/>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115"/>
-      <c r="F40" s="115"/>
-      <c r="G40" s="115"/>
-      <c r="H40" s="115"/>
+      <c r="B40" s="123" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="123"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="123"/>
     </row>
     <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="76"/>
-      <c r="C41" s="106" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" s="107"/>
-      <c r="E41" s="107"/>
-      <c r="F41" s="107"/>
-      <c r="G41" s="107"/>
-      <c r="H41" s="108"/>
+      <c r="C41" s="114" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="115"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="115"/>
+      <c r="G41" s="115"/>
+      <c r="H41" s="116"/>
     </row>
     <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="38"/>
       <c r="B42" s="49" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C42" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="50" t="s">
+      <c r="F42" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="G42" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="H42" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>55</v>
       </c>
       <c r="I42" s="38"/>
     </row>
     <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="75"/>
       <c r="B43" s="52" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -4501,7 +4514,7 @@
     <row r="48" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="75"/>
       <c r="B48" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
@@ -4522,51 +4535,51 @@
       <c r="H49" s="28"/>
     </row>
     <row r="50" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B50" s="105" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" s="105"/>
-      <c r="D50" s="105"/>
-      <c r="E50" s="105"/>
-      <c r="F50" s="105"/>
-      <c r="G50" s="105"/>
-      <c r="H50" s="105"/>
+      <c r="B50" s="113" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="113"/>
+      <c r="D50" s="113"/>
+      <c r="E50" s="113"/>
+      <c r="F50" s="113"/>
+      <c r="G50" s="113"/>
+      <c r="H50" s="113"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="38"/>
-      <c r="B51" s="112" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="113"/>
-      <c r="D51" s="113"/>
-      <c r="E51" s="113"/>
-      <c r="F51" s="113"/>
-      <c r="G51" s="113"/>
-      <c r="H51" s="114"/>
+      <c r="B51" s="120" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="121"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="121"/>
+      <c r="F51" s="121"/>
+      <c r="G51" s="121"/>
+      <c r="H51" s="122"/>
       <c r="I51" s="38"/>
       <c r="J51" s="38"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" s="43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C52" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="D52" s="45" t="s">
+      <c r="F52" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="45" t="s">
+      <c r="G52" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="F52" s="45" t="s">
+      <c r="H52" s="46" t="s">
         <v>44</v>
-      </c>
-      <c r="G52" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="H52" s="46" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -4952,30 +4965,30 @@
     <row r="70" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="71" spans="1:10" s="38" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="54"/>
-      <c r="B71" s="111" t="s">
-        <v>61</v>
-      </c>
-      <c r="C71" s="111"/>
-      <c r="D71" s="111"/>
-      <c r="E71" s="111"/>
-      <c r="F71" s="111"/>
-      <c r="G71" s="111"/>
-      <c r="H71" s="111"/>
+      <c r="B71" s="119" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="119"/>
+      <c r="D71" s="119"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
+      <c r="G71" s="119"/>
+      <c r="H71" s="119"/>
     </row>
     <row r="72" spans="1:10" s="38" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="1"/>
-      <c r="C72" s="100" t="s">
+      <c r="C72" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="100"/>
-      <c r="E72" s="100"/>
-      <c r="F72" s="100"/>
-      <c r="G72" s="100"/>
-      <c r="H72" s="100"/>
+      <c r="D72" s="108"/>
+      <c r="E72" s="108"/>
+      <c r="F72" s="108"/>
+      <c r="G72" s="108"/>
+      <c r="H72" s="108"/>
     </row>
     <row r="73" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>8</v>
@@ -4990,15 +5003,15 @@
         <v>11</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="110" t="s">
+      <c r="A74" s="118" t="s">
         <v>15</v>
       </c>
       <c r="B74" s="53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C74" s="26"/>
       <c r="D74" s="26"/>
@@ -5008,7 +5021,7 @@
       <c r="H74" s="26"/>
     </row>
     <row r="75" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="110"/>
+      <c r="A75" s="118"/>
       <c r="B75" s="2" t="s">
         <v>8</v>
       </c>
@@ -5020,7 +5033,7 @@
       <c r="H75" s="26"/>
     </row>
     <row r="76" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="110"/>
+      <c r="A76" s="118"/>
       <c r="B76" s="2" t="s">
         <v>9</v>
       </c>
@@ -5032,7 +5045,7 @@
       <c r="H76" s="26"/>
     </row>
     <row r="77" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="110"/>
+      <c r="A77" s="118"/>
       <c r="B77" s="2" t="s">
         <v>10</v>
       </c>
@@ -5044,7 +5057,7 @@
       <c r="H77" s="26"/>
     </row>
     <row r="78" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="110"/>
+      <c r="A78" s="118"/>
       <c r="B78" s="2" t="s">
         <v>11</v>
       </c>
@@ -5056,9 +5069,9 @@
       <c r="H78" s="26"/>
     </row>
     <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="110"/>
+      <c r="A79" s="118"/>
       <c r="B79" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C79" s="26"/>
       <c r="D79" s="26"/>
@@ -5083,22 +5096,22 @@
     </row>
     <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="38"/>
-      <c r="B81" s="105" t="s">
-        <v>60</v>
-      </c>
-      <c r="C81" s="105"/>
-      <c r="D81" s="105"/>
-      <c r="E81" s="105"/>
-      <c r="F81" s="105"/>
-      <c r="G81" s="105"/>
-      <c r="H81" s="105"/>
-      <c r="I81" s="105"/>
-      <c r="J81" s="105"/>
+      <c r="B81" s="113" t="s">
+        <v>58</v>
+      </c>
+      <c r="C81" s="113"/>
+      <c r="D81" s="113"/>
+      <c r="E81" s="113"/>
+      <c r="F81" s="113"/>
+      <c r="G81" s="113"/>
+      <c r="H81" s="113"/>
+      <c r="I81" s="113"/>
+      <c r="J81" s="113"/>
     </row>
     <row r="82" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="38"/>
       <c r="B82" s="43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C82" s="19" t="s">
         <v>21</v>
@@ -5128,7 +5141,7 @@
     <row r="83" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C83" s="29"/>
       <c r="D83" s="29"/>
@@ -5254,7 +5267,7 @@
     </row>
     <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="29"/>
@@ -5316,12 +5329,45 @@
       <c r="I90" s="38"/>
       <c r="J90" s="38"/>
     </row>
+    <row r="91" spans="1:10" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" s="86"/>
+      <c r="C91" s="86"/>
+      <c r="D91" s="86"/>
+      <c r="E91" s="86"/>
+      <c r="F91" s="86"/>
+      <c r="G91" s="86"/>
+      <c r="H91" s="86"/>
+      <c r="I91" s="86"/>
+      <c r="J91" s="86"/>
+    </row>
+    <row r="92" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="83"/>
+      <c r="D92" s="83"/>
+      <c r="E92" s="83"/>
+      <c r="F92" s="83"/>
+      <c r="G92" s="83"/>
+      <c r="H92" s="83"/>
+      <c r="I92" s="83"/>
+      <c r="J92" s="82"/>
+    </row>
+    <row r="93" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="C93" s="83"/>
+      <c r="D93" s="83"/>
+      <c r="E93" s="83"/>
+      <c r="F93" s="83"/>
+      <c r="G93" s="83"/>
+      <c r="H93" s="83"/>
+      <c r="I93" s="83"/>
+      <c r="J93" s="82"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B81:J81"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A74:A79"/>
+  <mergeCells count="14">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="C72:H72"/>
@@ -5331,6 +5377,11 @@
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="C41:H41"/>
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="B81:J81"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A74:A79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Use "Other land" rather than "Bare land". Also improve lc definition reading.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10250"/>
   </bookViews>
   <sheets>
     <sheet name="SDG 15.3.1" sheetId="5" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>Artificial areas</t>
   </si>
   <si>
-    <t>Bare lands</t>
-  </si>
-  <si>
     <t>Water bodies</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>Soil organic carbon change from baseline to target by type of land cover transition (as percentage of initial stock)*</t>
+  </si>
+  <si>
+    <t>Other lands</t>
   </si>
 </sst>
 </file>
@@ -978,43 +978,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1047,6 +1047,21 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1061,21 +1076,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1402,20 +1402,20 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="56"/>
-    <col min="2" max="2" width="14.5703125" style="56" customWidth="1"/>
-    <col min="3" max="5" width="15.5703125" style="57" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="57" customWidth="1"/>
-    <col min="7" max="9" width="15.5703125" style="57" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="58" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="56"/>
+    <col min="1" max="1" width="9.1796875" style="56"/>
+    <col min="2" max="2" width="14.54296875" style="56" customWidth="1"/>
+    <col min="3" max="5" width="15.54296875" style="57" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" style="57" customWidth="1"/>
+    <col min="7" max="9" width="15.54296875" style="57" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="58" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -1427,12 +1427,12 @@
       <c r="I1" s="13"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -1444,25 +1444,25 @@
       <c r="I3" s="85"/>
       <c r="J3" s="85"/>
     </row>
-    <row r="4" spans="1:10" s="62" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="62" customFormat="1" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="64"/>
       <c r="C4" s="65"/>
       <c r="D4" s="65"/>
       <c r="E4" s="65"/>
       <c r="F4" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="72" t="s">
         <v>84</v>
-      </c>
-      <c r="G4" s="72" t="s">
-        <v>85</v>
       </c>
       <c r="H4" s="65"/>
       <c r="I4" s="65"/>
       <c r="J4" s="66"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
@@ -1473,10 +1473,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="E6" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -1485,10 +1485,10 @@
       </c>
       <c r="H6" s="63"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="E7" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -1497,10 +1497,10 @@
       </c>
       <c r="H7" s="63"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="E8" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -1509,10 +1509,10 @@
       </c>
       <c r="H8" s="63"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="E9" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -1521,12 +1521,12 @@
       </c>
       <c r="H9" s="63"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="86"/>
       <c r="C11" s="86"/>
@@ -1538,9 +1538,9 @@
       <c r="I11" s="86"/>
       <c r="J11" s="86"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1559,18 +1559,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="56" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="56" customWidth="1"/>
-    <col min="3" max="9" width="15.5703125" style="57" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="58" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="56"/>
+    <col min="1" max="1" width="8.7265625" style="56" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="56" customWidth="1"/>
+    <col min="3" max="9" width="15.54296875" style="57" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="58" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1581,36 +1581,36 @@
       <c r="I1" s="13"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="99"/>
-    </row>
-    <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="91"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
@@ -1621,7 +1621,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="E6" s="31" t="s">
         <v>1</v>
@@ -1632,7 +1632,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="E7" s="31" t="s">
         <v>2</v>
@@ -1643,7 +1643,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="E8" s="31" t="s">
         <v>3</v>
@@ -1654,7 +1654,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="E9" s="31" t="s">
         <v>4</v>
@@ -1665,36 +1665,36 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="100" t="s">
+    <row r="11" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="93"/>
-    </row>
-    <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="93"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="95"/>
+    </row>
+    <row r="12" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
-      <c r="C12" s="94" t="s">
+      <c r="C12" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="95"/>
-      <c r="I12" s="95"/>
-    </row>
-    <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+    </row>
+    <row r="13" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="15" t="s">
         <v>7</v>
       </c>
@@ -1711,18 +1711,18 @@
         <v>11</v>
       </c>
       <c r="H13" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="J13" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="58" t="s">
+    </row>
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="96" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="87" t="s">
-        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>7</v>
@@ -1739,8 +1739,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="88"/>
+    <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="97"/>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1756,8 +1756,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="88"/>
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="97"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1773,8 +1773,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88"/>
+    <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="97"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1790,8 +1790,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
+    <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="97"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1807,10 +1807,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
+    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="97"/>
       <c r="B19" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
@@ -1824,10 +1824,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
+    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="97"/>
       <c r="B20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -1841,10 +1841,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="28">
         <f>SUM(C14:C20)</f>
@@ -1879,33 +1879,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="101" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="88"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="93"/>
-    </row>
-    <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="97"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="95"/>
+    </row>
+    <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="94" t="s">
+      <c r="C24" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-    </row>
-    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+    </row>
+    <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1922,18 +1922,18 @@
         <v>11</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="58" t="s">
+    </row>
+    <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="96" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="87" t="s">
-        <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
@@ -1950,8 +1950,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
+    <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="97"/>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1967,8 +1967,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="88"/>
+    <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="97"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
@@ -1984,8 +1984,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="88"/>
+    <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="97"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
@@ -2001,8 +2001,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="88"/>
+    <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="97"/>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
@@ -2018,10 +2018,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="88"/>
+    <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="97"/>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -2035,10 +2035,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="88"/>
+    <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="97"/>
       <c r="B32" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
@@ -2052,10 +2052,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33" s="28">
         <f>SUM(C26:C32)</f>
@@ -2090,33 +2090,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="91"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="92"/>
-      <c r="G35" s="92"/>
-      <c r="H35" s="92"/>
-      <c r="I35" s="92"/>
-      <c r="J35" s="93"/>
-    </row>
-    <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="93"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="95"/>
+    </row>
+    <row r="36" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="1"/>
-      <c r="C36" s="94" t="s">
+      <c r="C36" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
-      <c r="I36" s="95"/>
-    </row>
-    <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="88"/>
+    </row>
+    <row r="37" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2133,18 +2133,18 @@
         <v>11</v>
       </c>
       <c r="H37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="J37" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J37" s="58" t="s">
+    </row>
+    <row r="38" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="96" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="87" t="s">
-        <v>15</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>7</v>
@@ -2161,8 +2161,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="88"/>
+    <row r="39" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="97"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -2178,8 +2178,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="88"/>
+    <row r="40" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="97"/>
       <c r="B40" s="2" t="s">
         <v>9</v>
       </c>
@@ -2195,8 +2195,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="88"/>
+    <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="97"/>
       <c r="B41" s="2" t="s">
         <v>10</v>
       </c>
@@ -2212,8 +2212,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="88"/>
+    <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="97"/>
       <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
@@ -2229,10 +2229,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="88"/>
+    <row r="43" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="97"/>
       <c r="B43" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -2246,10 +2246,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="88"/>
+    <row r="44" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="97"/>
       <c r="B44" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -2263,10 +2263,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
       <c r="B45" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45" s="28">
         <f>SUM(C38:C44)</f>
@@ -2301,33 +2301,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="96" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" s="91"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="92"/>
-      <c r="E47" s="92"/>
-      <c r="F47" s="92"/>
-      <c r="G47" s="92"/>
-      <c r="H47" s="92"/>
-      <c r="I47" s="92"/>
-      <c r="J47" s="93"/>
-    </row>
-    <row r="48" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="93"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="94"/>
+      <c r="E47" s="94"/>
+      <c r="F47" s="94"/>
+      <c r="G47" s="94"/>
+      <c r="H47" s="94"/>
+      <c r="I47" s="94"/>
+      <c r="J47" s="95"/>
+    </row>
+    <row r="48" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="1"/>
-      <c r="C48" s="94" t="s">
+      <c r="C48" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="95"/>
-      <c r="E48" s="95"/>
-      <c r="F48" s="95"/>
-      <c r="G48" s="95"/>
-      <c r="H48" s="95"/>
-      <c r="I48" s="95"/>
-    </row>
-    <row r="49" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="88"/>
+      <c r="E48" s="88"/>
+      <c r="F48" s="88"/>
+      <c r="G48" s="88"/>
+      <c r="H48" s="88"/>
+      <c r="I48" s="88"/>
+    </row>
+    <row r="49" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2344,18 +2344,18 @@
         <v>11</v>
       </c>
       <c r="H49" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I49" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="J49" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J49" s="58" t="s">
+    </row>
+    <row r="50" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="96" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="87" t="s">
-        <v>15</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>7</v>
@@ -2372,8 +2372,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="88"/>
+    <row r="51" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="97"/>
       <c r="B51" s="2" t="s">
         <v>8</v>
       </c>
@@ -2389,8 +2389,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="88"/>
+    <row r="52" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="97"/>
       <c r="B52" s="2" t="s">
         <v>9</v>
       </c>
@@ -2406,8 +2406,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="88"/>
+    <row r="53" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="97"/>
       <c r="B53" s="2" t="s">
         <v>10</v>
       </c>
@@ -2423,8 +2423,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="88"/>
+    <row r="54" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="97"/>
       <c r="B54" s="2" t="s">
         <v>11</v>
       </c>
@@ -2440,10 +2440,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="88"/>
+    <row r="55" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="97"/>
       <c r="B55" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C55" s="26"/>
       <c r="D55" s="26"/>
@@ -2457,10 +2457,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="88"/>
+    <row r="56" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="97"/>
       <c r="B56" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C56" s="26"/>
       <c r="D56" s="26"/>
@@ -2474,10 +2474,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C57" s="28">
         <f>SUM(C50:C56)</f>
@@ -2512,33 +2512,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="86" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="89"/>
-      <c r="C59" s="89"/>
-      <c r="D59" s="89"/>
-      <c r="E59" s="89"/>
-      <c r="F59" s="89"/>
-      <c r="G59" s="89"/>
-      <c r="H59" s="89"/>
-      <c r="I59" s="89"/>
-      <c r="J59" s="89"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B59" s="99"/>
+      <c r="C59" s="99"/>
+      <c r="D59" s="99"/>
+      <c r="E59" s="99"/>
+      <c r="F59" s="99"/>
+      <c r="G59" s="99"/>
+      <c r="H59" s="99"/>
+      <c r="I59" s="99"/>
+      <c r="J59" s="99"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A23:J23"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A26:A32"/>
@@ -2547,6 +2541,12 @@
     <mergeCell ref="A38:A44"/>
     <mergeCell ref="A47:J47"/>
     <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2559,51 +2559,51 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="56"/>
-    <col min="2" max="2" width="14.5703125" style="56" customWidth="1"/>
-    <col min="3" max="10" width="15.5703125" style="56" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="56"/>
+    <col min="1" max="1" width="9.1796875" style="56"/>
+    <col min="2" max="2" width="14.54296875" style="56" customWidth="1"/>
+    <col min="3" max="10" width="15.54296875" style="56" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-    </row>
-    <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
       <c r="E5" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
@@ -2617,12 +2617,12 @@
       <c r="I5" s="57"/>
       <c r="J5" s="58"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
       <c r="E6" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -2633,12 +2633,12 @@
       <c r="I6" s="57"/>
       <c r="J6" s="58"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -2649,12 +2649,12 @@
       <c r="I7" s="57"/>
       <c r="J7" s="58"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -2665,12 +2665,12 @@
       <c r="I8" s="57"/>
       <c r="J8" s="58"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
       <c r="E9" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -2681,25 +2681,25 @@
       <c r="I9" s="57"/>
       <c r="J9" s="58"/>
     </row>
-    <row r="10" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="F11" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" s="37" t="e">
         <f>I22/G22</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="104" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="105"/>
       <c r="C13" s="105"/>
@@ -2711,36 +2711,36 @@
       <c r="I13" s="105"/>
       <c r="J13" s="105"/>
     </row>
-    <row r="14" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="E15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="19" t="s">
+      <c r="H15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="I15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="J15" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="106"/>
       <c r="B16" s="2" t="s">
         <v>7</v>
@@ -2766,8 +2766,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88"/>
+    <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="97"/>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2792,8 +2792,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
+    <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="97"/>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2818,8 +2818,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
+    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="97"/>
       <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2844,8 +2844,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
+    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="97"/>
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
@@ -2870,10 +2870,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="88"/>
+    <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="97"/>
       <c r="B21" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2896,11 +2896,11 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10"/>
       <c r="C22" s="28"/>
       <c r="D22" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" s="28">
         <f>SUM(E16:E21)</f>
@@ -2923,34 +2923,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="107" t="s">
-        <v>87</v>
-      </c>
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
-    </row>
-    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="B24" s="97"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+    </row>
+    <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
-    </row>
-    <row r="26" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="97"/>
+    </row>
+    <row r="26" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="18" t="s">
         <v>7</v>
       </c>
@@ -2967,12 +2967,12 @@
         <v>11</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="87" t="s">
-        <v>15</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="96" t="s">
+        <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
@@ -2984,8 +2984,8 @@
       <c r="G27" s="78"/>
       <c r="H27" s="78"/>
     </row>
-    <row r="28" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="88"/>
+    <row r="28" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="97"/>
       <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
@@ -2996,8 +2996,8 @@
       <c r="G28" s="78"/>
       <c r="H28" s="78"/>
     </row>
-    <row r="29" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="88"/>
+    <row r="29" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="97"/>
       <c r="B29" s="2" t="s">
         <v>9</v>
       </c>
@@ -3008,8 +3008,8 @@
       <c r="G29" s="78"/>
       <c r="H29" s="78"/>
     </row>
-    <row r="30" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="88"/>
+    <row r="30" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="97"/>
       <c r="B30" s="2" t="s">
         <v>10</v>
       </c>
@@ -3020,8 +3020,8 @@
       <c r="G30" s="78"/>
       <c r="H30" s="78"/>
     </row>
-    <row r="31" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="88"/>
+    <row r="31" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="97"/>
       <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
@@ -3032,10 +3032,10 @@
       <c r="G31" s="78"/>
       <c r="H31" s="78"/>
     </row>
-    <row r="32" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="88"/>
+    <row r="32" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="97"/>
       <c r="B32" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C32" s="78"/>
       <c r="D32" s="78"/>
@@ -3044,7 +3044,7 @@
       <c r="G32" s="78"/>
       <c r="H32" s="78"/>
     </row>
-    <row r="33" spans="1:10" s="60" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="60" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="79"/>
@@ -3056,9 +3056,9 @@
       <c r="I33" s="58"/>
       <c r="J33" s="58"/>
     </row>
-    <row r="34" spans="1:10" s="60" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="60" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="102" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" s="103"/>
       <c r="C34" s="103"/>
@@ -3070,23 +3070,23 @@
       <c r="I34" s="103"/>
       <c r="J34" s="103"/>
     </row>
-    <row r="36" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="86" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B36" s="99"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="99"/>
+      <c r="J36" s="99"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="57"/>
       <c r="D38" s="57"/>
@@ -3119,53 +3119,53 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="56" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="56" customWidth="1"/>
-    <col min="3" max="9" width="15.5703125" style="56" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="58" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="56"/>
+    <col min="1" max="1" width="8.7265625" style="56" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="56" customWidth="1"/>
+    <col min="3" max="9" width="15.54296875" style="56" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="58" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J1" s="14"/>
     </row>
-    <row r="2" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="93"/>
-    </row>
-    <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="95"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
       <c r="E5" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
@@ -3178,12 +3178,12 @@
       <c r="H5" s="57"/>
       <c r="I5" s="57"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
       <c r="E6" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -3193,12 +3193,12 @@
       <c r="H6" s="57"/>
       <c r="I6" s="57"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -3208,12 +3208,12 @@
       <c r="H7" s="57"/>
       <c r="I7" s="57"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -3223,12 +3223,12 @@
       <c r="H8" s="57"/>
       <c r="I8" s="57"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
       <c r="E9" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -3238,13 +3238,13 @@
       <c r="H9" s="57"/>
       <c r="I9" s="57"/>
     </row>
-    <row r="10" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
       <c r="J10" s="56"/>
     </row>
-    <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="109" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="110"/>
       <c r="C11" s="110"/>
@@ -3256,25 +3256,25 @@
       <c r="I11" s="110"/>
       <c r="J11" s="111"/>
     </row>
-    <row r="12" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
       <c r="J12" s="56"/>
     </row>
-    <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="E13" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="F13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="106"/>
       <c r="B14" s="2" t="s">
         <v>7</v>
@@ -3296,8 +3296,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="88"/>
+    <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="97"/>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -3318,8 +3318,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="88"/>
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="97"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -3340,8 +3340,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88"/>
+    <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="97"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
@@ -3362,8 +3362,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
+    <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="97"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -3384,10 +3384,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
+    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="97"/>
       <c r="B19" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C19" s="26">
         <f t="shared" si="1"/>
@@ -3406,10 +3406,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
+    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="97"/>
       <c r="B20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="26">
         <f t="shared" si="1"/>
@@ -3428,10 +3428,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="28">
         <f>SUM(C14:C20)</f>
@@ -3447,39 +3447,39 @@
       </c>
       <c r="F21" s="25"/>
     </row>
-    <row r="22" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5"/>
       <c r="B22" s="7"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
     </row>
-    <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="112" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="88"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="93"/>
-    </row>
-    <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="95"/>
+    </row>
+    <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="94" t="s">
+      <c r="C24" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-    </row>
-    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+    </row>
+    <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="22" t="s">
         <v>7</v>
       </c>
@@ -3496,18 +3496,18 @@
         <v>11</v>
       </c>
       <c r="H25" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="24" t="s">
+      <c r="J25" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="58" t="s">
+    </row>
+    <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="96" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="87" t="s">
-        <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
@@ -3524,8 +3524,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
+    <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="97"/>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3541,8 +3541,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="88"/>
+    <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="97"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3558,8 +3558,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="88"/>
+    <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="97"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
@@ -3575,8 +3575,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="88"/>
+    <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="97"/>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
@@ -3592,10 +3592,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="88"/>
+    <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="97"/>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -3609,10 +3609,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="88"/>
+    <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="97"/>
       <c r="B32" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
@@ -3626,10 +3626,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="60" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="60" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33" s="28">
         <f t="shared" ref="C33:I33" si="5">SUM(C26:C32)</f>
@@ -3664,23 +3664,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="86" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B35" s="99"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="99"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="99"/>
+      <c r="J35" s="99"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="57"/>
       <c r="D37" s="57"/>
@@ -3711,16 +3711,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="10" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+    <col min="3" max="10" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -3732,7 +3732,7 @@
       <c r="I1" s="13"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="2" spans="1:10" s="39" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="39" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="40"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -3743,30 +3743,30 @@
       <c r="H2" s="41"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="51"/>
       <c r="B3" s="113" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="113"/>
       <c r="D3" s="113"/>
       <c r="E3" s="113"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="D4" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="E4" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="50" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="74"/>
       <c r="B5" s="43">
         <v>2000</v>
@@ -3778,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="74"/>
       <c r="B6" s="43">
         <v>2005</v>
@@ -3790,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="74"/>
       <c r="B7" s="43">
         <v>2010</v>
@@ -3802,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="74"/>
       <c r="B8" s="43">
         <v>2015</v>
@@ -3814,10 +3814,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="51"/>
       <c r="B10" s="113" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="113"/>
       <c r="D10" s="113"/>
@@ -3826,33 +3826,33 @@
       <c r="G10" s="113"/>
       <c r="H10" s="113"/>
     </row>
-    <row r="11" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="B11" s="43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="E11" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="F11" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="G11" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="46" t="s">
+      <c r="H11" s="46" t="s">
         <v>43</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>44</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12"/>
       <c r="B12" s="47">
         <v>2000</v>
@@ -3878,7 +3878,7 @@
       <c r="I12"/>
       <c r="J12"/>
     </row>
-    <row r="13" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13" s="47">
         <v>2001</v>
@@ -3904,7 +3904,7 @@
       <c r="I13"/>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="47">
         <v>2002</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B15" s="47">
         <v>2003</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="73"/>
       <c r="B16" s="47">
         <v>2004</v>
@@ -3974,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="73"/>
       <c r="B17" s="47">
         <v>2005</v>
@@ -3998,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="73"/>
       <c r="B18" s="47">
         <v>2006</v>
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="73"/>
       <c r="B19" s="47">
         <v>2007</v>
@@ -4046,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="73"/>
       <c r="B20" s="47">
         <v>2008</v>
@@ -4070,7 +4070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="73"/>
       <c r="B21" s="47">
         <v>2009</v>
@@ -4094,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="73"/>
       <c r="B22" s="47">
         <v>2010</v>
@@ -4118,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="73"/>
       <c r="B23" s="47">
         <v>2011</v>
@@ -4144,7 +4144,7 @@
       <c r="I23" s="38"/>
       <c r="J23" s="38"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="73"/>
       <c r="B24" s="47">
         <v>2012</v>
@@ -4170,7 +4170,7 @@
       <c r="I24" s="38"/>
       <c r="J24" s="38"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="73"/>
       <c r="B25" s="47">
         <v>2013</v>
@@ -4196,7 +4196,7 @@
       <c r="I25" s="38"/>
       <c r="J25" s="38"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="73"/>
       <c r="B26" s="47">
         <v>2014</v>
@@ -4220,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="73"/>
       <c r="B27" s="47">
         <v>2015</v>
@@ -4244,9 +4244,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="28">
         <f t="shared" ref="C28:H28" si="0">SUM(C12:C27)</f>
@@ -4273,34 +4273,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="123" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="123"/>
-      <c r="D30" s="123"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="123"/>
-    </row>
-    <row r="31" spans="1:10" s="56" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="118" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="118"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="118"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="118"/>
+      <c r="H30" s="118"/>
+    </row>
+    <row r="31" spans="1:10" s="56" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="61"/>
-      <c r="C31" s="114" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="115"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="115"/>
-      <c r="H31" s="116"/>
-    </row>
-    <row r="32" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="119" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="120"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="120"/>
+      <c r="G31" s="120"/>
+      <c r="H31" s="121"/>
+    </row>
+    <row r="32" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="38"/>
       <c r="B32" s="38"/>
       <c r="C32" s="50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>8</v>
@@ -4315,15 +4315,15 @@
         <v>11</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="117" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="122" t="s">
+        <v>14</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
@@ -4332,8 +4332,8 @@
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
     </row>
-    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="91"/>
+    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="93"/>
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
@@ -4344,8 +4344,8 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
     </row>
-    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="91"/>
+    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="93"/>
       <c r="B35" s="2" t="s">
         <v>9</v>
       </c>
@@ -4356,8 +4356,8 @@
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
     </row>
-    <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="91"/>
+    <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="93"/>
       <c r="B36" s="2" t="s">
         <v>10</v>
       </c>
@@ -4368,8 +4368,8 @@
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
     </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="91"/>
+    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="93"/>
       <c r="B37" s="2" t="s">
         <v>11</v>
       </c>
@@ -4380,10 +4380,10 @@
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
     </row>
-    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="91"/>
+    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="93"/>
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -4392,7 +4392,7 @@
       <c r="G38" s="26"/>
       <c r="H38" s="26"/>
     </row>
-    <row r="39" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -4403,58 +4403,58 @@
       <c r="H39"/>
       <c r="I39"/>
     </row>
-    <row r="40" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="76"/>
-      <c r="B40" s="123" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="123"/>
-      <c r="D40" s="123"/>
-      <c r="E40" s="123"/>
-      <c r="F40" s="123"/>
-      <c r="G40" s="123"/>
-      <c r="H40" s="123"/>
-    </row>
-    <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="118" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="118"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
+      <c r="F40" s="118"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="118"/>
+    </row>
+    <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="76"/>
-      <c r="C41" s="114" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41" s="115"/>
-      <c r="E41" s="115"/>
-      <c r="F41" s="115"/>
-      <c r="G41" s="115"/>
-      <c r="H41" s="116"/>
-    </row>
-    <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="119" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
+      <c r="G41" s="120"/>
+      <c r="H41" s="121"/>
+    </row>
+    <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="38"/>
       <c r="B42" s="49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="50" t="s">
+      <c r="E42" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="F42" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="G42" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="H42" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H42" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="I42" s="38"/>
     </row>
-    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="75"/>
       <c r="B43" s="52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -4463,7 +4463,7 @@
       <c r="G43" s="26"/>
       <c r="H43" s="26"/>
     </row>
-    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="75"/>
       <c r="B44" s="2" t="s">
         <v>8</v>
@@ -4475,7 +4475,7 @@
       <c r="G44" s="26"/>
       <c r="H44" s="26"/>
     </row>
-    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="75"/>
       <c r="B45" s="2" t="s">
         <v>9</v>
@@ -4487,7 +4487,7 @@
       <c r="G45" s="26"/>
       <c r="H45" s="26"/>
     </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="75"/>
       <c r="B46" s="2" t="s">
         <v>10</v>
@@ -4499,7 +4499,7 @@
       <c r="G46" s="26"/>
       <c r="H46" s="26"/>
     </row>
-    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="75"/>
       <c r="B47" s="2" t="s">
         <v>11</v>
@@ -4511,10 +4511,10 @@
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
     </row>
-    <row r="48" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="75"/>
       <c r="B48" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
@@ -4525,7 +4525,7 @@
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="7"/>
       <c r="C49" s="28"/>
       <c r="D49" s="28"/>
@@ -4534,9 +4534,9 @@
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
     </row>
-    <row r="50" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B50" s="113" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C50" s="113"/>
       <c r="D50" s="113"/>
@@ -4545,44 +4545,44 @@
       <c r="G50" s="113"/>
       <c r="H50" s="113"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="38"/>
-      <c r="B51" s="120" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="121"/>
-      <c r="D51" s="121"/>
-      <c r="E51" s="121"/>
-      <c r="F51" s="121"/>
-      <c r="G51" s="121"/>
-      <c r="H51" s="122"/>
+      <c r="B51" s="115" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="116"/>
+      <c r="D51" s="116"/>
+      <c r="E51" s="116"/>
+      <c r="F51" s="116"/>
+      <c r="G51" s="116"/>
+      <c r="H51" s="117"/>
       <c r="I51" s="38"/>
       <c r="J51" s="38"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B52" s="43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C52" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D52" s="45" t="s">
+      <c r="E52" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="E52" s="45" t="s">
+      <c r="F52" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F52" s="45" t="s">
+      <c r="G52" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="G52" s="46" t="s">
+      <c r="H52" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="H52" s="46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B53" s="47">
         <v>2000</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B54" s="47">
         <v>2001</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B55" s="47">
         <v>2002</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B56" s="47">
         <v>2003</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B57" s="47">
         <v>2004</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B58" s="47">
         <v>2005</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B59" s="47">
         <v>2006</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B60" s="47">
         <v>2007</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B61" s="47">
         <v>2008</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B62" s="47">
         <v>2009</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B63" s="47">
         <v>2010</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B64" s="47">
         <v>2011</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B65" s="47">
         <v>2012</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B66" s="47">
         <v>2013</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67"/>
       <c r="B67" s="47">
         <v>2014</v>
@@ -4928,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68"/>
       <c r="B68" s="47">
         <v>2015</v>
@@ -4952,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -4962,20 +4962,20 @@
       <c r="G69"/>
       <c r="H69"/>
     </row>
-    <row r="70" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:10" s="38" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="71" spans="1:10" s="38" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="54"/>
-      <c r="B71" s="119" t="s">
-        <v>59</v>
-      </c>
-      <c r="C71" s="119"/>
-      <c r="D71" s="119"/>
-      <c r="E71" s="119"/>
-      <c r="F71" s="119"/>
-      <c r="G71" s="119"/>
-      <c r="H71" s="119"/>
-    </row>
-    <row r="72" spans="1:10" s="38" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="114" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" s="114"/>
+      <c r="D71" s="114"/>
+      <c r="E71" s="114"/>
+      <c r="F71" s="114"/>
+      <c r="G71" s="114"/>
+      <c r="H71" s="114"/>
+    </row>
+    <row r="72" spans="1:10" s="38" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B72" s="1"/>
       <c r="C72" s="108" t="s">
         <v>6</v>
@@ -4986,9 +4986,9 @@
       <c r="G72" s="108"/>
       <c r="H72" s="108"/>
     </row>
-    <row r="73" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C73" s="53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>8</v>
@@ -5003,15 +5003,15 @@
         <v>11</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="118" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="123" t="s">
+        <v>14</v>
       </c>
       <c r="B74" s="53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C74" s="26"/>
       <c r="D74" s="26"/>
@@ -5020,8 +5020,8 @@
       <c r="G74" s="26"/>
       <c r="H74" s="26"/>
     </row>
-    <row r="75" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="118"/>
+    <row r="75" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="123"/>
       <c r="B75" s="2" t="s">
         <v>8</v>
       </c>
@@ -5032,8 +5032,8 @@
       <c r="G75" s="26"/>
       <c r="H75" s="26"/>
     </row>
-    <row r="76" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="118"/>
+    <row r="76" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="123"/>
       <c r="B76" s="2" t="s">
         <v>9</v>
       </c>
@@ -5044,8 +5044,8 @@
       <c r="G76" s="26"/>
       <c r="H76" s="26"/>
     </row>
-    <row r="77" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="118"/>
+    <row r="77" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="123"/>
       <c r="B77" s="2" t="s">
         <v>10</v>
       </c>
@@ -5056,8 +5056,8 @@
       <c r="G77" s="26"/>
       <c r="H77" s="26"/>
     </row>
-    <row r="78" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="118"/>
+    <row r="78" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="123"/>
       <c r="B78" s="2" t="s">
         <v>11</v>
       </c>
@@ -5068,10 +5068,10 @@
       <c r="G78" s="26"/>
       <c r="H78" s="26"/>
     </row>
-    <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="118"/>
+    <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="123"/>
       <c r="B79" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C79" s="26"/>
       <c r="D79" s="26"/>
@@ -5082,7 +5082,7 @@
       <c r="I79" s="38"/>
       <c r="J79" s="38"/>
     </row>
-    <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="38"/>
       <c r="B80" s="38"/>
       <c r="C80" s="38"/>
@@ -5094,10 +5094,10 @@
       <c r="I80" s="38"/>
       <c r="J80" s="38"/>
     </row>
-    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="38"/>
       <c r="B81" s="113" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C81" s="113"/>
       <c r="D81" s="113"/>
@@ -5108,40 +5108,40 @@
       <c r="I81" s="113"/>
       <c r="J81" s="113"/>
     </row>
-    <row r="82" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="38"/>
       <c r="B82" s="43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C82" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D82" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D82" s="19" t="s">
+      <c r="E82" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F82" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G82" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E82" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G82" s="19" t="s">
+      <c r="H82" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H82" s="19" t="s">
+      <c r="I82" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="I82" s="20" t="s">
+      <c r="J82" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J82" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="10"/>
       <c r="B83" s="53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C83" s="29"/>
       <c r="D83" s="29"/>
@@ -5164,7 +5164,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="38"/>
       <c r="B84" s="2" t="s">
         <v>8</v>
@@ -5190,7 +5190,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="2" t="s">
         <v>9</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B86" s="2" t="s">
         <v>10</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="2" t="s">
         <v>11</v>
       </c>
@@ -5265,9 +5265,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="29"/>
@@ -5290,11 +5290,11 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B89" s="38"/>
       <c r="C89" s="28"/>
       <c r="D89" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E89" s="28">
         <f>SUM(E83:E88)</f>
@@ -5318,7 +5318,7 @@
       </c>
       <c r="J89" s="38"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B90" s="38"/>
       <c r="C90" s="38"/>
       <c r="D90" s="38"/>
@@ -5329,9 +5329,9 @@
       <c r="I90" s="38"/>
       <c r="J90" s="38"/>
     </row>
-    <row r="91" spans="1:10" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B91" s="86"/>
       <c r="C91" s="86"/>
@@ -5343,7 +5343,7 @@
       <c r="I91" s="86"/>
       <c r="J91" s="86"/>
     </row>
-    <row r="92" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C92" s="83"/>
       <c r="D92" s="83"/>
       <c r="E92" s="83"/>
@@ -5353,9 +5353,9 @@
       <c r="I92" s="83"/>
       <c r="J92" s="82"/>
     </row>
-    <row r="93" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="84" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C93" s="83"/>
       <c r="D93" s="83"/>
@@ -5368,6 +5368,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="B81:J81"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A74:A79"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="C72:H72"/>
@@ -5377,11 +5382,6 @@
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="C41:H41"/>
-    <mergeCell ref="A91:J91"/>
-    <mergeCell ref="B81:J81"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A74:A79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update units (tons -> tonnes).
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10250" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SDG 15.3.1" sheetId="5" r:id="rId1"/>
@@ -85,21 +85,6 @@
     <t>Summary of change in soil organic carbon</t>
   </si>
   <si>
-    <t>Baseline soil organic carbon (tons / ha)</t>
-  </si>
-  <si>
-    <t>Target soil organic carbon (tons / ha)</t>
-  </si>
-  <si>
-    <t>Baseline soil organic carbon (tons)</t>
-  </si>
-  <si>
-    <t>Target soil organic carbon (tons)</t>
-  </si>
-  <si>
-    <t>Change in soil organic carbon (tons)</t>
-  </si>
-  <si>
     <t>Change in soil organic carbon (percent)</t>
   </si>
   <si>
@@ -190,9 +175,6 @@
     <t>Land cover class</t>
   </si>
   <si>
-    <t>Soil organic carbon stock in topsoil, tons per ha</t>
-  </si>
-  <si>
     <t>Page 8 of 34 - SO1-3 Trends in carbon stock above and below ground</t>
   </si>
   <si>
@@ -287,6 +269,24 @@
   </si>
   <si>
     <t>Other lands</t>
+  </si>
+  <si>
+    <t>Baseline soil organic carbon (tonnes / ha)</t>
+  </si>
+  <si>
+    <t>Target soil organic carbon (tonnes / ha)</t>
+  </si>
+  <si>
+    <t>Baseline soil organic carbon (tonnes)</t>
+  </si>
+  <si>
+    <t>Target soil organic carbon (tonnes)</t>
+  </si>
+  <si>
+    <t>Change in soil organic carbon (tonnes)</t>
+  </si>
+  <si>
+    <t>Soil organic carbon stock in topsoil, tonnes per ha</t>
   </si>
 </sst>
 </file>
@@ -978,10 +978,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -994,27 +1014,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1047,6 +1047,21 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1061,21 +1076,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1400,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1415,7 +1415,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -1450,10 +1450,10 @@
       <c r="D4" s="65"/>
       <c r="E4" s="65"/>
       <c r="F4" s="72" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H4" s="65"/>
       <c r="I4" s="65"/>
@@ -1462,7 +1462,7 @@
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
@@ -1476,7 +1476,7 @@
     <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="E6" s="31" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -1488,7 +1488,7 @@
     <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="E7" s="31" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -1500,7 +1500,7 @@
     <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="E8" s="31" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -1512,7 +1512,7 @@
     <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="E9" s="31" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -1540,7 +1540,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="55" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1570,7 +1570,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1588,29 +1588,29 @@
       <c r="A3" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
@@ -1669,30 +1669,30 @@
       <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="92" t="s">
+      <c r="A11" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="93"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="95"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="93"/>
     </row>
     <row r="12" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
-      <c r="C12" s="87" t="s">
+      <c r="C12" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
     </row>
     <row r="13" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="15" t="s">
@@ -1711,7 +1711,7 @@
         <v>11</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>12</v>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="87" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1740,7 +1740,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="97"/>
+      <c r="A15" s="88"/>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1757,7 +1757,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="97"/>
+      <c r="A16" s="88"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1774,7 +1774,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="97"/>
+      <c r="A17" s="88"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1791,7 +1791,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="97"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1808,9 +1808,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="97"/>
+      <c r="A19" s="88"/>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
@@ -1825,7 +1825,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="97"/>
+      <c r="A20" s="88"/>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1880,30 +1880,30 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="97"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="95"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="93"/>
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="87" t="s">
+      <c r="C24" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="95"/>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="3" t="s">
@@ -1922,7 +1922,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>12</v>
@@ -1932,7 +1932,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="96" t="s">
+      <c r="A26" s="87" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1951,7 +1951,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="97"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1968,7 +1968,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="97"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="97"/>
+      <c r="A29" s="88"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2002,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="97"/>
+      <c r="A30" s="88"/>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
@@ -2019,9 +2019,9 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="97"/>
+      <c r="A31" s="88"/>
       <c r="B31" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="97"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
@@ -2091,30 +2091,30 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="100" t="s">
+      <c r="A35" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="94"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="94"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="94"/>
-      <c r="I35" s="94"/>
-      <c r="J35" s="95"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="92"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="92"/>
+      <c r="G35" s="92"/>
+      <c r="H35" s="92"/>
+      <c r="I35" s="92"/>
+      <c r="J35" s="93"/>
     </row>
     <row r="36" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="1"/>
-      <c r="C36" s="87" t="s">
+      <c r="C36" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="88"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="88"/>
-      <c r="H36" s="88"/>
-      <c r="I36" s="88"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="95"/>
+      <c r="I36" s="95"/>
     </row>
     <row r="37" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="3" t="s">
@@ -2133,7 +2133,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>12</v>
@@ -2143,7 +2143,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="96" t="s">
+      <c r="A38" s="87" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2162,7 +2162,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="97"/>
+      <c r="A39" s="88"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -2179,7 +2179,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="97"/>
+      <c r="A40" s="88"/>
       <c r="B40" s="2" t="s">
         <v>9</v>
       </c>
@@ -2196,7 +2196,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="97"/>
+      <c r="A41" s="88"/>
       <c r="B41" s="2" t="s">
         <v>10</v>
       </c>
@@ -2213,7 +2213,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="97"/>
+      <c r="A42" s="88"/>
       <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
@@ -2230,9 +2230,9 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="97"/>
+      <c r="A43" s="88"/>
       <c r="B43" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -2247,7 +2247,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="97"/>
+      <c r="A44" s="88"/>
       <c r="B44" s="2" t="s">
         <v>12</v>
       </c>
@@ -2302,30 +2302,30 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="101" t="s">
+      <c r="A47" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="94"/>
-      <c r="D47" s="94"/>
-      <c r="E47" s="94"/>
-      <c r="F47" s="94"/>
-      <c r="G47" s="94"/>
-      <c r="H47" s="94"/>
-      <c r="I47" s="94"/>
-      <c r="J47" s="95"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
+      <c r="E47" s="92"/>
+      <c r="F47" s="92"/>
+      <c r="G47" s="92"/>
+      <c r="H47" s="92"/>
+      <c r="I47" s="92"/>
+      <c r="J47" s="93"/>
     </row>
     <row r="48" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="1"/>
-      <c r="C48" s="87" t="s">
+      <c r="C48" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="88"/>
-      <c r="E48" s="88"/>
-      <c r="F48" s="88"/>
-      <c r="G48" s="88"/>
-      <c r="H48" s="88"/>
-      <c r="I48" s="88"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="95"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="95"/>
+      <c r="H48" s="95"/>
+      <c r="I48" s="95"/>
     </row>
     <row r="49" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C49" s="3" t="s">
@@ -2344,7 +2344,7 @@
         <v>11</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>12</v>
@@ -2354,7 +2354,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="96" t="s">
+      <c r="A50" s="87" t="s">
         <v>14</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2373,7 +2373,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="97"/>
+      <c r="A51" s="88"/>
       <c r="B51" s="2" t="s">
         <v>8</v>
       </c>
@@ -2390,7 +2390,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="97"/>
+      <c r="A52" s="88"/>
       <c r="B52" s="2" t="s">
         <v>9</v>
       </c>
@@ -2407,7 +2407,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="97"/>
+      <c r="A53" s="88"/>
       <c r="B53" s="2" t="s">
         <v>10</v>
       </c>
@@ -2424,7 +2424,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="97"/>
+      <c r="A54" s="88"/>
       <c r="B54" s="2" t="s">
         <v>11</v>
       </c>
@@ -2441,9 +2441,9 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="97"/>
+      <c r="A55" s="88"/>
       <c r="B55" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C55" s="26"/>
       <c r="D55" s="26"/>
@@ -2458,7 +2458,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="97"/>
+      <c r="A56" s="88"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
@@ -2516,23 +2516,29 @@
       <c r="A59" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="99"/>
-      <c r="C59" s="99"/>
-      <c r="D59" s="99"/>
-      <c r="E59" s="99"/>
-      <c r="F59" s="99"/>
-      <c r="G59" s="99"/>
-      <c r="H59" s="99"/>
-      <c r="I59" s="99"/>
-      <c r="J59" s="99"/>
+      <c r="B59" s="89"/>
+      <c r="C59" s="89"/>
+      <c r="D59" s="89"/>
+      <c r="E59" s="89"/>
+      <c r="F59" s="89"/>
+      <c r="G59" s="89"/>
+      <c r="H59" s="89"/>
+      <c r="I59" s="89"/>
+      <c r="J59" s="89"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="55" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A23:J23"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A26:A32"/>
@@ -2541,12 +2547,6 @@
     <mergeCell ref="A38:A44"/>
     <mergeCell ref="A47:J47"/>
     <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2557,7 +2557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2569,7 +2571,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -2579,23 +2581,23 @@
       <c r="A3" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
@@ -2603,7 +2605,7 @@
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
       <c r="E5" s="31" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
@@ -2622,7 +2624,7 @@
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
       <c r="E6" s="31" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -2638,7 +2640,7 @@
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="31" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -2654,7 +2656,7 @@
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="31" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -2670,7 +2672,7 @@
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
       <c r="E9" s="31" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -2687,7 +2689,7 @@
     <row r="11" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="F11" s="30" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G11" s="37" t="e">
         <f>I22/G22</f>
@@ -2699,7 +2701,7 @@
     </row>
     <row r="13" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="104" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B13" s="105"/>
       <c r="C13" s="105"/>
@@ -2716,28 +2718,28 @@
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="J15" s="20" t="s">
         <v>20</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2767,7 +2769,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="97"/>
+      <c r="A17" s="88"/>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2793,7 +2795,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="97"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2819,7 +2821,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="97"/>
+      <c r="A19" s="88"/>
       <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2845,7 +2847,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="97"/>
+      <c r="A20" s="88"/>
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
@@ -2871,9 +2873,9 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="97"/>
+      <c r="A21" s="88"/>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2925,30 +2927,30 @@
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="107" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="97"/>
-      <c r="C24" s="97"/>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="97"/>
-      <c r="H24" s="97"/>
-      <c r="I24" s="97"/>
-      <c r="J24" s="97"/>
+        <v>80</v>
+      </c>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="97"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="97"/>
-      <c r="J25" s="97"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
     </row>
     <row r="26" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="18" t="s">
@@ -2967,11 +2969,11 @@
         <v>11</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="96" t="s">
+      <c r="A27" s="87" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2985,7 +2987,7 @@
       <c r="H27" s="78"/>
     </row>
     <row r="28" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="97"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
@@ -2997,7 +2999,7 @@
       <c r="H28" s="78"/>
     </row>
     <row r="29" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="97"/>
+      <c r="A29" s="88"/>
       <c r="B29" s="2" t="s">
         <v>9</v>
       </c>
@@ -3009,7 +3011,7 @@
       <c r="H29" s="78"/>
     </row>
     <row r="30" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="97"/>
+      <c r="A30" s="88"/>
       <c r="B30" s="2" t="s">
         <v>10</v>
       </c>
@@ -3021,7 +3023,7 @@
       <c r="H30" s="78"/>
     </row>
     <row r="31" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="97"/>
+      <c r="A31" s="88"/>
       <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
@@ -3033,9 +3035,9 @@
       <c r="H31" s="78"/>
     </row>
     <row r="32" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="97"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C32" s="78"/>
       <c r="D32" s="78"/>
@@ -3058,7 +3060,7 @@
     </row>
     <row r="34" spans="1:10" s="60" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="102" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B34" s="103"/>
       <c r="C34" s="103"/>
@@ -3074,19 +3076,19 @@
       <c r="A36" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="55" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C38" s="57"/>
       <c r="D38" s="57"/>
@@ -3130,7 +3132,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J1" s="14"/>
     </row>
@@ -3139,25 +3141,25 @@
     </row>
     <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="95"/>
+        <v>21</v>
+      </c>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="93"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="72" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
@@ -3165,7 +3167,7 @@
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
       <c r="E5" s="31" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F5" s="67">
         <f>SUM(F6:F9)</f>
@@ -3183,7 +3185,7 @@
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
       <c r="E6" s="31" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="32" t="e">
@@ -3198,7 +3200,7 @@
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="31" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="33" t="e">
@@ -3213,7 +3215,7 @@
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="31" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="34" t="e">
@@ -3228,7 +3230,7 @@
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
       <c r="E9" s="31" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="35" t="e">
@@ -3244,7 +3246,7 @@
     </row>
     <row r="11" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="109" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B11" s="110"/>
       <c r="C11" s="110"/>
@@ -3262,16 +3264,16 @@
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3297,7 +3299,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="97"/>
+      <c r="A15" s="88"/>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -3319,7 +3321,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="97"/>
+      <c r="A16" s="88"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -3341,7 +3343,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="97"/>
+      <c r="A17" s="88"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
@@ -3363,7 +3365,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="97"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -3385,9 +3387,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="97"/>
+      <c r="A19" s="88"/>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C19" s="26">
         <f t="shared" si="1"/>
@@ -3407,7 +3409,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="97"/>
+      <c r="A20" s="88"/>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
@@ -3455,29 +3457,29 @@
     </row>
     <row r="23" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="112" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="97"/>
-      <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="95"/>
+        <v>26</v>
+      </c>
+      <c r="B23" s="88"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="93"/>
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="87" t="s">
+      <c r="C24" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="97"/>
-      <c r="H24" s="97"/>
-      <c r="I24" s="97"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="22" t="s">
@@ -3496,7 +3498,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I25" s="24" t="s">
         <v>12</v>
@@ -3506,7 +3508,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="96" t="s">
+      <c r="A26" s="87" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -3525,7 +3527,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="97"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3542,7 +3544,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="97"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3559,7 +3561,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="97"/>
+      <c r="A29" s="88"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
@@ -3576,7 +3578,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="97"/>
+      <c r="A30" s="88"/>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
@@ -3593,9 +3595,9 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="97"/>
+      <c r="A31" s="88"/>
       <c r="B31" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -3610,7 +3612,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="97"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
@@ -3668,19 +3670,19 @@
       <c r="A35" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="99"/>
-      <c r="C35" s="99"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="99"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="55" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C37" s="57"/>
       <c r="D37" s="57"/>
@@ -3709,7 +3711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3720,7 +3724,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -3746,7 +3750,7 @@
     <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="51"/>
       <c r="B3" s="113" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C3" s="113"/>
       <c r="D3" s="113"/>
@@ -3754,16 +3758,16 @@
     </row>
     <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="43" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3817,7 +3821,7 @@
     <row r="10" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="51"/>
       <c r="B10" s="113" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C10" s="113"/>
       <c r="D10" s="113"/>
@@ -3829,25 +3833,25 @@
     <row r="11" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="B11" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="D11" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="46" t="s">
         <v>38</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>43</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -4246,7 +4250,7 @@
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C28" s="28">
         <f t="shared" ref="C28:H28" si="0">SUM(C12:C27)</f>
@@ -4275,32 +4279,32 @@
     </row>
     <row r="29" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="118" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="118"/>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
+      <c r="B30" s="123" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="123"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="123"/>
+      <c r="H30" s="123"/>
     </row>
     <row r="31" spans="1:10" s="56" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="61"/>
-      <c r="C31" s="119" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="120"/>
-      <c r="E31" s="120"/>
-      <c r="F31" s="120"/>
-      <c r="G31" s="120"/>
-      <c r="H31" s="121"/>
+      <c r="C31" s="114" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="115"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="115"/>
+      <c r="G31" s="115"/>
+      <c r="H31" s="116"/>
     </row>
     <row r="32" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="38"/>
       <c r="B32" s="38"/>
       <c r="C32" s="50" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>8</v>
@@ -4315,15 +4319,15 @@
         <v>11</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="122" t="s">
+      <c r="A33" s="117" t="s">
         <v>14</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
@@ -4333,7 +4337,7 @@
       <c r="H33" s="26"/>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="93"/>
+      <c r="A34" s="91"/>
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
@@ -4345,7 +4349,7 @@
       <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="93"/>
+      <c r="A35" s="91"/>
       <c r="B35" s="2" t="s">
         <v>9</v>
       </c>
@@ -4357,7 +4361,7 @@
       <c r="H35" s="26"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="93"/>
+      <c r="A36" s="91"/>
       <c r="B36" s="2" t="s">
         <v>10</v>
       </c>
@@ -4369,7 +4373,7 @@
       <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="93"/>
+      <c r="A37" s="91"/>
       <c r="B37" s="2" t="s">
         <v>11</v>
       </c>
@@ -4381,9 +4385,9 @@
       <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="93"/>
+      <c r="A38" s="91"/>
       <c r="B38" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -4405,56 +4409,56 @@
     </row>
     <row r="40" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="76"/>
-      <c r="B40" s="118" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="118"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
+      <c r="B40" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="123"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="123"/>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="76"/>
-      <c r="C41" s="119" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="120"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120"/>
-      <c r="G41" s="120"/>
-      <c r="H41" s="121"/>
+      <c r="C41" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="115"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="115"/>
+      <c r="G41" s="115"/>
+      <c r="H41" s="116"/>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="38"/>
       <c r="B42" s="49" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C42" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" s="18" t="s">
         <v>47</v>
-      </c>
-      <c r="D42" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>52</v>
       </c>
       <c r="I42" s="38"/>
     </row>
     <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="75"/>
       <c r="B43" s="52" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -4514,7 +4518,7 @@
     <row r="48" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="75"/>
       <c r="B48" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
@@ -4536,7 +4540,7 @@
     </row>
     <row r="50" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B50" s="113" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C50" s="113"/>
       <c r="D50" s="113"/>
@@ -4547,39 +4551,39 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="38"/>
-      <c r="B51" s="115" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="116"/>
-      <c r="D51" s="116"/>
-      <c r="E51" s="116"/>
-      <c r="F51" s="116"/>
-      <c r="G51" s="116"/>
-      <c r="H51" s="117"/>
+      <c r="B51" s="120" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="121"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="121"/>
+      <c r="F51" s="121"/>
+      <c r="G51" s="121"/>
+      <c r="H51" s="122"/>
       <c r="I51" s="38"/>
       <c r="J51" s="38"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B52" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="D52" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="G52" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="H52" s="46" t="s">
         <v>38</v>
-      </c>
-      <c r="D52" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E52" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="G52" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="H52" s="46" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -4965,15 +4969,15 @@
     <row r="70" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="71" spans="1:10" s="38" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="54"/>
-      <c r="B71" s="114" t="s">
-        <v>58</v>
-      </c>
-      <c r="C71" s="114"/>
-      <c r="D71" s="114"/>
-      <c r="E71" s="114"/>
-      <c r="F71" s="114"/>
-      <c r="G71" s="114"/>
-      <c r="H71" s="114"/>
+      <c r="B71" s="119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" s="119"/>
+      <c r="D71" s="119"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
+      <c r="G71" s="119"/>
+      <c r="H71" s="119"/>
     </row>
     <row r="72" spans="1:10" s="38" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B72" s="1"/>
@@ -4988,7 +4992,7 @@
     </row>
     <row r="73" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C73" s="53" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>8</v>
@@ -5003,15 +5007,15 @@
         <v>11</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="123" t="s">
+      <c r="A74" s="118" t="s">
         <v>14</v>
       </c>
       <c r="B74" s="53" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C74" s="26"/>
       <c r="D74" s="26"/>
@@ -5021,7 +5025,7 @@
       <c r="H74" s="26"/>
     </row>
     <row r="75" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="123"/>
+      <c r="A75" s="118"/>
       <c r="B75" s="2" t="s">
         <v>8</v>
       </c>
@@ -5033,7 +5037,7 @@
       <c r="H75" s="26"/>
     </row>
     <row r="76" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="123"/>
+      <c r="A76" s="118"/>
       <c r="B76" s="2" t="s">
         <v>9</v>
       </c>
@@ -5045,7 +5049,7 @@
       <c r="H76" s="26"/>
     </row>
     <row r="77" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="123"/>
+      <c r="A77" s="118"/>
       <c r="B77" s="2" t="s">
         <v>10</v>
       </c>
@@ -5057,7 +5061,7 @@
       <c r="H77" s="26"/>
     </row>
     <row r="78" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="123"/>
+      <c r="A78" s="118"/>
       <c r="B78" s="2" t="s">
         <v>11</v>
       </c>
@@ -5069,9 +5073,9 @@
       <c r="H78" s="26"/>
     </row>
     <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="123"/>
+      <c r="A79" s="118"/>
       <c r="B79" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C79" s="26"/>
       <c r="D79" s="26"/>
@@ -5097,7 +5101,7 @@
     <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="38"/>
       <c r="B81" s="113" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C81" s="113"/>
       <c r="D81" s="113"/>
@@ -5111,37 +5115,37 @@
     <row r="82" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="38"/>
       <c r="B82" s="43" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C82" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F82" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G82" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="H82" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I82" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="J82" s="20" t="s">
         <v>20</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G82" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H82" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I82" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J82" s="20" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="10"/>
       <c r="B83" s="53" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C83" s="29"/>
       <c r="D83" s="29"/>
@@ -5267,7 +5271,7 @@
     </row>
     <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="29"/>
@@ -5355,7 +5359,7 @@
     </row>
     <row r="93" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="84" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C93" s="83"/>
       <c r="D93" s="83"/>
@@ -5368,11 +5372,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A91:J91"/>
-    <mergeCell ref="B81:J81"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A74:A79"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="C72:H72"/>
@@ -5382,6 +5381,11 @@
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="C41:H41"/>
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="B81:J81"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A74:A79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add LPD table to reporting output.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10250" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10250"/>
   </bookViews>
   <sheets>
     <sheet name="SDG 15.3.1" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="87">
   <si>
     <t>Summary of change in productivity</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Page 4 of 34 - SO1-1 Land cover area change matrix (sq. km)</t>
   </si>
   <si>
-    <t>Page 6 of 34 - SO1-2 Trends in land productivity or functioning of the land</t>
-  </si>
-  <si>
     <t>Declining</t>
   </si>
   <si>
@@ -178,12 +175,6 @@
     <t>Page 8 of 34 - SO1-3 Trends in carbon stock above and below ground</t>
   </si>
   <si>
-    <t>Page 9 of 34 - SO1-3 Significant negative or positive changes in carbon stock</t>
-  </si>
-  <si>
-    <t>Page 8 of 34 - SO1-3 Estimate of change of organic carbon stock in soil due to land conversion to a new land cover type</t>
-  </si>
-  <si>
     <t>trends.earth output summarized in UNCCD reporting format</t>
   </si>
   <si>
@@ -287,6 +278,12 @@
   </si>
   <si>
     <t>Soil organic carbon stock in topsoil, tonnes per ha</t>
+  </si>
+  <si>
+    <t>Land cover type</t>
+  </si>
+  <si>
+    <t>Page 6 of 34 - SO1-2 Trends in land productivity or functioning of the land (for pixels with unchanged land cover)</t>
   </si>
 </sst>
 </file>
@@ -754,7 +751,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -870,22 +867,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -894,10 +880,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -950,9 +932,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -965,56 +944,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1044,9 +1041,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1059,11 +1053,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1400,22 +1391,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="56"/>
-    <col min="2" max="2" width="14.54296875" style="56" customWidth="1"/>
-    <col min="3" max="5" width="15.54296875" style="57" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" style="57" customWidth="1"/>
-    <col min="7" max="9" width="15.54296875" style="57" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="58" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="56"/>
+    <col min="1" max="1" width="9.1796875" style="49"/>
+    <col min="2" max="2" width="14.54296875" style="49" customWidth="1"/>
+    <col min="3" max="5" width="15.54296875" style="50" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" style="50" customWidth="1"/>
+    <col min="7" max="9" width="15.54296875" style="50" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="51" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -1431,44 +1422,44 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-    </row>
-    <row r="4" spans="1:10" s="62" customFormat="1" ht="30" x14ac:dyDescent="0.45">
-      <c r="A4" s="64"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
+      <c r="A3" s="83" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+    </row>
+    <row r="4" spans="1:10" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+      <c r="A4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="67">
+        <v>73</v>
+      </c>
+      <c r="F5" s="60">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="77" t="e">
+      <c r="G5" s="69" t="e">
         <f>SUM(G6:G9)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1476,71 +1467,71 @@
     <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="E6" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="68"/>
+        <v>53</v>
+      </c>
+      <c r="F6" s="61"/>
       <c r="G6" s="32" t="e">
         <f>F6/$F$5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="56"/>
     </row>
     <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="E7" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="69"/>
+        <v>54</v>
+      </c>
+      <c r="F7" s="62"/>
       <c r="G7" s="33" t="e">
         <f t="shared" ref="G7:G9" si="0">F7/$F$5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H7" s="63"/>
+      <c r="H7" s="56"/>
     </row>
     <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="E8" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="70"/>
+        <v>55</v>
+      </c>
+      <c r="F8" s="63"/>
       <c r="G8" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="63"/>
+      <c r="H8" s="56"/>
     </row>
     <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="E9" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="71"/>
+        <v>56</v>
+      </c>
+      <c r="F9" s="64"/>
       <c r="G9" s="35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H9" s="63"/>
+      <c r="H9" s="56"/>
     </row>
     <row r="10" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="86" t="s">
+    <row r="11" spans="1:10" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="55" t="s">
-        <v>60</v>
+      <c r="A13" s="48" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1557,20 +1548,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="56" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="56" customWidth="1"/>
-    <col min="3" max="9" width="15.54296875" style="57" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="58" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="56"/>
+    <col min="1" max="1" width="8.7265625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="49" customWidth="1"/>
+    <col min="3" max="9" width="15.54296875" style="50" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="51" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1585,38 +1578,38 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="99"/>
+      <c r="A3" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="89"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
-      <c r="F4" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="72" t="s">
-        <v>78</v>
+      <c r="F4" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="67">
+        <v>73</v>
+      </c>
+      <c r="F5" s="60">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="77" t="e">
+      <c r="G5" s="69" t="e">
         <f>SUM(G6:G9)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1626,7 +1619,7 @@
       <c r="E6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="68"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="32" t="e">
         <f>F6/$F$5</f>
         <v>#DIV/0!</v>
@@ -1637,7 +1630,7 @@
       <c r="E7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="69"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="33" t="e">
         <f t="shared" ref="G7:G9" si="0">F7/$F$5</f>
         <v>#DIV/0!</v>
@@ -1648,7 +1641,7 @@
       <c r="E8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="70"/>
+      <c r="F8" s="63"/>
       <c r="G8" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1659,7 +1652,7 @@
       <c r="E9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="71"/>
+      <c r="F9" s="64"/>
       <c r="G9" s="35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1669,7 +1662,7 @@
       <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="90" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="91"/>
@@ -1684,15 +1677,15 @@
     </row>
     <row r="12" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
-      <c r="C12" s="94" t="s">
+      <c r="C12" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="95"/>
-      <c r="I12" s="95"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
     </row>
     <row r="13" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="15" t="s">
@@ -1711,17 +1704,17 @@
         <v>11</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="51" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="94" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1740,7 +1733,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="88"/>
+      <c r="A15" s="95"/>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1757,7 +1750,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="88"/>
+      <c r="A16" s="95"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1774,7 +1767,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="88"/>
+      <c r="A17" s="95"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1791,7 +1784,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="88"/>
+      <c r="A18" s="95"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1808,9 +1801,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="88"/>
+      <c r="A19" s="95"/>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
@@ -1825,7 +1818,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="88"/>
+      <c r="A20" s="95"/>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1880,30 +1873,30 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="101" t="s">
+      <c r="A23" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="88"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
       <c r="J23" s="93"/>
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="94" t="s">
+      <c r="C24" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="3" t="s">
@@ -1922,17 +1915,17 @@
         <v>11</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="58" t="s">
+      <c r="J25" s="51" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="94" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1951,7 +1944,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="88"/>
+      <c r="A27" s="95"/>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1968,7 +1961,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="88"/>
+      <c r="A28" s="95"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
@@ -1985,7 +1978,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="88"/>
+      <c r="A29" s="95"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +1995,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="88"/>
+      <c r="A30" s="95"/>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
@@ -2019,9 +2012,9 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="88"/>
+      <c r="A31" s="95"/>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -2036,7 +2029,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="88"/>
+      <c r="A32" s="95"/>
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
@@ -2091,7 +2084,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="98" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="91"/>
@@ -2106,15 +2099,15 @@
     </row>
     <row r="36" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="1"/>
-      <c r="C36" s="94" t="s">
+      <c r="C36" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
-      <c r="I36" s="95"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="86"/>
+      <c r="I36" s="86"/>
     </row>
     <row r="37" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="3" t="s">
@@ -2133,17 +2126,17 @@
         <v>11</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J37" s="58" t="s">
+      <c r="J37" s="51" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="87" t="s">
+      <c r="A38" s="94" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2162,7 +2155,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="88"/>
+      <c r="A39" s="95"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -2179,7 +2172,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="88"/>
+      <c r="A40" s="95"/>
       <c r="B40" s="2" t="s">
         <v>9</v>
       </c>
@@ -2196,7 +2189,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="88"/>
+      <c r="A41" s="95"/>
       <c r="B41" s="2" t="s">
         <v>10</v>
       </c>
@@ -2213,7 +2206,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="88"/>
+      <c r="A42" s="95"/>
       <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
@@ -2230,9 +2223,9 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="88"/>
+      <c r="A43" s="95"/>
       <c r="B43" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -2247,7 +2240,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="88"/>
+      <c r="A44" s="95"/>
       <c r="B44" s="2" t="s">
         <v>12</v>
       </c>
@@ -2302,7 +2295,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="96" t="s">
+      <c r="A47" s="99" t="s">
         <v>17</v>
       </c>
       <c r="B47" s="91"/>
@@ -2317,15 +2310,15 @@
     </row>
     <row r="48" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="1"/>
-      <c r="C48" s="94" t="s">
+      <c r="C48" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="95"/>
-      <c r="E48" s="95"/>
-      <c r="F48" s="95"/>
-      <c r="G48" s="95"/>
-      <c r="H48" s="95"/>
-      <c r="I48" s="95"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="86"/>
+      <c r="H48" s="86"/>
+      <c r="I48" s="86"/>
     </row>
     <row r="49" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C49" s="3" t="s">
@@ -2344,17 +2337,17 @@
         <v>11</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J49" s="58" t="s">
+      <c r="J49" s="51" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="87" t="s">
+      <c r="A50" s="94" t="s">
         <v>14</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2373,7 +2366,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="88"/>
+      <c r="A51" s="95"/>
       <c r="B51" s="2" t="s">
         <v>8</v>
       </c>
@@ -2390,7 +2383,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="88"/>
+      <c r="A52" s="95"/>
       <c r="B52" s="2" t="s">
         <v>9</v>
       </c>
@@ -2407,7 +2400,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="88"/>
+      <c r="A53" s="95"/>
       <c r="B53" s="2" t="s">
         <v>10</v>
       </c>
@@ -2424,7 +2417,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="88"/>
+      <c r="A54" s="95"/>
       <c r="B54" s="2" t="s">
         <v>11</v>
       </c>
@@ -2441,9 +2434,9 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="88"/>
+      <c r="A55" s="95"/>
       <c r="B55" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C55" s="26"/>
       <c r="D55" s="26"/>
@@ -2458,7 +2451,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="88"/>
+      <c r="A56" s="95"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
@@ -2512,33 +2505,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="86" t="s">
+    <row r="59" spans="1:10" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="89"/>
-      <c r="C59" s="89"/>
-      <c r="D59" s="89"/>
-      <c r="E59" s="89"/>
-      <c r="F59" s="89"/>
-      <c r="G59" s="89"/>
-      <c r="H59" s="89"/>
-      <c r="I59" s="89"/>
-      <c r="J59" s="89"/>
+      <c r="B59" s="97"/>
+      <c r="C59" s="97"/>
+      <c r="D59" s="97"/>
+      <c r="E59" s="97"/>
+      <c r="F59" s="97"/>
+      <c r="G59" s="97"/>
+      <c r="H59" s="97"/>
+      <c r="I59" s="97"/>
+      <c r="J59" s="97"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A61" s="55" t="s">
-        <v>60</v>
+      <c r="A61" s="48" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A23:J23"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A26:A32"/>
@@ -2547,6 +2534,12 @@
     <mergeCell ref="A38:A44"/>
     <mergeCell ref="A47:J47"/>
     <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2558,130 +2551,130 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="56"/>
-    <col min="2" max="2" width="14.54296875" style="56" customWidth="1"/>
-    <col min="3" max="10" width="15.54296875" style="56" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="56"/>
+    <col min="1" max="1" width="9.1796875" style="49"/>
+    <col min="2" max="2" width="14.54296875" style="49" customWidth="1"/>
+    <col min="3" max="10" width="15.54296875" style="49" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
-      <c r="F4" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="72" t="s">
-        <v>78</v>
+      <c r="F4" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="67">
+        <v>73</v>
+      </c>
+      <c r="F5" s="60">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="77" t="e">
+      <c r="G5" s="69" t="e">
         <f>SUM(G6:G9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="58"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
     </row>
     <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="68"/>
+        <v>60</v>
+      </c>
+      <c r="F6" s="61"/>
       <c r="G6" s="32" t="e">
         <f>F6/$F$5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51"/>
     </row>
     <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="F7" s="62"/>
       <c r="G7" s="33" t="e">
         <f t="shared" ref="G7:G9" si="0">F7/$F$5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="51"/>
     </row>
     <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="70"/>
+        <v>62</v>
+      </c>
+      <c r="F8" s="63"/>
       <c r="G8" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="71"/>
+        <v>63</v>
+      </c>
+      <c r="F9" s="64"/>
       <c r="G9" s="35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="51"/>
     </row>
     <row r="10" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
@@ -2689,7 +2682,7 @@
     <row r="11" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="F11" s="30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G11" s="37" t="e">
         <f>I22/G22</f>
@@ -2700,28 +2693,28 @@
       <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="105"/>
+      <c r="A13" s="102" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="103"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="103"/>
     </row>
     <row r="14" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>22</v>
@@ -2730,20 +2723,20 @@
         <v>23</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J15" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="106"/>
+      <c r="A16" s="104"/>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
@@ -2769,7 +2762,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="88"/>
+      <c r="A17" s="95"/>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2795,7 +2788,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="88"/>
+      <c r="A18" s="95"/>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2821,7 +2814,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="88"/>
+      <c r="A19" s="95"/>
       <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2847,7 +2840,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="88"/>
+      <c r="A20" s="95"/>
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
@@ -2873,9 +2866,9 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="88"/>
+      <c r="A21" s="95"/>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2926,31 +2919,31 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
+      <c r="A24" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="95"/>
+      <c r="J24" s="95"/>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="108" t="s">
+      <c r="C25" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95"/>
+      <c r="G25" s="95"/>
+      <c r="H25" s="95"/>
+      <c r="I25" s="95"/>
+      <c r="J25" s="95"/>
     </row>
     <row r="26" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="18" t="s">
@@ -2969,135 +2962,135 @@
         <v>11</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="94" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
     </row>
     <row r="28" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="88"/>
+      <c r="A28" s="95"/>
       <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
     </row>
     <row r="29" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="88"/>
+      <c r="A29" s="95"/>
       <c r="B29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
     </row>
     <row r="30" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="88"/>
+      <c r="A30" s="95"/>
       <c r="B30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
     </row>
     <row r="31" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="88"/>
+      <c r="A31" s="95"/>
       <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
     </row>
     <row r="32" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="88"/>
+      <c r="A32" s="95"/>
       <c r="B32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-    </row>
-    <row r="33" spans="1:10" s="60" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+    </row>
+    <row r="33" spans="1:10" s="53" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-    </row>
-    <row r="34" spans="1:10" s="60" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="103"/>
-      <c r="C34" s="103"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="103"/>
-      <c r="G34" s="103"/>
-      <c r="H34" s="103"/>
-      <c r="I34" s="103"/>
-      <c r="J34" s="103"/>
-    </row>
-    <row r="36" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="86" t="s">
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+    </row>
+    <row r="34" spans="1:10" s="53" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="101"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
+    </row>
+    <row r="36" spans="1:10" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="97"/>
+      <c r="E36" s="97"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="97"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="58"/>
+      <c r="A38" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3123,16 +3116,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="56" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="56" customWidth="1"/>
-    <col min="3" max="9" width="15.54296875" style="56" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="58" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="56"/>
+    <col min="1" max="1" width="8.7265625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="49" customWidth="1"/>
+    <col min="3" max="9" width="15.54296875" style="49" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="51" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J1" s="14"/>
     </row>
@@ -3140,127 +3133,127 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
       <c r="J3" s="93"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
-      <c r="F4" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="72" t="s">
-        <v>78</v>
+      <c r="F4" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="67">
+        <v>73</v>
+      </c>
+      <c r="F5" s="60">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="77" t="e">
+      <c r="G5" s="69" t="e">
         <f>SUM(G6:G9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
     </row>
     <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="68"/>
+        <v>67</v>
+      </c>
+      <c r="F6" s="61"/>
       <c r="G6" s="32" t="e">
         <f>F6/$F$5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="69"/>
+        <v>68</v>
+      </c>
+      <c r="F7" s="62"/>
       <c r="G7" s="33" t="e">
         <f t="shared" ref="G7:G9" si="0">F7/$F$5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
     </row>
     <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="70"/>
+        <v>69</v>
+      </c>
+      <c r="F8" s="63"/>
       <c r="G8" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
     </row>
     <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="71"/>
+        <v>70</v>
+      </c>
+      <c r="F9" s="64"/>
       <c r="G9" s="35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="10" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
-      <c r="J10" s="56"/>
+      <c r="J10" s="49"/>
     </row>
     <row r="11" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="109" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="110"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="111"/>
+      <c r="A11" s="107" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="108"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="108"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="108"/>
+      <c r="J11" s="109"/>
     </row>
     <row r="12" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
-      <c r="J12" s="56"/>
+      <c r="J12" s="49"/>
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="19" t="s">
@@ -3277,7 +3270,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="106"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
@@ -3299,7 +3292,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="88"/>
+      <c r="A15" s="95"/>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -3321,7 +3314,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="88"/>
+      <c r="A16" s="95"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -3343,7 +3336,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="88"/>
+      <c r="A17" s="95"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
@@ -3365,7 +3358,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="88"/>
+      <c r="A18" s="95"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -3387,9 +3380,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="88"/>
+      <c r="A19" s="95"/>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19" s="26">
         <f t="shared" si="1"/>
@@ -3409,7 +3402,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="88"/>
+      <c r="A20" s="95"/>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
@@ -3456,30 +3449,30 @@
       <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="112" t="s">
+      <c r="A23" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="88"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="95"/>
       <c r="J23" s="93"/>
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="94" t="s">
+      <c r="C24" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="95"/>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="22" t="s">
@@ -3498,17 +3491,17 @@
         <v>11</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I25" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="58" t="s">
+      <c r="J25" s="51" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="94" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -3527,7 +3520,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="88"/>
+      <c r="A27" s="95"/>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3544,7 +3537,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="88"/>
+      <c r="A28" s="95"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3561,7 +3554,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="88"/>
+      <c r="A29" s="95"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
@@ -3578,7 +3571,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="88"/>
+      <c r="A30" s="95"/>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
@@ -3595,9 +3588,9 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="88"/>
+      <c r="A31" s="95"/>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -3612,7 +3605,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="88"/>
+      <c r="A32" s="95"/>
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
@@ -3628,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="60" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" s="53" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="7" t="s">
         <v>13</v>
@@ -3666,31 +3659,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="86" t="s">
+    <row r="35" spans="1:10" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="97"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="97"/>
+      <c r="F35" s="97"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="97"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
+      <c r="A37" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3709,24 +3702,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="10" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="76" customWidth="1"/>
+    <col min="3" max="9" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="12"/>
+        <v>50</v>
+      </c>
+      <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -3734,11 +3725,10 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
-    </row>
-    <row r="2" spans="1:10" s="39" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" s="39" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="40"/>
-      <c r="B2" s="41"/>
+      <c r="B2" s="77"/>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
@@ -3747,563 +3737,364 @@
       <c r="H2" s="41"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="51"/>
-      <c r="B3" s="113" t="s">
+    <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="46"/>
+      <c r="B3" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
-    </row>
-    <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B4" s="43" t="s">
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+    </row>
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="43">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="67"/>
+      <c r="B5" s="18">
         <v>2000</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44">
-        <f>SUM(C5,D5,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="74"/>
-      <c r="B6" s="43">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26">
+        <f>SUM(C5:D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="67"/>
+      <c r="B6" s="18">
         <v>2005</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44">
-        <f>SUM(C6,D6,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="74"/>
-      <c r="B7" s="43">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26">
+        <f t="shared" ref="E6:E8" si="0">SUM(C6:D6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="67"/>
+      <c r="B7" s="18">
         <v>2010</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44">
-        <f>SUM(C7,D7,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="74"/>
-      <c r="B8" s="43">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="67"/>
+      <c r="B8" s="18">
         <v>2015</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44">
-        <f>SUM(C8,D8,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="51"/>
-      <c r="B10" s="113" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="46"/>
+      <c r="B10" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="113"/>
-      <c r="H10" s="113"/>
-    </row>
-    <row r="11" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="115"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="115"/>
+    </row>
+    <row r="11" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11"/>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="46" t="s">
+      <c r="G11" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="44" t="s">
         <v>38</v>
       </c>
       <c r="I11"/>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:9" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12"/>
-      <c r="B12" s="47">
+      <c r="B12" s="18">
         <v>2000</v>
       </c>
-      <c r="C12" s="26">
-        <v>0</v>
-      </c>
-      <c r="D12" s="26">
-        <v>0</v>
-      </c>
-      <c r="E12" s="26">
-        <v>0</v>
-      </c>
-      <c r="F12" s="26">
-        <v>0</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0</v>
-      </c>
-      <c r="H12" s="26">
-        <v>0</v>
-      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
       <c r="I12"/>
-      <c r="J12"/>
-    </row>
-    <row r="13" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13"/>
-      <c r="B13" s="47">
+      <c r="B13" s="18">
         <v>2001</v>
       </c>
-      <c r="C13" s="26">
-        <v>0</v>
-      </c>
-      <c r="D13" s="26">
-        <v>0</v>
-      </c>
-      <c r="E13" s="26">
-        <v>0</v>
-      </c>
-      <c r="F13" s="26">
-        <v>0</v>
-      </c>
-      <c r="G13" s="26">
-        <v>0</v>
-      </c>
-      <c r="H13" s="26">
-        <v>0</v>
-      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
       <c r="I13"/>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="47">
+    </row>
+    <row r="14" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="18">
         <v>2002</v>
       </c>
-      <c r="C14" s="26">
-        <v>0</v>
-      </c>
-      <c r="D14" s="26">
-        <v>0</v>
-      </c>
-      <c r="E14" s="26">
-        <v>0</v>
-      </c>
-      <c r="F14" s="26">
-        <v>0</v>
-      </c>
-      <c r="G14" s="26">
-        <v>0</v>
-      </c>
-      <c r="H14" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="47">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="18">
         <v>2003</v>
       </c>
-      <c r="C15" s="26">
-        <v>0</v>
-      </c>
-      <c r="D15" s="26">
-        <v>0</v>
-      </c>
-      <c r="E15" s="26">
-        <v>0</v>
-      </c>
-      <c r="F15" s="26">
-        <v>0</v>
-      </c>
-      <c r="G15" s="26">
-        <v>0</v>
-      </c>
-      <c r="H15" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="73"/>
-      <c r="B16" s="47">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="66"/>
+      <c r="B16" s="18">
         <v>2004</v>
       </c>
-      <c r="C16" s="26">
-        <v>0</v>
-      </c>
-      <c r="D16" s="26">
-        <v>0</v>
-      </c>
-      <c r="E16" s="26">
-        <v>0</v>
-      </c>
-      <c r="F16" s="26">
-        <v>0</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="H16" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="73"/>
-      <c r="B17" s="47">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="66"/>
+      <c r="B17" s="18">
         <v>2005</v>
       </c>
-      <c r="C17" s="26">
-        <v>0</v>
-      </c>
-      <c r="D17" s="26">
-        <v>0</v>
-      </c>
-      <c r="E17" s="26">
-        <v>0</v>
-      </c>
-      <c r="F17" s="26">
-        <v>0</v>
-      </c>
-      <c r="G17" s="26">
-        <v>0</v>
-      </c>
-      <c r="H17" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="73"/>
-      <c r="B18" s="47">
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="66"/>
+      <c r="B18" s="18">
         <v>2006</v>
       </c>
-      <c r="C18" s="26">
-        <v>0</v>
-      </c>
-      <c r="D18" s="26">
-        <v>0</v>
-      </c>
-      <c r="E18" s="26">
-        <v>0</v>
-      </c>
-      <c r="F18" s="26">
-        <v>0</v>
-      </c>
-      <c r="G18" s="26">
-        <v>0</v>
-      </c>
-      <c r="H18" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="73"/>
-      <c r="B19" s="47">
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+    </row>
+    <row r="19" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="66"/>
+      <c r="B19" s="18">
         <v>2007</v>
       </c>
-      <c r="C19" s="26">
-        <v>0</v>
-      </c>
-      <c r="D19" s="26">
-        <v>0</v>
-      </c>
-      <c r="E19" s="26">
-        <v>0</v>
-      </c>
-      <c r="F19" s="26">
-        <v>0</v>
-      </c>
-      <c r="G19" s="26">
-        <v>0</v>
-      </c>
-      <c r="H19" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="73"/>
-      <c r="B20" s="47">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+    </row>
+    <row r="20" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="66"/>
+      <c r="B20" s="18">
         <v>2008</v>
       </c>
-      <c r="C20" s="26">
-        <v>0</v>
-      </c>
-      <c r="D20" s="26">
-        <v>0</v>
-      </c>
-      <c r="E20" s="26">
-        <v>0</v>
-      </c>
-      <c r="F20" s="26">
-        <v>0</v>
-      </c>
-      <c r="G20" s="26">
-        <v>0</v>
-      </c>
-      <c r="H20" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="73"/>
-      <c r="B21" s="47">
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="66"/>
+      <c r="B21" s="18">
         <v>2009</v>
       </c>
-      <c r="C21" s="26">
-        <v>0</v>
-      </c>
-      <c r="D21" s="26">
-        <v>0</v>
-      </c>
-      <c r="E21" s="26">
-        <v>0</v>
-      </c>
-      <c r="F21" s="26">
-        <v>0</v>
-      </c>
-      <c r="G21" s="26">
-        <v>0</v>
-      </c>
-      <c r="H21" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="73"/>
-      <c r="B22" s="47">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+    </row>
+    <row r="22" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="66"/>
+      <c r="B22" s="18">
         <v>2010</v>
       </c>
-      <c r="C22" s="26">
-        <v>0</v>
-      </c>
-      <c r="D22" s="26">
-        <v>0</v>
-      </c>
-      <c r="E22" s="26">
-        <v>0</v>
-      </c>
-      <c r="F22" s="26">
-        <v>0</v>
-      </c>
-      <c r="G22" s="26">
-        <v>0</v>
-      </c>
-      <c r="H22" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="73"/>
-      <c r="B23" s="47">
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="66"/>
+      <c r="B23" s="18">
         <v>2011</v>
       </c>
-      <c r="C23" s="26">
-        <v>0</v>
-      </c>
-      <c r="D23" s="26">
-        <v>0</v>
-      </c>
-      <c r="E23" s="26">
-        <v>0</v>
-      </c>
-      <c r="F23" s="26">
-        <v>0</v>
-      </c>
-      <c r="G23" s="26">
-        <v>0</v>
-      </c>
-      <c r="H23" s="26">
-        <v>0</v>
-      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
       <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="73"/>
-      <c r="B24" s="47">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="66"/>
+      <c r="B24" s="18">
         <v>2012</v>
       </c>
-      <c r="C24" s="26">
-        <v>0</v>
-      </c>
-      <c r="D24" s="26">
-        <v>0</v>
-      </c>
-      <c r="E24" s="26">
-        <v>0</v>
-      </c>
-      <c r="F24" s="26">
-        <v>0</v>
-      </c>
-      <c r="G24" s="26">
-        <v>0</v>
-      </c>
-      <c r="H24" s="26">
-        <v>0</v>
-      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
       <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="73"/>
-      <c r="B25" s="47">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="66"/>
+      <c r="B25" s="18">
         <v>2013</v>
       </c>
-      <c r="C25" s="26">
-        <v>0</v>
-      </c>
-      <c r="D25" s="26">
-        <v>0</v>
-      </c>
-      <c r="E25" s="26">
-        <v>0</v>
-      </c>
-      <c r="F25" s="26">
-        <v>0</v>
-      </c>
-      <c r="G25" s="26">
-        <v>0</v>
-      </c>
-      <c r="H25" s="26">
-        <v>0</v>
-      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
       <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="73"/>
-      <c r="B26" s="47">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="66"/>
+      <c r="B26" s="18">
         <v>2014</v>
       </c>
-      <c r="C26" s="26">
-        <v>0</v>
-      </c>
-      <c r="D26" s="26">
-        <v>0</v>
-      </c>
-      <c r="E26" s="26">
-        <v>0</v>
-      </c>
-      <c r="F26" s="26">
-        <v>0</v>
-      </c>
-      <c r="G26" s="26">
-        <v>0</v>
-      </c>
-      <c r="H26" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="73"/>
-      <c r="B27" s="47">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="66"/>
+      <c r="B27" s="18">
         <v>2015</v>
       </c>
-      <c r="C27" s="26">
-        <v>0</v>
-      </c>
-      <c r="D27" s="26">
-        <v>0</v>
-      </c>
-      <c r="E27" s="26">
-        <v>0</v>
-      </c>
-      <c r="F27" s="26">
-        <v>0</v>
-      </c>
-      <c r="G27" s="26">
-        <v>0</v>
-      </c>
-      <c r="H27" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="48" t="s">
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="78" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="28">
-        <f t="shared" ref="C28:H28" si="0">SUM(C12:C27)</f>
+        <f>C27-C12</f>
         <v>0</v>
       </c>
       <c r="D28" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D28:H28" si="1">D27-D12</f>
         <v>0</v>
       </c>
       <c r="E28" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F28" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G28" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H28" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="123" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="123"/>
-      <c r="D30" s="123"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="123"/>
-    </row>
-    <row r="31" spans="1:10" s="56" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="61"/>
-      <c r="C31" s="114" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="115"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="115"/>
-      <c r="H31" s="116"/>
-    </row>
-    <row r="32" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="119"/>
+      <c r="F30" s="119"/>
+      <c r="G30" s="119"/>
+      <c r="H30" s="119"/>
+    </row>
+    <row r="31" spans="1:9" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="54"/>
+      <c r="C31" s="111" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="112"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="112"/>
+      <c r="G31" s="112"/>
+      <c r="H31" s="113"/>
+    </row>
+    <row r="32" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="38"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="50" t="s">
+      <c r="C32" s="45" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="18" t="s">
@@ -4322,83 +4113,191 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="117" t="s">
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-    </row>
-    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="26">
+        <f>'Land cover'!C26</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="26">
+        <f>'Land cover'!D26</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="26">
+        <f>'Land cover'!E26</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="26">
+        <f>'Land cover'!F26</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="26">
+        <f>'Land cover'!G26</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="26">
+        <f>'Land cover'!H26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="91"/>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-    </row>
-    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="26">
+        <f>'Land cover'!C27</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="26">
+        <f>'Land cover'!D27</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="26">
+        <f>'Land cover'!E27</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="26">
+        <f>'Land cover'!F27</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="26">
+        <f>'Land cover'!G27</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="26">
+        <f>'Land cover'!H27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="91"/>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-    </row>
-    <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="26">
+        <f>'Land cover'!C28</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="26">
+        <f>'Land cover'!D28</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="26">
+        <f>'Land cover'!E28</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="26">
+        <f>'Land cover'!F28</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="26">
+        <f>'Land cover'!G28</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="26">
+        <f>'Land cover'!H28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="91"/>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-    </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="26">
+        <f>'Land cover'!C29</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="26">
+        <f>'Land cover'!D29</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="26">
+        <f>'Land cover'!E29</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="26">
+        <f>'Land cover'!F29</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="26">
+        <f>'Land cover'!G29</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="26">
+        <f>'Land cover'!H29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="91"/>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-    </row>
-    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="26">
+        <f>'Land cover'!C30</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="26">
+        <f>'Land cover'!D30</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="26">
+        <f>'Land cover'!E30</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="26">
+        <f>'Land cover'!F30</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="26">
+        <f>'Land cover'!G30</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="26">
+        <f>'Land cover'!H30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="91"/>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-    </row>
-    <row r="39" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="26">
+        <f>'Land cover'!C31</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="26">
+        <f>'Land cover'!D31</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="26">
+        <f>'Land cover'!E31</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="26">
+        <f>'Land cover'!F31</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="26">
+        <f>'Land cover'!G31</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="26">
+        <f>'Land cover'!H31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39"/>
-      <c r="B39"/>
+      <c r="B39" s="76"/>
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
@@ -4407,57 +4306,59 @@
       <c r="H39"/>
       <c r="I39"/>
     </row>
-    <row r="40" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="76"/>
-      <c r="B40" s="123" t="s">
+    <row r="40" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="68"/>
+      <c r="B40" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="119"/>
+      <c r="D40" s="119"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="119"/>
+      <c r="H40" s="119"/>
+    </row>
+    <row r="41" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="80"/>
+      <c r="C41" s="111" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="112"/>
+      <c r="H41" s="113"/>
+    </row>
+    <row r="42" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="38"/>
+      <c r="B42" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="123"/>
-      <c r="D40" s="123"/>
-      <c r="E40" s="123"/>
-      <c r="F40" s="123"/>
-      <c r="G40" s="123"/>
-      <c r="H40" s="123"/>
-    </row>
-    <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="76"/>
-      <c r="C41" s="114" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="115"/>
-      <c r="E41" s="115"/>
-      <c r="F41" s="115"/>
-      <c r="G41" s="115"/>
-      <c r="H41" s="116"/>
-    </row>
-    <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="38"/>
-      <c r="B42" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="18" t="s">
+      <c r="D42" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="50" t="s">
+      <c r="E42" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="F42" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="G42" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="H42" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H42" s="18" t="s">
-        <v>47</v>
-      </c>
       <c r="I42" s="38"/>
     </row>
-    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="75"/>
-      <c r="B43" s="52" t="s">
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="114" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="47" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="26"/>
@@ -4467,9 +4368,9 @@
       <c r="G43" s="26"/>
       <c r="H43" s="26"/>
     </row>
-    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="75"/>
-      <c r="B44" s="2" t="s">
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="91"/>
+      <c r="B44" s="79" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="26"/>
@@ -4479,9 +4380,9 @@
       <c r="G44" s="26"/>
       <c r="H44" s="26"/>
     </row>
-    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="75"/>
-      <c r="B45" s="2" t="s">
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="91"/>
+      <c r="B45" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="26"/>
@@ -4491,9 +4392,9 @@
       <c r="G45" s="26"/>
       <c r="H45" s="26"/>
     </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="75"/>
-      <c r="B46" s="2" t="s">
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="91"/>
+      <c r="B46" s="79" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="26"/>
@@ -4503,9 +4404,9 @@
       <c r="G46" s="26"/>
       <c r="H46" s="26"/>
     </row>
-    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="75"/>
-      <c r="B47" s="2" t="s">
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="91"/>
+      <c r="B47" s="79" t="s">
         <v>11</v>
       </c>
       <c r="C47" s="26"/>
@@ -4515,9 +4416,9 @@
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
     </row>
-    <row r="48" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="75"/>
-      <c r="B48" s="2" t="s">
+    <row r="48" spans="1:9" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="91"/>
+      <c r="B48" s="79" t="s">
         <v>38</v>
       </c>
       <c r="C48" s="26"/>
@@ -4527,438 +4428,244 @@
       <c r="G48" s="26"/>
       <c r="H48" s="26"/>
       <c r="I48"/>
-      <c r="J48"/>
-    </row>
-    <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="7"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-    </row>
-    <row r="50" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B50" s="113" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="113"/>
-      <c r="D50" s="113"/>
-      <c r="E50" s="113"/>
-      <c r="F50" s="113"/>
-      <c r="G50" s="113"/>
-      <c r="H50" s="113"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:9" s="68" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="81"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="82"/>
+    </row>
+    <row r="50" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B50" s="115" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="115"/>
+      <c r="D50" s="115"/>
+      <c r="E50" s="115"/>
+      <c r="F50" s="115"/>
+      <c r="G50" s="115"/>
+      <c r="H50" s="115"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="38"/>
-      <c r="B51" s="120" t="s">
-        <v>87</v>
-      </c>
-      <c r="C51" s="121"/>
-      <c r="D51" s="121"/>
-      <c r="E51" s="121"/>
-      <c r="F51" s="121"/>
-      <c r="G51" s="121"/>
-      <c r="H51" s="122"/>
+      <c r="B51" s="116" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="117"/>
+      <c r="D51" s="117"/>
+      <c r="E51" s="117"/>
+      <c r="F51" s="117"/>
+      <c r="G51" s="117"/>
+      <c r="H51" s="118"/>
       <c r="I51" s="38"/>
-      <c r="J51" s="38"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B52" s="43" t="s">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B52" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D52" s="45" t="s">
+      <c r="D52" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="45" t="s">
+      <c r="E52" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F52" s="45" t="s">
+      <c r="F52" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="G52" s="46" t="s">
+      <c r="G52" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="H52" s="46" t="s">
+      <c r="H52" s="44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B53" s="47">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B53" s="18">
         <v>2000</v>
       </c>
-      <c r="C53" s="26">
-        <v>0</v>
-      </c>
-      <c r="D53" s="26">
-        <v>0</v>
-      </c>
-      <c r="E53" s="26">
-        <v>0</v>
-      </c>
-      <c r="F53" s="26">
-        <v>0</v>
-      </c>
-      <c r="G53" s="26">
-        <v>0</v>
-      </c>
-      <c r="H53" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B54" s="47">
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B54" s="18">
         <v>2001</v>
       </c>
-      <c r="C54" s="26">
-        <v>0</v>
-      </c>
-      <c r="D54" s="26">
-        <v>0</v>
-      </c>
-      <c r="E54" s="26">
-        <v>0</v>
-      </c>
-      <c r="F54" s="26">
-        <v>0</v>
-      </c>
-      <c r="G54" s="26">
-        <v>0</v>
-      </c>
-      <c r="H54" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B55" s="47">
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B55" s="18">
         <v>2002</v>
       </c>
-      <c r="C55" s="26">
-        <v>0</v>
-      </c>
-      <c r="D55" s="26">
-        <v>0</v>
-      </c>
-      <c r="E55" s="26">
-        <v>0</v>
-      </c>
-      <c r="F55" s="26">
-        <v>0</v>
-      </c>
-      <c r="G55" s="26">
-        <v>0</v>
-      </c>
-      <c r="H55" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B56" s="47">
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B56" s="18">
         <v>2003</v>
       </c>
-      <c r="C56" s="26">
-        <v>0</v>
-      </c>
-      <c r="D56" s="26">
-        <v>0</v>
-      </c>
-      <c r="E56" s="26">
-        <v>0</v>
-      </c>
-      <c r="F56" s="26">
-        <v>0</v>
-      </c>
-      <c r="G56" s="26">
-        <v>0</v>
-      </c>
-      <c r="H56" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B57" s="47">
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B57" s="18">
         <v>2004</v>
       </c>
-      <c r="C57" s="26">
-        <v>0</v>
-      </c>
-      <c r="D57" s="26">
-        <v>0</v>
-      </c>
-      <c r="E57" s="26">
-        <v>0</v>
-      </c>
-      <c r="F57" s="26">
-        <v>0</v>
-      </c>
-      <c r="G57" s="26">
-        <v>0</v>
-      </c>
-      <c r="H57" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B58" s="47">
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B58" s="18">
         <v>2005</v>
       </c>
-      <c r="C58" s="26">
-        <v>0</v>
-      </c>
-      <c r="D58" s="26">
-        <v>0</v>
-      </c>
-      <c r="E58" s="26">
-        <v>0</v>
-      </c>
-      <c r="F58" s="26">
-        <v>0</v>
-      </c>
-      <c r="G58" s="26">
-        <v>0</v>
-      </c>
-      <c r="H58" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B59" s="47">
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B59" s="18">
         <v>2006</v>
       </c>
-      <c r="C59" s="26">
-        <v>0</v>
-      </c>
-      <c r="D59" s="26">
-        <v>0</v>
-      </c>
-      <c r="E59" s="26">
-        <v>0</v>
-      </c>
-      <c r="F59" s="26">
-        <v>0</v>
-      </c>
-      <c r="G59" s="26">
-        <v>0</v>
-      </c>
-      <c r="H59" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B60" s="47">
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B60" s="18">
         <v>2007</v>
       </c>
-      <c r="C60" s="26">
-        <v>0</v>
-      </c>
-      <c r="D60" s="26">
-        <v>0</v>
-      </c>
-      <c r="E60" s="26">
-        <v>0</v>
-      </c>
-      <c r="F60" s="26">
-        <v>0</v>
-      </c>
-      <c r="G60" s="26">
-        <v>0</v>
-      </c>
-      <c r="H60" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B61" s="47">
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B61" s="18">
         <v>2008</v>
       </c>
-      <c r="C61" s="26">
-        <v>0</v>
-      </c>
-      <c r="D61" s="26">
-        <v>0</v>
-      </c>
-      <c r="E61" s="26">
-        <v>0</v>
-      </c>
-      <c r="F61" s="26">
-        <v>0</v>
-      </c>
-      <c r="G61" s="26">
-        <v>0</v>
-      </c>
-      <c r="H61" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B62" s="47">
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B62" s="18">
         <v>2009</v>
       </c>
-      <c r="C62" s="26">
-        <v>0</v>
-      </c>
-      <c r="D62" s="26">
-        <v>0</v>
-      </c>
-      <c r="E62" s="26">
-        <v>0</v>
-      </c>
-      <c r="F62" s="26">
-        <v>0</v>
-      </c>
-      <c r="G62" s="26">
-        <v>0</v>
-      </c>
-      <c r="H62" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B63" s="47">
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B63" s="18">
         <v>2010</v>
       </c>
-      <c r="C63" s="26">
-        <v>0</v>
-      </c>
-      <c r="D63" s="26">
-        <v>0</v>
-      </c>
-      <c r="E63" s="26">
-        <v>0</v>
-      </c>
-      <c r="F63" s="26">
-        <v>0</v>
-      </c>
-      <c r="G63" s="26">
-        <v>0</v>
-      </c>
-      <c r="H63" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B64" s="47">
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B64" s="18">
         <v>2011</v>
       </c>
-      <c r="C64" s="26">
-        <v>0</v>
-      </c>
-      <c r="D64" s="26">
-        <v>0</v>
-      </c>
-      <c r="E64" s="26">
-        <v>0</v>
-      </c>
-      <c r="F64" s="26">
-        <v>0</v>
-      </c>
-      <c r="G64" s="26">
-        <v>0</v>
-      </c>
-      <c r="H64" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B65" s="47">
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B65" s="18">
         <v>2012</v>
       </c>
-      <c r="C65" s="26">
-        <v>0</v>
-      </c>
-      <c r="D65" s="26">
-        <v>0</v>
-      </c>
-      <c r="E65" s="26">
-        <v>0</v>
-      </c>
-      <c r="F65" s="26">
-        <v>0</v>
-      </c>
-      <c r="G65" s="26">
-        <v>0</v>
-      </c>
-      <c r="H65" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B66" s="47">
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B66" s="18">
         <v>2013</v>
       </c>
-      <c r="C66" s="26">
-        <v>0</v>
-      </c>
-      <c r="D66" s="26">
-        <v>0</v>
-      </c>
-      <c r="E66" s="26">
-        <v>0</v>
-      </c>
-      <c r="F66" s="26">
-        <v>0</v>
-      </c>
-      <c r="G66" s="26">
-        <v>0</v>
-      </c>
-      <c r="H66" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="26"/>
+    </row>
+    <row r="67" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67"/>
-      <c r="B67" s="47">
+      <c r="B67" s="18">
         <v>2014</v>
       </c>
-      <c r="C67" s="26">
-        <v>0</v>
-      </c>
-      <c r="D67" s="26">
-        <v>0</v>
-      </c>
-      <c r="E67" s="26">
-        <v>0</v>
-      </c>
-      <c r="F67" s="26">
-        <v>0</v>
-      </c>
-      <c r="G67" s="26">
-        <v>0</v>
-      </c>
-      <c r="H67" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
+      <c r="H67" s="26"/>
+    </row>
+    <row r="68" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68"/>
-      <c r="B68" s="47">
+      <c r="B68" s="18">
         <v>2015</v>
       </c>
-      <c r="C68" s="26">
-        <v>0</v>
-      </c>
-      <c r="D68" s="26">
-        <v>0</v>
-      </c>
-      <c r="E68" s="26">
-        <v>0</v>
-      </c>
-      <c r="F68" s="26">
-        <v>0</v>
-      </c>
-      <c r="G68" s="26">
-        <v>0</v>
-      </c>
-      <c r="H68" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
+    </row>
+    <row r="69" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69"/>
-      <c r="B69"/>
+      <c r="B69" s="76"/>
       <c r="C69"/>
       <c r="D69"/>
       <c r="E69"/>
@@ -4966,426 +4673,58 @@
       <c r="G69"/>
       <c r="H69"/>
     </row>
-    <row r="70" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="1:10" s="38" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="54"/>
-      <c r="B71" s="119" t="s">
-        <v>52</v>
-      </c>
-      <c r="C71" s="119"/>
-      <c r="D71" s="119"/>
-      <c r="E71" s="119"/>
-      <c r="F71" s="119"/>
-      <c r="G71" s="119"/>
-      <c r="H71" s="119"/>
-    </row>
-    <row r="72" spans="1:10" s="38" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B72" s="1"/>
-      <c r="C72" s="108" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="108"/>
-      <c r="E72" s="108"/>
-      <c r="F72" s="108"/>
-      <c r="G72" s="108"/>
-      <c r="H72" s="108"/>
-    </row>
-    <row r="73" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C73" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E73" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H73" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="118" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="26"/>
-      <c r="H74" s="26"/>
-    </row>
-    <row r="75" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="118"/>
-      <c r="B75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="26"/>
-      <c r="G75" s="26"/>
-      <c r="H75" s="26"/>
-    </row>
-    <row r="76" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="118"/>
-      <c r="B76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="26"/>
-      <c r="G76" s="26"/>
-      <c r="H76" s="26"/>
-    </row>
-    <row r="77" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="118"/>
-      <c r="B77" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
-      <c r="E77" s="26"/>
-      <c r="F77" s="26"/>
-      <c r="G77" s="26"/>
-      <c r="H77" s="26"/>
-    </row>
-    <row r="78" spans="1:10" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="118"/>
-      <c r="B78" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26"/>
-      <c r="E78" s="26"/>
-      <c r="F78" s="26"/>
-      <c r="G78" s="26"/>
-      <c r="H78" s="26"/>
-    </row>
-    <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="118"/>
-      <c r="B79" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C79" s="26"/>
-      <c r="D79" s="26"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="26"/>
-      <c r="G79" s="26"/>
-      <c r="H79" s="26"/>
-      <c r="I79" s="38"/>
-      <c r="J79" s="38"/>
-    </row>
-    <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="38"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
-      <c r="F80" s="38"/>
-      <c r="G80" s="38"/>
-      <c r="H80" s="38"/>
-      <c r="I80" s="38"/>
-      <c r="J80" s="38"/>
-    </row>
-    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="38"/>
-      <c r="B81" s="113" t="s">
-        <v>51</v>
-      </c>
-      <c r="C81" s="113"/>
-      <c r="D81" s="113"/>
-      <c r="E81" s="113"/>
-      <c r="F81" s="113"/>
-      <c r="G81" s="113"/>
-      <c r="H81" s="113"/>
-      <c r="I81" s="113"/>
-      <c r="J81" s="113"/>
-    </row>
-    <row r="82" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="38"/>
-      <c r="B82" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G82" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H82" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="I82" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="J82" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="10"/>
-      <c r="B83" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="C83" s="29"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
-      <c r="G83" s="29">
-        <f>C83*E83*100</f>
-        <v>0</v>
-      </c>
-      <c r="H83" s="29">
-        <f>D83*F83*100</f>
-        <v>0</v>
-      </c>
-      <c r="I83" s="26">
-        <f t="shared" ref="I83:I88" si="1">H83-G83</f>
-        <v>0</v>
-      </c>
-      <c r="J83" s="36" t="e">
-        <f>I83/G83</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="38"/>
-      <c r="B84" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="29"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
-      <c r="G84" s="29">
-        <f t="shared" ref="G84:H88" si="2">C84*E84*100</f>
-        <v>0</v>
-      </c>
-      <c r="H84" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I84" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J84" s="36" t="e">
-        <f t="shared" ref="J84:J88" si="3">I84/G84</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
-      <c r="G85" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H85" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I85" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J85" s="36" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C86" s="29"/>
-      <c r="D86" s="29"/>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
-      <c r="G86" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H86" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I86" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J86" s="36" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C87" s="29"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H87" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I87" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J87" s="36" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C88" s="29"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="29"/>
-      <c r="G88" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H88" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I88" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J88" s="36" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B89" s="38"/>
-      <c r="C89" s="28"/>
-      <c r="D89" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E89" s="28">
-        <f>SUM(E83:E88)</f>
-        <v>0</v>
-      </c>
-      <c r="F89" s="28">
-        <f>SUM(F83:F88)</f>
-        <v>0</v>
-      </c>
-      <c r="G89" s="28">
-        <f>SUM(G83:G88)</f>
-        <v>0</v>
-      </c>
-      <c r="H89" s="28">
-        <f>SUM(H83:H88)</f>
-        <v>0</v>
-      </c>
-      <c r="I89" s="28">
-        <f>SUM(I83:I88)</f>
-        <v>0</v>
-      </c>
-      <c r="J89" s="38"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B90" s="38"/>
-      <c r="C90" s="38"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="38"/>
-      <c r="I90" s="38"/>
-      <c r="J90" s="38"/>
-    </row>
-    <row r="91" spans="1:10" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="86" t="s">
+    <row r="70" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="76"/>
+    </row>
+    <row r="71" spans="1:9" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B91" s="86"/>
-      <c r="C91" s="86"/>
-      <c r="D91" s="86"/>
-      <c r="E91" s="86"/>
-      <c r="F91" s="86"/>
-      <c r="G91" s="86"/>
-      <c r="H91" s="86"/>
-      <c r="I91" s="86"/>
-      <c r="J91" s="86"/>
-    </row>
-    <row r="92" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C92" s="83"/>
-      <c r="D92" s="83"/>
-      <c r="E92" s="83"/>
-      <c r="F92" s="83"/>
-      <c r="G92" s="83"/>
-      <c r="H92" s="83"/>
-      <c r="I92" s="83"/>
-      <c r="J92" s="82"/>
-    </row>
-    <row r="93" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="84" t="s">
-        <v>60</v>
-      </c>
-      <c r="C93" s="83"/>
-      <c r="D93" s="83"/>
-      <c r="E93" s="83"/>
-      <c r="F93" s="83"/>
-      <c r="G93" s="83"/>
-      <c r="H93" s="83"/>
-      <c r="I93" s="83"/>
-      <c r="J93" s="82"/>
+      <c r="B71" s="84"/>
+      <c r="C71" s="84"/>
+      <c r="D71" s="84"/>
+      <c r="E71" s="84"/>
+      <c r="F71" s="84"/>
+      <c r="G71" s="84"/>
+      <c r="H71" s="84"/>
+      <c r="I71" s="84"/>
+    </row>
+    <row r="72" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="76"/>
+      <c r="C72" s="74"/>
+      <c r="D72" s="74"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="74"/>
+      <c r="G72" s="74"/>
+      <c r="H72" s="74"/>
+      <c r="I72" s="74"/>
+    </row>
+    <row r="73" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73" s="76"/>
+      <c r="C73" s="74"/>
+      <c r="D73" s="74"/>
+      <c r="E73" s="74"/>
+      <c r="F73" s="74"/>
+      <c r="G73" s="74"/>
+      <c r="H73" s="74"/>
+      <c r="I73" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="11">
+    <mergeCell ref="A71:I71"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A43:A48"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="C72:H72"/>
-    <mergeCell ref="B71:H71"/>
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B51:H51"/>
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="C41:H41"/>
-    <mergeCell ref="A91:J91"/>
-    <mergeCell ref="B81:J81"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A74:A79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalize UNCCD reporting table.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="88">
   <si>
     <t>Land area with improved productivity:</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>Other land</t>
-  </si>
-  <si>
-    <t>Net area change</t>
   </si>
   <si>
     <t>Page 4 of 34 - SO1-1 Land cover area change matrix (sq. km)</t>
@@ -794,7 +791,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -979,28 +976,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1123,24 +1145,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1471,9 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1488,7 +1490,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -1504,18 +1506,18 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="A3" s="89" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
     </row>
     <row r="4" spans="1:10" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="54"/>
@@ -1523,10 +1525,10 @@
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
       <c r="F4" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="59" t="s">
         <v>69</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>70</v>
       </c>
       <c r="H4" s="55"/>
       <c r="I4" s="55"/>
@@ -1535,7 +1537,7 @@
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="57">
         <f>SUM(F6:F9)</f>
@@ -1549,10 +1551,10 @@
     <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="E6" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="128"/>
-      <c r="G6" s="129" t="e">
+        <v>47</v>
+      </c>
+      <c r="F6" s="79"/>
+      <c r="G6" s="80" t="e">
         <f>F6/$F$5</f>
         <v>#DIV/0!</v>
       </c>
@@ -1561,7 +1563,7 @@
     <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="E7" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="32" t="e">
@@ -1573,10 +1575,10 @@
     <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="E8" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="132"/>
-      <c r="G8" s="133" t="e">
+        <v>49</v>
+      </c>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1585,10 +1587,10 @@
     <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="E9" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131" t="e">
+        <v>50</v>
+      </c>
+      <c r="F9" s="81"/>
+      <c r="G9" s="82" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1598,22 +1600,22 @@
       <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:10" s="49" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1630,9 +1632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:I14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1643,41 +1643,41 @@
     <col min="11" max="16384" width="9.1796875" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="79" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" s="78" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="79" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="78" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+    <row r="3" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="59" t="s">
         <v>69</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="E5" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="57">
         <f>SUM(F6:F9)</f>
@@ -1693,8 +1693,8 @@
       <c r="E6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="128"/>
-      <c r="G6" s="129" t="e">
+      <c r="F6" s="79"/>
+      <c r="G6" s="80" t="e">
         <f>F6/$F$5</f>
         <v>#DIV/0!</v>
       </c>
@@ -1715,8 +1715,8 @@
       <c r="E8" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="132"/>
-      <c r="G8" s="133" t="e">
+      <c r="F8" s="83"/>
+      <c r="G8" s="84" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1726,73 +1726,73 @@
       <c r="E9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131" t="e">
+      <c r="F9" s="81"/>
+      <c r="G9" s="82" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="78"/>
-    </row>
-    <row r="11" spans="1:10" s="79" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
-    </row>
-    <row r="12" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="77"/>
+    </row>
+    <row r="11" spans="1:10" s="78" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="90" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="93"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="93"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="93"/>
+    </row>
+    <row r="12" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="78"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
+      <c r="A13" s="91" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
     </row>
     <row r="14" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="1"/>
-      <c r="C14" s="85" t="s">
+      <c r="C14" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="95"/>
     </row>
     <row r="15" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="15" t="s">
@@ -1811,7 +1811,7 @@
         <v>9</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>10</v>
@@ -1821,7 +1821,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1840,7 +1840,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="83"/>
+      <c r="A17" s="92"/>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +1857,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="83"/>
+      <c r="A18" s="92"/>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
@@ -1874,7 +1874,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="83"/>
+      <c r="A19" s="92"/>
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="83"/>
+      <c r="A20" s="92"/>
       <c r="B20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1908,9 +1908,9 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="83"/>
+      <c r="A21" s="92"/>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -1925,7 +1925,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="83"/>
+      <c r="A22" s="92"/>
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1980,30 +1980,30 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="88" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
+      <c r="A25" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="97"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="97"/>
     </row>
     <row r="26" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="85" t="s">
+      <c r="C26" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
     </row>
     <row r="27" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
@@ -2022,7 +2022,7 @@
         <v>9</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>10</v>
@@ -2032,7 +2032,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="87" t="s">
+      <c r="A28" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="83"/>
+      <c r="A29" s="92"/>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
@@ -2068,7 +2068,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="83"/>
+      <c r="A30" s="92"/>
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="83"/>
+      <c r="A31" s="92"/>
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
@@ -2102,7 +2102,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="83"/>
+      <c r="A32" s="92"/>
       <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
@@ -2119,9 +2119,9 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="83"/>
+      <c r="A33" s="92"/>
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
@@ -2136,7 +2136,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="83"/>
+      <c r="A34" s="92"/>
       <c r="B34" s="2" t="s">
         <v>10</v>
       </c>
@@ -2191,30 +2191,30 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="90" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="92"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
-      <c r="G37" s="92"/>
-      <c r="H37" s="92"/>
-      <c r="I37" s="92"/>
-      <c r="J37" s="93"/>
+      <c r="A37" s="99" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="100"/>
+      <c r="C37" s="101"/>
+      <c r="D37" s="101"/>
+      <c r="E37" s="101"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="101"/>
+      <c r="I37" s="101"/>
+      <c r="J37" s="102"/>
     </row>
     <row r="38" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="1"/>
-      <c r="C38" s="85" t="s">
+      <c r="C38" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
+      <c r="D38" s="95"/>
+      <c r="E38" s="95"/>
+      <c r="F38" s="95"/>
+      <c r="G38" s="95"/>
+      <c r="H38" s="95"/>
+      <c r="I38" s="95"/>
     </row>
     <row r="39" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C39" s="3" t="s">
@@ -2233,7 +2233,7 @@
         <v>9</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>10</v>
@@ -2243,7 +2243,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="87" t="s">
+      <c r="A40" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -2262,7 +2262,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="83"/>
+      <c r="A41" s="92"/>
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
@@ -2279,7 +2279,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="83"/>
+      <c r="A42" s="92"/>
       <c r="B42" s="2" t="s">
         <v>7</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="83"/>
+      <c r="A43" s="92"/>
       <c r="B43" s="2" t="s">
         <v>8</v>
       </c>
@@ -2313,7 +2313,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="83"/>
+      <c r="A44" s="92"/>
       <c r="B44" s="2" t="s">
         <v>9</v>
       </c>
@@ -2330,9 +2330,9 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="83"/>
+      <c r="A45" s="92"/>
       <c r="B45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="83"/>
+      <c r="A46" s="92"/>
       <c r="B46" s="2" t="s">
         <v>10</v>
       </c>
@@ -2402,30 +2402,30 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="94" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="95"/>
-      <c r="C49" s="96"/>
-      <c r="D49" s="96"/>
-      <c r="E49" s="96"/>
-      <c r="F49" s="96"/>
-      <c r="G49" s="96"/>
-      <c r="H49" s="96"/>
-      <c r="I49" s="96"/>
-      <c r="J49" s="97"/>
+      <c r="A49" s="103" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="104"/>
+      <c r="C49" s="105"/>
+      <c r="D49" s="105"/>
+      <c r="E49" s="105"/>
+      <c r="F49" s="105"/>
+      <c r="G49" s="105"/>
+      <c r="H49" s="105"/>
+      <c r="I49" s="105"/>
+      <c r="J49" s="106"/>
     </row>
     <row r="50" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="1"/>
-      <c r="C50" s="85" t="s">
+      <c r="C50" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="86"/>
-      <c r="E50" s="86"/>
-      <c r="F50" s="86"/>
-      <c r="G50" s="86"/>
-      <c r="H50" s="86"/>
-      <c r="I50" s="86"/>
+      <c r="D50" s="95"/>
+      <c r="E50" s="95"/>
+      <c r="F50" s="95"/>
+      <c r="G50" s="95"/>
+      <c r="H50" s="95"/>
+      <c r="I50" s="95"/>
     </row>
     <row r="51" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C51" s="3" t="s">
@@ -2444,7 +2444,7 @@
         <v>9</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I51" s="8" t="s">
         <v>10</v>
@@ -2454,7 +2454,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="87" t="s">
+      <c r="A52" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2473,7 +2473,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="83"/>
+      <c r="A53" s="92"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -2490,7 +2490,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="83"/>
+      <c r="A54" s="92"/>
       <c r="B54" s="2" t="s">
         <v>7</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="83"/>
+      <c r="A55" s="92"/>
       <c r="B55" s="2" t="s">
         <v>8</v>
       </c>
@@ -2524,7 +2524,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="83"/>
+      <c r="A56" s="92"/>
       <c r="B56" s="2" t="s">
         <v>9</v>
       </c>
@@ -2541,9 +2541,9 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="83"/>
+      <c r="A57" s="92"/>
       <c r="B57" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="26"/>
       <c r="D57" s="26"/>
@@ -2558,7 +2558,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="83"/>
+      <c r="A58" s="92"/>
       <c r="B58" s="2" t="s">
         <v>10</v>
       </c>
@@ -2612,34 +2612,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="98" t="s">
-        <v>83</v>
-      </c>
-      <c r="B61" s="99"/>
-      <c r="C61" s="100"/>
-      <c r="D61" s="100"/>
-      <c r="E61" s="100"/>
-      <c r="F61" s="100"/>
-      <c r="G61" s="100"/>
-      <c r="H61" s="100"/>
-      <c r="I61" s="100"/>
-      <c r="J61" s="101"/>
-    </row>
-    <row r="62" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="107" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="108"/>
+      <c r="C61" s="109"/>
+      <c r="D61" s="109"/>
+      <c r="E61" s="109"/>
+      <c r="F61" s="109"/>
+      <c r="G61" s="109"/>
+      <c r="H61" s="109"/>
+      <c r="I61" s="109"/>
+      <c r="J61" s="110"/>
+    </row>
+    <row r="62" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="1"/>
-      <c r="C62" s="85" t="s">
+      <c r="C62" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="86"/>
-      <c r="E62" s="86"/>
-      <c r="F62" s="86"/>
-      <c r="G62" s="86"/>
-      <c r="H62" s="86"/>
-      <c r="I62" s="86"/>
-      <c r="J62" s="78"/>
-    </row>
-    <row r="63" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D62" s="95"/>
+      <c r="E62" s="95"/>
+      <c r="F62" s="95"/>
+      <c r="G62" s="95"/>
+      <c r="H62" s="95"/>
+      <c r="I62" s="95"/>
+      <c r="J62" s="77"/>
+    </row>
+    <row r="63" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C63" s="3" t="s">
         <v>5</v>
       </c>
@@ -2656,17 +2656,17 @@
         <v>9</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I63" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J63" s="78" t="s">
+      <c r="J63" s="77" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="87" t="s">
+    <row r="64" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -2684,8 +2684,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="83"/>
+    <row r="65" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="92"/>
       <c r="B65" s="2" t="s">
         <v>6</v>
       </c>
@@ -2701,8 +2701,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="83"/>
+    <row r="66" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="92"/>
       <c r="B66" s="2" t="s">
         <v>7</v>
       </c>
@@ -2718,8 +2718,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="83"/>
+    <row r="67" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="92"/>
       <c r="B67" s="2" t="s">
         <v>8</v>
       </c>
@@ -2735,8 +2735,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="83"/>
+    <row r="68" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="92"/>
       <c r="B68" s="2" t="s">
         <v>9</v>
       </c>
@@ -2752,10 +2752,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="83"/>
+    <row r="69" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="92"/>
       <c r="B69" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="26"/>
       <c r="D69" s="26"/>
@@ -2769,8 +2769,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="83"/>
+    <row r="70" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="92"/>
       <c r="B70" s="2" t="s">
         <v>10</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="6"/>
       <c r="B71" s="7" t="s">
         <v>11</v>
@@ -2824,44 +2824,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="79" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C72" s="77"/>
-      <c r="D72" s="77"/>
-      <c r="E72" s="77"/>
-      <c r="F72" s="77"/>
-      <c r="G72" s="77"/>
-      <c r="H72" s="77"/>
-      <c r="I72" s="77"/>
-      <c r="J72" s="78"/>
-    </row>
-    <row r="73" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="102" t="s">
-        <v>88</v>
-      </c>
-      <c r="B73" s="103"/>
-      <c r="C73" s="104"/>
-      <c r="D73" s="104"/>
-      <c r="E73" s="104"/>
-      <c r="F73" s="104"/>
-      <c r="G73" s="104"/>
-      <c r="H73" s="104"/>
-      <c r="I73" s="104"/>
-      <c r="J73" s="105"/>
-    </row>
-    <row r="74" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C72" s="76"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="76"/>
+      <c r="G72" s="76"/>
+      <c r="H72" s="76"/>
+      <c r="I72" s="76"/>
+      <c r="J72" s="77"/>
+    </row>
+    <row r="73" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="111" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" s="112"/>
+      <c r="C73" s="113"/>
+      <c r="D73" s="113"/>
+      <c r="E73" s="113"/>
+      <c r="F73" s="113"/>
+      <c r="G73" s="113"/>
+      <c r="H73" s="113"/>
+      <c r="I73" s="113"/>
+      <c r="J73" s="114"/>
+    </row>
+    <row r="74" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B74" s="1"/>
-      <c r="C74" s="85" t="s">
+      <c r="C74" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D74" s="86"/>
-      <c r="E74" s="86"/>
-      <c r="F74" s="86"/>
-      <c r="G74" s="86"/>
-      <c r="H74" s="86"/>
-      <c r="I74" s="86"/>
-      <c r="J74" s="78"/>
-    </row>
-    <row r="75" spans="1:10" s="79" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D74" s="95"/>
+      <c r="E74" s="95"/>
+      <c r="F74" s="95"/>
+      <c r="G74" s="95"/>
+      <c r="H74" s="95"/>
+      <c r="I74" s="95"/>
+      <c r="J74" s="77"/>
+    </row>
+    <row r="75" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C75" s="3" t="s">
         <v>5</v>
       </c>
@@ -2878,17 +2878,17 @@
         <v>9</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J75" s="78" t="s">
+      <c r="J75" s="77" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="87" t="s">
+    <row r="76" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -2906,8 +2906,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="83"/>
+    <row r="77" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="92"/>
       <c r="B77" s="2" t="s">
         <v>6</v>
       </c>
@@ -2923,8 +2923,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="83"/>
+    <row r="78" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="92"/>
       <c r="B78" s="2" t="s">
         <v>7</v>
       </c>
@@ -2940,8 +2940,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="83"/>
+    <row r="79" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="92"/>
       <c r="B79" s="2" t="s">
         <v>8</v>
       </c>
@@ -2957,8 +2957,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="83"/>
+    <row r="80" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="92"/>
       <c r="B80" s="2" t="s">
         <v>9</v>
       </c>
@@ -2974,10 +2974,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="83"/>
+    <row r="81" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="92"/>
       <c r="B81" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C81" s="26"/>
       <c r="D81" s="26"/>
@@ -2991,8 +2991,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="83"/>
+    <row r="82" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="92"/>
       <c r="B82" s="2" t="s">
         <v>10</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="7" t="s">
         <v>11</v>
@@ -3046,33 +3046,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="79" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C84" s="77"/>
-      <c r="D84" s="77"/>
-      <c r="E84" s="77"/>
-      <c r="F84" s="77"/>
-      <c r="G84" s="77"/>
-      <c r="H84" s="77"/>
-      <c r="I84" s="77"/>
-      <c r="J84" s="78"/>
+    <row r="84" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C84" s="76"/>
+      <c r="D84" s="76"/>
+      <c r="E84" s="76"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="76"/>
+      <c r="H84" s="76"/>
+      <c r="I84" s="76"/>
+      <c r="J84" s="77"/>
     </row>
     <row r="85" spans="1:10" s="49" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="81" t="s">
+      <c r="A85" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B85" s="89"/>
-      <c r="C85" s="89"/>
-      <c r="D85" s="89"/>
-      <c r="E85" s="89"/>
-      <c r="F85" s="89"/>
-      <c r="G85" s="89"/>
-      <c r="H85" s="89"/>
-      <c r="I85" s="89"/>
-      <c r="J85" s="89"/>
+      <c r="B85" s="98"/>
+      <c r="C85" s="98"/>
+      <c r="D85" s="98"/>
+      <c r="E85" s="98"/>
+      <c r="F85" s="98"/>
+      <c r="G85" s="98"/>
+      <c r="H85" s="98"/>
+      <c r="I85" s="98"/>
+      <c r="J85" s="98"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3108,9 +3108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G9"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3122,33 +3120,33 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="59" t="s">
         <v>69</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
@@ -3156,7 +3154,7 @@
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
       <c r="E5" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="57">
         <f>SUM(F6:F9)</f>
@@ -3175,10 +3173,10 @@
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
       <c r="E6" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="128"/>
-      <c r="G6" s="129" t="e">
+        <v>54</v>
+      </c>
+      <c r="F6" s="79"/>
+      <c r="G6" s="80" t="e">
         <f>F6/$F$5</f>
         <v>#DIV/0!</v>
       </c>
@@ -3191,7 +3189,7 @@
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
       <c r="E7" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="32" t="e">
@@ -3207,10 +3205,10 @@
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
       <c r="E8" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="132"/>
-      <c r="G8" s="133" t="e">
+        <v>56</v>
+      </c>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -3223,10 +3221,10 @@
       <c r="C9" s="47"/>
       <c r="D9" s="47"/>
       <c r="E9" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131" t="e">
+        <v>57</v>
+      </c>
+      <c r="F9" s="81"/>
+      <c r="G9" s="82" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -3240,7 +3238,7 @@
     <row r="11" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="F11" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="34" t="e">
         <f>I22/G22</f>
@@ -3251,28 +3249,28 @@
       <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="108" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="109"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
+      <c r="A13" s="117" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="118"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="118"/>
     </row>
     <row r="14" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>17</v>
@@ -3281,20 +3279,20 @@
         <v>18</v>
       </c>
       <c r="G15" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="I15" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>78</v>
       </c>
       <c r="J15" s="20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="110"/>
+      <c r="A16" s="119"/>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -3320,7 +3318,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="83"/>
+      <c r="A17" s="92"/>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
@@ -3346,7 +3344,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="83"/>
+      <c r="A18" s="92"/>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
@@ -3372,7 +3370,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="83"/>
+      <c r="A19" s="92"/>
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
@@ -3398,7 +3396,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="83"/>
+      <c r="A20" s="92"/>
       <c r="B20" s="2" t="s">
         <v>9</v>
       </c>
@@ -3424,9 +3422,9 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="83"/>
+      <c r="A21" s="92"/>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -3477,31 +3475,31 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="111" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
+      <c r="A24" s="120" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="92"/>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="112" t="s">
+      <c r="C25" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="83"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
     </row>
     <row r="26" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="18" t="s">
@@ -3520,11 +3518,11 @@
         <v>9</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -3538,7 +3536,7 @@
       <c r="H27" s="64"/>
     </row>
     <row r="28" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="83"/>
+      <c r="A28" s="92"/>
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
@@ -3550,7 +3548,7 @@
       <c r="H28" s="64"/>
     </row>
     <row r="29" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="83"/>
+      <c r="A29" s="92"/>
       <c r="B29" s="2" t="s">
         <v>7</v>
       </c>
@@ -3562,7 +3560,7 @@
       <c r="H29" s="64"/>
     </row>
     <row r="30" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="83"/>
+      <c r="A30" s="92"/>
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
@@ -3574,7 +3572,7 @@
       <c r="H30" s="64"/>
     </row>
     <row r="31" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="83"/>
+      <c r="A31" s="92"/>
       <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
@@ -3586,9 +3584,9 @@
       <c r="H31" s="64"/>
     </row>
     <row r="32" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="83"/>
+      <c r="A32" s="92"/>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="64"/>
       <c r="D32" s="64"/>
@@ -3610,36 +3608,36 @@
       <c r="J33" s="48"/>
     </row>
     <row r="34" spans="1:10" s="50" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="106" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="107"/>
-      <c r="C34" s="107"/>
-      <c r="D34" s="107"/>
-      <c r="E34" s="107"/>
-      <c r="F34" s="107"/>
-      <c r="G34" s="107"/>
-      <c r="H34" s="107"/>
-      <c r="I34" s="107"/>
-      <c r="J34" s="107"/>
+      <c r="A34" s="115" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="116"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="116"/>
+      <c r="J34" s="116"/>
     </row>
     <row r="36" spans="1:10" s="49" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="81" t="s">
+      <c r="A36" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="98"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="47"/>
       <c r="D38" s="47"/>
@@ -3670,9 +3668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3685,7 +3681,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J1" s="14"/>
     </row>
@@ -3693,26 +3689,26 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="113"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="122"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="F4" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="59" t="s">
         <v>69</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
@@ -3720,7 +3716,7 @@
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
       <c r="E5" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="57">
         <f>SUM(F6:F9)</f>
@@ -3738,10 +3734,10 @@
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
       <c r="E6" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="128"/>
-      <c r="G6" s="129" t="e">
+        <v>61</v>
+      </c>
+      <c r="F6" s="79"/>
+      <c r="G6" s="80" t="e">
         <f>F6/$F$5</f>
         <v>#DIV/0!</v>
       </c>
@@ -3753,7 +3749,7 @@
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
       <c r="E7" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="32" t="e">
@@ -3768,10 +3764,10 @@
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
       <c r="E8" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="132"/>
-      <c r="G8" s="133" t="e">
+        <v>63</v>
+      </c>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -3783,10 +3779,10 @@
       <c r="C9" s="47"/>
       <c r="D9" s="47"/>
       <c r="E9" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131" t="e">
+        <v>64</v>
+      </c>
+      <c r="F9" s="81"/>
+      <c r="G9" s="82" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -3798,18 +3794,18 @@
       <c r="J10" s="46"/>
     </row>
     <row r="11" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="114" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="115"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="115"/>
-      <c r="J11" s="116"/>
+      <c r="A11" s="123" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="124"/>
+      <c r="C11" s="124"/>
+      <c r="D11" s="124"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="125"/>
     </row>
     <row r="12" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
@@ -3830,7 +3826,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="110"/>
+      <c r="A14" s="119"/>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -3852,7 +3848,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="83"/>
+      <c r="A15" s="92"/>
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
@@ -3874,7 +3870,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="83"/>
+      <c r="A16" s="92"/>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
@@ -3896,7 +3892,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="83"/>
+      <c r="A17" s="92"/>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
@@ -3918,7 +3914,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="83"/>
+      <c r="A18" s="92"/>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -3940,9 +3936,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="83"/>
+      <c r="A19" s="92"/>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="26">
         <f t="shared" si="1"/>
@@ -3962,7 +3958,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="83"/>
+      <c r="A20" s="92"/>
       <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
@@ -4009,30 +4005,30 @@
       <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="117" t="s">
+      <c r="A23" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="113"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="122"/>
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="22" t="s">
@@ -4051,7 +4047,7 @@
         <v>9</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I25" s="24" t="s">
         <v>10</v>
@@ -4061,7 +4057,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -4080,7 +4076,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="83"/>
+      <c r="A27" s="92"/>
       <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
@@ -4097,7 +4093,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="83"/>
+      <c r="A28" s="92"/>
       <c r="B28" s="2" t="s">
         <v>7</v>
       </c>
@@ -4114,7 +4110,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="83"/>
+      <c r="A29" s="92"/>
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4131,7 +4127,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="83"/>
+      <c r="A30" s="92"/>
       <c r="B30" s="2" t="s">
         <v>9</v>
       </c>
@@ -4148,9 +4144,9 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="83"/>
+      <c r="A31" s="92"/>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -4165,7 +4161,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="83"/>
+      <c r="A32" s="92"/>
       <c r="B32" s="2" t="s">
         <v>10</v>
       </c>
@@ -4220,22 +4216,22 @@
       </c>
     </row>
     <row r="35" spans="1:10" s="49" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="81" t="s">
+      <c r="A35" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="98"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="47"/>
       <c r="D37" s="47"/>
@@ -4262,11 +4258,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4277,7 +4271,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -4301,12 +4295,12 @@
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="43"/>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="18" t="s">
@@ -4322,130 +4316,207 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="18"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+    <row r="5" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="86" t="str">
+        <f>IF(ISBLANK(B24),"",B24)</f>
+        <v/>
+      </c>
+      <c r="C5" s="86" t="str">
+        <f>IF(ISBLANK(B24),"",SUM(C24:H24))</f>
+        <v/>
+      </c>
+      <c r="D5" s="87"/>
       <c r="E5" s="26">
-        <f t="shared" ref="E5:E17" si="0">SUM(C5:D5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="61"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+        <f t="shared" ref="E5:E18" si="0">SUM(C5:D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="78" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="86" t="str">
+        <f t="shared" ref="B6:B20" si="1">IF(ISBLANK(B25),"",B25)</f>
+        <v/>
+      </c>
+      <c r="C6" s="86" t="str">
+        <f t="shared" ref="C6:C20" si="2">IF(ISBLANK(B25),"",SUM(C25:H25))</f>
+        <v/>
+      </c>
+      <c r="D6" s="87"/>
       <c r="E6" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="61"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C7" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D7" s="88"/>
       <c r="E7" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="61"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
+      <c r="B8" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C8" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D8" s="88"/>
       <c r="E8" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="61"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="B9" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C9" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D9" s="88"/>
       <c r="E9" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="61"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="B10" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C10" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D10" s="88"/>
       <c r="E10" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="61"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+      <c r="B11" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C11" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D11" s="88"/>
       <c r="E11" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="61"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="B12" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C12" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D12" s="88"/>
       <c r="E12" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="61"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="B13" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C13" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D13" s="88"/>
       <c r="E13" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="61"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
+      <c r="B14" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C14" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D14" s="88"/>
       <c r="E14" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="61"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="B15" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C15" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D15" s="88"/>
       <c r="E15" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="61"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+      <c r="B16" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C16" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D16" s="88"/>
       <c r="E16" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="61"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
+      <c r="B17" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C17" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D17" s="88"/>
       <c r="E17" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4453,70 +4524,87 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="61"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
+      <c r="B18" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C18" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D18" s="88"/>
       <c r="E18" s="26">
-        <f t="shared" ref="E18:E19" si="1">SUM(C18:D18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="61"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="B19" s="86" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C19" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D19" s="88"/>
       <c r="E19" s="26">
+        <f t="shared" ref="E19:E20" si="3">SUM(C19:D19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="61"/>
+      <c r="B20" s="86" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="43"/>
-      <c r="B21" s="123" t="s">
+        <v/>
+      </c>
+      <c r="C20" s="86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D20" s="88"/>
+      <c r="E20" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="43"/>
+      <c r="B22" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="123"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="123"/>
-      <c r="H21" s="123"/>
-    </row>
-    <row r="22" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22"/>
-      <c r="B22" s="18" t="s">
+      <c r="C22" s="132"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="132"/>
+      <c r="G22" s="132"/>
+      <c r="H22" s="132"/>
+    </row>
+    <row r="23" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23"/>
+      <c r="B23" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C23" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D23" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E23" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F23" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G23" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H23" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:9" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -4539,7 +4627,7 @@
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
     </row>
-    <row r="26" spans="1:9" s="79" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" s="78" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="18"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -4680,326 +4768,309 @@
       <c r="G39" s="26"/>
       <c r="H39" s="26"/>
     </row>
-    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="72" t="s">
+    <row r="40" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="28">
-        <f>C39-C23</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="28">
-        <f t="shared" ref="D40:H40" si="2">D39-D23</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H40" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="127" t="s">
+      <c r="C41" s="136"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="136"/>
+      <c r="F41" s="136"/>
+      <c r="G41" s="136"/>
+      <c r="H41" s="136"/>
+    </row>
+    <row r="42" spans="1:9" s="46" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="51"/>
+      <c r="C42" s="127" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="128"/>
+      <c r="E42" s="128"/>
+      <c r="F42" s="128"/>
+      <c r="G42" s="128"/>
+      <c r="H42" s="129"/>
+    </row>
+    <row r="43" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="35"/>
+      <c r="C43" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="130" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="26">
+        <f>'Land cover'!C26</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="26">
+        <f>'Land cover'!D26</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="26">
+        <f>'Land cover'!E26</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="26">
+        <f>'Land cover'!F26</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="26">
+        <f>'Land cover'!G26</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="26">
+        <f>'Land cover'!H26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="131"/>
+      <c r="B45" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="26">
+        <f>'Land cover'!C27</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="26">
+        <f>'Land cover'!D27</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="26">
+        <f>'Land cover'!E27</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="26">
+        <f>'Land cover'!F27</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="26">
+        <f>'Land cover'!G27</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="26">
+        <f>'Land cover'!H27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="131"/>
+      <c r="B46" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="26">
+        <f>'Land cover'!C28</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="26">
+        <f>'Land cover'!D28</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="26">
+        <f>'Land cover'!E28</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="26">
+        <f>'Land cover'!F28</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="26">
+        <f>'Land cover'!G28</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="26">
+        <f>'Land cover'!H28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="131"/>
+      <c r="B47" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="26">
+        <f>'Land cover'!C29</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="26">
+        <f>'Land cover'!D29</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="26">
+        <f>'Land cover'!E29</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="26">
+        <f>'Land cover'!F29</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="26">
+        <f>'Land cover'!G29</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="26">
+        <f>'Land cover'!H29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="131"/>
+      <c r="B48" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="26">
+        <f>'Land cover'!C30</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="26">
+        <f>'Land cover'!D30</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="26">
+        <f>'Land cover'!E30</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="26">
+        <f>'Land cover'!F30</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="26">
+        <f>'Land cover'!G30</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="26">
+        <f>'Land cover'!H30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="131"/>
+      <c r="B49" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="26">
+        <f>'Land cover'!C31</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="26">
+        <f>'Land cover'!D31</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="26">
+        <f>'Land cover'!E31</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="26">
+        <f>'Land cover'!F31</f>
+        <v>0</v>
+      </c>
+      <c r="G49" s="26">
+        <f>'Land cover'!G31</f>
+        <v>0</v>
+      </c>
+      <c r="H49" s="26">
+        <f>'Land cover'!H31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50"/>
+      <c r="B50" s="70"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="62"/>
+      <c r="B51" s="136" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="136"/>
+      <c r="D51" s="136"/>
+      <c r="E51" s="136"/>
+      <c r="F51" s="136"/>
+      <c r="G51" s="136"/>
+      <c r="H51" s="136"/>
+    </row>
+    <row r="52" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="73"/>
+      <c r="C52" s="127" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="128"/>
+      <c r="E52" s="128"/>
+      <c r="F52" s="128"/>
+      <c r="G52" s="128"/>
+      <c r="H52" s="129"/>
+    </row>
+    <row r="53" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="35"/>
+      <c r="B53" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="127"/>
-      <c r="D42" s="127"/>
-      <c r="E42" s="127"/>
-      <c r="F42" s="127"/>
-      <c r="G42" s="127"/>
-      <c r="H42" s="127"/>
-    </row>
-    <row r="43" spans="1:9" s="46" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="51"/>
-      <c r="C43" s="118" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="119"/>
-      <c r="E43" s="119"/>
-      <c r="F43" s="119"/>
-      <c r="G43" s="119"/>
-      <c r="H43" s="120"/>
-    </row>
-    <row r="44" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="35"/>
-      <c r="C44" s="42" t="s">
+      <c r="D53" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I53" s="35"/>
+    </row>
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="130" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+    </row>
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="131"/>
+      <c r="B55" s="72" t="s">
         <v>6</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H44" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="26">
-        <f>'Land cover'!C26</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="26">
-        <f>'Land cover'!D26</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="26">
-        <f>'Land cover'!E26</f>
-        <v>0</v>
-      </c>
-      <c r="F45" s="26">
-        <f>'Land cover'!F26</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="26">
-        <f>'Land cover'!G26</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="26">
-        <f>'Land cover'!H26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="122"/>
-      <c r="B46" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="26">
-        <f>'Land cover'!C27</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="26">
-        <f>'Land cover'!D27</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="26">
-        <f>'Land cover'!E27</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="26">
-        <f>'Land cover'!F27</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="26">
-        <f>'Land cover'!G27</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="26">
-        <f>'Land cover'!H27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="122"/>
-      <c r="B47" s="73" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="26">
-        <f>'Land cover'!C28</f>
-        <v>0</v>
-      </c>
-      <c r="D47" s="26">
-        <f>'Land cover'!D28</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="26">
-        <f>'Land cover'!E28</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="26">
-        <f>'Land cover'!F28</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="26">
-        <f>'Land cover'!G28</f>
-        <v>0</v>
-      </c>
-      <c r="H47" s="26">
-        <f>'Land cover'!H28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="122"/>
-      <c r="B48" s="73" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="26">
-        <f>'Land cover'!C29</f>
-        <v>0</v>
-      </c>
-      <c r="D48" s="26">
-        <f>'Land cover'!D29</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="26">
-        <f>'Land cover'!E29</f>
-        <v>0</v>
-      </c>
-      <c r="F48" s="26">
-        <f>'Land cover'!F29</f>
-        <v>0</v>
-      </c>
-      <c r="G48" s="26">
-        <f>'Land cover'!G29</f>
-        <v>0</v>
-      </c>
-      <c r="H48" s="26">
-        <f>'Land cover'!H29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="122"/>
-      <c r="B49" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="26">
-        <f>'Land cover'!C30</f>
-        <v>0</v>
-      </c>
-      <c r="D49" s="26">
-        <f>'Land cover'!D30</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="26">
-        <f>'Land cover'!E30</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="26">
-        <f>'Land cover'!F30</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="26">
-        <f>'Land cover'!G30</f>
-        <v>0</v>
-      </c>
-      <c r="H49" s="26">
-        <f>'Land cover'!H30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="122"/>
-      <c r="B50" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="26">
-        <f>'Land cover'!C31</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="26">
-        <f>'Land cover'!D31</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="26">
-        <f>'Land cover'!E31</f>
-        <v>0</v>
-      </c>
-      <c r="F50" s="26">
-        <f>'Land cover'!F31</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="26">
-        <f>'Land cover'!G31</f>
-        <v>0</v>
-      </c>
-      <c r="H50" s="26">
-        <f>'Land cover'!H31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51"/>
-      <c r="B51" s="70"/>
-      <c r="C51"/>
-      <c r="D51"/>
-      <c r="E51"/>
-      <c r="F51"/>
-      <c r="G51"/>
-      <c r="H51"/>
-      <c r="I51"/>
-    </row>
-    <row r="52" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="62"/>
-      <c r="B52" s="127" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="127"/>
-      <c r="D52" s="127"/>
-      <c r="E52" s="127"/>
-      <c r="F52" s="127"/>
-      <c r="G52" s="127"/>
-      <c r="H52" s="127"/>
-    </row>
-    <row r="53" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="74"/>
-      <c r="C53" s="118" t="s">
-        <v>42</v>
-      </c>
-      <c r="D53" s="119"/>
-      <c r="E53" s="119"/>
-      <c r="F53" s="119"/>
-      <c r="G53" s="119"/>
-      <c r="H53" s="120"/>
-    </row>
-    <row r="54" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="35"/>
-      <c r="B54" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D54" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="E54" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="H54" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I54" s="35"/>
-    </row>
-    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="121" t="s">
-        <v>80</v>
-      </c>
-      <c r="B55" s="44" t="s">
-        <v>28</v>
       </c>
       <c r="C55" s="26"/>
       <c r="D55" s="26"/>
@@ -5009,9 +5080,9 @@
       <c r="H55" s="26"/>
     </row>
     <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="122"/>
-      <c r="B56" s="73" t="s">
-        <v>6</v>
+      <c r="A56" s="131"/>
+      <c r="B56" s="72" t="s">
+        <v>7</v>
       </c>
       <c r="C56" s="26"/>
       <c r="D56" s="26"/>
@@ -5021,9 +5092,9 @@
       <c r="H56" s="26"/>
     </row>
     <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="122"/>
-      <c r="B57" s="73" t="s">
-        <v>7</v>
+      <c r="A57" s="131"/>
+      <c r="B57" s="72" t="s">
+        <v>8</v>
       </c>
       <c r="C57" s="26"/>
       <c r="D57" s="26"/>
@@ -5033,9 +5104,9 @@
       <c r="H57" s="26"/>
     </row>
     <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="122"/>
-      <c r="B58" s="73" t="s">
-        <v>8</v>
+      <c r="A58" s="131"/>
+      <c r="B58" s="72" t="s">
+        <v>9</v>
       </c>
       <c r="C58" s="26"/>
       <c r="D58" s="26"/>
@@ -5044,10 +5115,10 @@
       <c r="G58" s="26"/>
       <c r="H58" s="26"/>
     </row>
-    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="122"/>
-      <c r="B59" s="73" t="s">
-        <v>9</v>
+    <row r="59" spans="1:9" s="35" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="131"/>
+      <c r="B59" s="72" t="s">
+        <v>33</v>
       </c>
       <c r="C59" s="26"/>
       <c r="D59" s="26"/>
@@ -5055,75 +5126,72 @@
       <c r="F59" s="26"/>
       <c r="G59" s="26"/>
       <c r="H59" s="26"/>
-    </row>
-    <row r="60" spans="1:9" s="35" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="122"/>
-      <c r="B60" s="73" t="s">
+      <c r="I59"/>
+    </row>
+    <row r="60" spans="1:9" s="62" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="74"/>
+      <c r="C60" s="75"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="75"/>
+      <c r="F60" s="75"/>
+      <c r="G60" s="75"/>
+      <c r="H60" s="75"/>
+    </row>
+    <row r="61" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B61" s="132" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="132"/>
+      <c r="D61" s="132"/>
+      <c r="E61" s="132"/>
+      <c r="F61" s="132"/>
+      <c r="G61" s="132"/>
+      <c r="H61" s="132"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="35"/>
+      <c r="B62" s="133" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="134"/>
+      <c r="D62" s="134"/>
+      <c r="E62" s="134"/>
+      <c r="F62" s="134"/>
+      <c r="G62" s="134"/>
+      <c r="H62" s="135"/>
+      <c r="I62" s="35"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B63" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E63" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="G63" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="26"/>
-      <c r="I60"/>
-    </row>
-    <row r="61" spans="1:9" s="62" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="75"/>
-      <c r="C61" s="76"/>
-      <c r="D61" s="76"/>
-      <c r="E61" s="76"/>
-      <c r="F61" s="76"/>
-      <c r="G61" s="76"/>
-      <c r="H61" s="76"/>
-    </row>
-    <row r="62" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B62" s="123" t="s">
-        <v>44</v>
-      </c>
-      <c r="C62" s="123"/>
-      <c r="D62" s="123"/>
-      <c r="E62" s="123"/>
-      <c r="F62" s="123"/>
-      <c r="G62" s="123"/>
-      <c r="H62" s="123"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" s="35"/>
-      <c r="B63" s="124" t="s">
-        <v>79</v>
-      </c>
-      <c r="C63" s="125"/>
-      <c r="D63" s="125"/>
-      <c r="E63" s="125"/>
-      <c r="F63" s="125"/>
-      <c r="G63" s="125"/>
-      <c r="H63" s="126"/>
-      <c r="I63" s="35"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B64" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C64" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="D64" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E64" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="F64" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="G64" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H64" s="41" t="s">
-        <v>33</v>
-      </c>
+      <c r="B64" s="18"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B65" s="18"/>
@@ -5242,7 +5310,8 @@
       <c r="G77" s="26"/>
       <c r="H77" s="26"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A78"/>
       <c r="B78" s="18"/>
       <c r="C78" s="26"/>
       <c r="D78" s="26"/>
@@ -5263,41 +5332,44 @@
     </row>
     <row r="80" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="26"/>
-      <c r="E80" s="26"/>
-      <c r="F80" s="26"/>
-      <c r="G80" s="26"/>
-      <c r="H80" s="26"/>
+      <c r="B80" s="70"/>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
     </row>
     <row r="81" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A81"/>
       <c r="B81" s="70"/>
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
-    </row>
-    <row r="82" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="70"/>
-    </row>
-    <row r="83" spans="1:9" s="67" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="81" t="s">
+    </row>
+    <row r="82" spans="1:9" s="67" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B83" s="81"/>
-      <c r="C83" s="81"/>
-      <c r="D83" s="81"/>
-      <c r="E83" s="81"/>
-      <c r="F83" s="81"/>
-      <c r="G83" s="81"/>
-      <c r="H83" s="81"/>
-      <c r="I83" s="81"/>
+      <c r="B82" s="90"/>
+      <c r="C82" s="90"/>
+      <c r="D82" s="90"/>
+      <c r="E82" s="90"/>
+      <c r="F82" s="90"/>
+      <c r="G82" s="90"/>
+      <c r="H82" s="90"/>
+      <c r="I82" s="90"/>
+    </row>
+    <row r="83" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="70"/>
+      <c r="C83" s="68"/>
+      <c r="D83" s="68"/>
+      <c r="E83" s="68"/>
+      <c r="F83" s="68"/>
+      <c r="G83" s="68"/>
+      <c r="H83" s="68"/>
+      <c r="I83" s="68"/>
     </row>
     <row r="84" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="69" t="s">
+        <v>51</v>
+      </c>
       <c r="B84" s="70"/>
       <c r="C84" s="68"/>
       <c r="D84" s="68"/>
@@ -5307,32 +5379,19 @@
       <c r="H84" s="68"/>
       <c r="I84" s="68"/>
     </row>
-    <row r="85" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="69" t="s">
-        <v>52</v>
-      </c>
-      <c r="B85" s="70"/>
-      <c r="C85" s="68"/>
-      <c r="D85" s="68"/>
-      <c r="E85" s="68"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="68"/>
-      <c r="I85" s="68"/>
-    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A83:I83"/>
-    <mergeCell ref="C43:H43"/>
-    <mergeCell ref="A45:A50"/>
-    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A54:A59"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B61:H61"/>
     <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="C53:H53"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="C52:H52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor table formatting fix.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -1026,23 +1026,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1056,6 +1043,12 @@
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1084,6 +1077,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1744,15 +1744,15 @@
       <c r="A11" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
     </row>
     <row r="12" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
@@ -1766,30 +1766,30 @@
       <c r="J12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="111" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
     </row>
     <row r="14" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="1"/>
-      <c r="C14" s="93" t="s">
+      <c r="C14" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
     </row>
     <row r="15" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="15" t="s">
@@ -1818,7 +1818,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1977,30 +1977,30 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="96" t="s">
+      <c r="A25" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="96"/>
-      <c r="I25" s="96"/>
-      <c r="J25" s="96"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="113"/>
+      <c r="G25" s="113"/>
+      <c r="H25" s="113"/>
+      <c r="I25" s="113"/>
+      <c r="J25" s="113"/>
     </row>
     <row r="26" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="93" t="s">
+      <c r="C26" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94"/>
-      <c r="F26" s="94"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="94"/>
-      <c r="I26" s="94"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="98"/>
     </row>
     <row r="27" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
@@ -2029,7 +2029,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="95" t="s">
+      <c r="A28" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2188,30 +2188,30 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="98" t="s">
+      <c r="A37" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="99"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="100"/>
-      <c r="G37" s="100"/>
-      <c r="H37" s="100"/>
-      <c r="I37" s="100"/>
-      <c r="J37" s="101"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="95"/>
+      <c r="G37" s="95"/>
+      <c r="H37" s="95"/>
+      <c r="I37" s="95"/>
+      <c r="J37" s="96"/>
     </row>
     <row r="38" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="1"/>
-      <c r="C38" s="93" t="s">
+      <c r="C38" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="94"/>
-      <c r="H38" s="94"/>
-      <c r="I38" s="94"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="98"/>
+      <c r="I38" s="98"/>
     </row>
     <row r="39" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C39" s="3" t="s">
@@ -2240,7 +2240,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="95" t="s">
+      <c r="A40" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -2399,30 +2399,30 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="102" t="s">
+      <c r="A49" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="B49" s="103"/>
-      <c r="C49" s="104"/>
-      <c r="D49" s="104"/>
-      <c r="E49" s="104"/>
-      <c r="F49" s="104"/>
-      <c r="G49" s="104"/>
-      <c r="H49" s="104"/>
-      <c r="I49" s="104"/>
-      <c r="J49" s="105"/>
+      <c r="B49" s="100"/>
+      <c r="C49" s="101"/>
+      <c r="D49" s="101"/>
+      <c r="E49" s="101"/>
+      <c r="F49" s="101"/>
+      <c r="G49" s="101"/>
+      <c r="H49" s="101"/>
+      <c r="I49" s="101"/>
+      <c r="J49" s="102"/>
     </row>
     <row r="50" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="1"/>
-      <c r="C50" s="93" t="s">
+      <c r="C50" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="94"/>
-      <c r="E50" s="94"/>
-      <c r="F50" s="94"/>
-      <c r="G50" s="94"/>
-      <c r="H50" s="94"/>
-      <c r="I50" s="94"/>
+      <c r="D50" s="98"/>
+      <c r="E50" s="98"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98"/>
     </row>
     <row r="51" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C51" s="3" t="s">
@@ -2451,7 +2451,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="95" t="s">
+      <c r="A52" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2610,30 +2610,30 @@
       </c>
     </row>
     <row r="61" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="106" t="s">
+      <c r="A61" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B61" s="107"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="108"/>
-      <c r="E61" s="108"/>
-      <c r="F61" s="108"/>
-      <c r="G61" s="108"/>
-      <c r="H61" s="108"/>
-      <c r="I61" s="108"/>
-      <c r="J61" s="109"/>
+      <c r="B61" s="104"/>
+      <c r="C61" s="105"/>
+      <c r="D61" s="105"/>
+      <c r="E61" s="105"/>
+      <c r="F61" s="105"/>
+      <c r="G61" s="105"/>
+      <c r="H61" s="105"/>
+      <c r="I61" s="105"/>
+      <c r="J61" s="106"/>
     </row>
     <row r="62" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="1"/>
-      <c r="C62" s="93" t="s">
+      <c r="C62" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="94"/>
-      <c r="E62" s="94"/>
-      <c r="F62" s="94"/>
-      <c r="G62" s="94"/>
-      <c r="H62" s="94"/>
-      <c r="I62" s="94"/>
+      <c r="D62" s="98"/>
+      <c r="E62" s="98"/>
+      <c r="F62" s="98"/>
+      <c r="G62" s="98"/>
+      <c r="H62" s="98"/>
+      <c r="I62" s="98"/>
       <c r="J62" s="77"/>
     </row>
     <row r="63" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -2663,7 +2663,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="95" t="s">
+      <c r="A64" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -2832,30 +2832,30 @@
       <c r="J72" s="77"/>
     </row>
     <row r="73" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="110" t="s">
+      <c r="A73" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="B73" s="111"/>
-      <c r="C73" s="112"/>
-      <c r="D73" s="112"/>
-      <c r="E73" s="112"/>
-      <c r="F73" s="112"/>
-      <c r="G73" s="112"/>
-      <c r="H73" s="112"/>
-      <c r="I73" s="112"/>
-      <c r="J73" s="113"/>
+      <c r="B73" s="108"/>
+      <c r="C73" s="109"/>
+      <c r="D73" s="109"/>
+      <c r="E73" s="109"/>
+      <c r="F73" s="109"/>
+      <c r="G73" s="109"/>
+      <c r="H73" s="109"/>
+      <c r="I73" s="109"/>
+      <c r="J73" s="110"/>
     </row>
     <row r="74" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B74" s="1"/>
-      <c r="C74" s="93" t="s">
+      <c r="C74" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D74" s="94"/>
-      <c r="E74" s="94"/>
-      <c r="F74" s="94"/>
-      <c r="G74" s="94"/>
-      <c r="H74" s="94"/>
-      <c r="I74" s="94"/>
+      <c r="D74" s="98"/>
+      <c r="E74" s="98"/>
+      <c r="F74" s="98"/>
+      <c r="G74" s="98"/>
+      <c r="H74" s="98"/>
+      <c r="I74" s="98"/>
       <c r="J74" s="77"/>
     </row>
     <row r="75" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -2885,7 +2885,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="95" t="s">
+      <c r="A76" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -3057,15 +3057,15 @@
       <c r="A85" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B85" s="97"/>
-      <c r="C85" s="97"/>
-      <c r="D85" s="97"/>
-      <c r="E85" s="97"/>
-      <c r="F85" s="97"/>
-      <c r="G85" s="97"/>
-      <c r="H85" s="97"/>
-      <c r="I85" s="97"/>
-      <c r="J85" s="97"/>
+      <c r="B85" s="92"/>
+      <c r="C85" s="92"/>
+      <c r="D85" s="92"/>
+      <c r="E85" s="92"/>
+      <c r="F85" s="92"/>
+      <c r="G85" s="92"/>
+      <c r="H85" s="92"/>
+      <c r="I85" s="92"/>
+      <c r="J85" s="92"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="45" t="s">
@@ -3074,6 +3074,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A25:J25"/>
     <mergeCell ref="A52:A58"/>
     <mergeCell ref="A85:J85"/>
     <mergeCell ref="A28:A34"/>
@@ -3088,13 +3095,6 @@
     <mergeCell ref="A73:J73"/>
     <mergeCell ref="C74:I74"/>
     <mergeCell ref="A76:A82"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3519,7 +3519,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -3622,15 +3622,15 @@
       <c r="A36" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="97"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="97"/>
-      <c r="E36" s="97"/>
-      <c r="F36" s="97"/>
-      <c r="G36" s="97"/>
-      <c r="H36" s="97"/>
-      <c r="I36" s="97"/>
-      <c r="J36" s="97"/>
+      <c r="B36" s="92"/>
+      <c r="C36" s="92"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="92"/>
+      <c r="H36" s="92"/>
+      <c r="I36" s="92"/>
+      <c r="J36" s="92"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="45" t="s">
@@ -4017,7 +4017,7 @@
     </row>
     <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="93" t="s">
+      <c r="C24" s="97" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="91"/>
@@ -4054,7 +4054,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="95" t="s">
+      <c r="A26" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -4216,15 +4216,15 @@
       <c r="A35" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="97"/>
-      <c r="C35" s="97"/>
-      <c r="D35" s="97"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="97"/>
-      <c r="I35" s="97"/>
-      <c r="J35" s="97"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="92"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="92"/>
+      <c r="G35" s="92"/>
+      <c r="H35" s="92"/>
+      <c r="I35" s="92"/>
+      <c r="J35" s="92"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="45" t="s">
@@ -4315,7 +4315,7 @@
     </row>
     <row r="5" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="18" t="str">
-        <f>IF(ISBLANK(B24),"",)</f>
+        <f>IF(ISBLANK(B24),"",B24)</f>
         <v/>
       </c>
       <c r="C5" s="86" t="str">
@@ -4330,7 +4330,7 @@
     </row>
     <row r="6" spans="1:9" s="78" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="18" t="str">
-        <f t="shared" ref="B6:B20" si="0">IF(ISBLANK(B25),"",)</f>
+        <f t="shared" ref="B6:B20" si="0">IF(ISBLANK(B25),"",B25)</f>
         <v/>
       </c>
       <c r="C6" s="86" t="str">

</xml_diff>

<commit_message>
Fix heading on table.
</commit_message>
<xml_diff>
--- a/LDMP/data/SummaryTable.xlsx
+++ b/LDMP/data/SummaryTable.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="89">
   <si>
     <t>Land area with improved productivity:</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>Area of land with no data for productivity by type of land cover transition (sq. km)</t>
+  </si>
+  <si>
+    <t>Summary of change in productivity</t>
   </si>
 </sst>
 </file>
@@ -1650,7 +1653,7 @@
     </row>
     <row r="3" spans="1:10" s="78" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="88" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="B3" s="91"/>
       <c r="C3" s="91"/>

</xml_diff>